<commit_message>
fleshed out the git tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://blueorigins-my.sharepoint.us/personal/thoyle_blueorigin_com/Documents/cmd spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="13_ncr:1_{FB0CBD0E-D21F-4DB0-AEBF-968D4B2CDF64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F053822-DE40-45CD-9979-B5EAF47A5F41}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919B333F-E02A-4255-9DF3-8E17562C49B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="9600" yWindow="4560" windowWidth="28800" windowHeight="15460" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="638">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -24874,48 +24874,30 @@
     <t>git commands</t>
   </si>
   <si>
-    <t>version</t>
-  </si>
-  <si>
     <t>git version</t>
   </si>
   <si>
     <t>displays the installed version of git</t>
   </si>
   <si>
-    <t>bash</t>
-  </si>
-  <si>
     <t>git bash</t>
   </si>
   <si>
     <t>starts up the git console</t>
   </si>
   <si>
-    <t>--global user.name</t>
-  </si>
-  <si>
     <t>git config --global user.name &lt;user_name&gt;</t>
   </si>
   <si>
     <t>sets your username for the '--global' context</t>
   </si>
   <si>
-    <t>--global user.name &lt;user_name&gt;</t>
-  </si>
-  <si>
     <t>git config --global user.name</t>
   </si>
   <si>
     <t>query the user name for the '--global' context</t>
   </si>
   <si>
-    <t>--global user.email</t>
-  </si>
-  <si>
-    <t>--global user.email &lt;user_emailAddress&gt;</t>
-  </si>
-  <si>
     <t>git config --global user.email &lt;user_emailAddress&gt;</t>
   </si>
   <si>
@@ -24928,13 +24910,70 @@
     <t>sets your user email for the '--global' context</t>
   </si>
   <si>
-    <t>log &lt;file_name&gt;</t>
-  </si>
-  <si>
     <t>git log &lt;file_name&gt;</t>
   </si>
   <si>
     <t>shows the change history for a file</t>
+  </si>
+  <si>
+    <t>set user name, global context</t>
+  </si>
+  <si>
+    <t>query user name, global context</t>
+  </si>
+  <si>
+    <t>set user email, global context</t>
+  </si>
+  <si>
+    <t>check version</t>
+  </si>
+  <si>
+    <t>start git bash terminal</t>
+  </si>
+  <si>
+    <t>view file change history</t>
+  </si>
+  <si>
+    <t>SET UP</t>
+  </si>
+  <si>
+    <t>COMMON COMMANDS</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t>selects all files in the folder for updating</t>
+  </si>
+  <si>
+    <t>select all files in folder for updating</t>
+  </si>
+  <si>
+    <t>git push origin main</t>
+  </si>
+  <si>
+    <t>pushes the files from the 'main' branch to GitHub repository</t>
+  </si>
+  <si>
+    <t>pull down GitHub repository to local folder</t>
+  </si>
+  <si>
+    <t>git clone &lt;url_of_your_repository&gt;</t>
+  </si>
+  <si>
+    <t>'clones' or pulls down your repository from GitHub to a local folder</t>
+  </si>
+  <si>
+    <t>save file changes to your local repository</t>
+  </si>
+  <si>
+    <t>push file changes to GitHub repository</t>
+  </si>
+  <si>
+    <t>git commit -m "&lt;message_about_changes&gt;"</t>
+  </si>
+  <si>
+    <t>saves file changes locally with a message about those changes</t>
   </si>
 </sst>
 </file>
@@ -25089,7 +25128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -25282,7 +25321,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -25849,12 +25909,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="82" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B4" s="27" t="s">
@@ -25862,11 +25922,11 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="78" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" s="27" t="s">
@@ -25884,19 +25944,19 @@
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="82" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="75"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="75" t="s">
+      <c r="B12" s="82" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="75"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -25977,7 +26037,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="83" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -25991,7 +26051,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="76"/>
+      <c r="A9" s="83"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -26003,7 +26063,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="76"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -26015,7 +26075,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="76"/>
+      <c r="A11" s="83"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -26027,7 +26087,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="76"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -26048,7 +26108,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="84" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="52" t="s">
@@ -26062,7 +26122,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="77"/>
+      <c r="A16" s="84"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -26074,7 +26134,7 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="77"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -26086,7 +26146,7 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="87" x14ac:dyDescent="0.35">
-      <c r="A18" s="77"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -26098,7 +26158,7 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="84" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -26112,7 +26172,7 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="77"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -26124,7 +26184,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="77"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -26136,7 +26196,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="77"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="56" t="s">
         <v>532</v>
       </c>
@@ -26186,17 +26246,17 @@
       <c r="D26" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="E26" s="72" t="s">
+      <c r="E26" s="79" t="s">
         <v>537</v>
       </c>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="79"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
@@ -26211,15 +26271,15 @@
       <c r="D27" s="36" t="s">
         <v>545</v>
       </c>
-      <c r="E27" s="78"/>
-      <c r="F27" s="78"/>
-      <c r="G27" s="78"/>
-      <c r="H27" s="78"/>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="78"/>
-      <c r="M27" s="78"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="85"/>
+      <c r="M27" s="85"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
@@ -28159,14 +28219,14 @@
       <c r="D18" s="14" t="s">
         <v>591</v>
       </c>
-      <c r="E18" s="69" t="s">
+      <c r="E18" s="76" t="s">
         <v>592</v>
       </c>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
     </row>
     <row r="19" spans="2:13" ht="232" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
@@ -28178,17 +28238,17 @@
       <c r="D19" s="14" t="s">
         <v>595</v>
       </c>
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="76" t="s">
         <v>596</v>
       </c>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="76"/>
     </row>
     <row r="20" spans="2:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="7" t="s">
@@ -28224,17 +28284,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D10"/>
+  <dimension ref="B2:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="66"/>
     <col min="2" max="3" width="43.6328125" style="66" customWidth="1"/>
-    <col min="4" max="4" width="53.6328125" style="66" customWidth="1"/>
+    <col min="4" max="4" width="56.36328125" style="66" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="66"/>
   </cols>
   <sheetData>
@@ -28243,81 +28303,135 @@
         <v>603</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B4" s="43" t="s">
+    <row r="4" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="74" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="72" t="s">
+        <v>622</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>606</v>
+      </c>
+      <c r="D5" s="65" t="s">
         <v>607</v>
       </c>
-      <c r="C4" s="43" t="s">
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="72" t="s">
+        <v>621</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>604</v>
+      </c>
+      <c r="D6" s="65" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="73" t="s">
+        <v>618</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>608</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D7" s="65" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B5" s="43" t="s">
-        <v>604</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>605</v>
-      </c>
-      <c r="D5" s="65" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B6" s="68" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" s="73" t="s">
+        <v>619</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>610</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="73" t="s">
+        <v>620</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>612</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="73" t="s">
+        <v>619</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>613</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>611</v>
-      </c>
-      <c r="D6" s="65" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B7" s="68" t="s">
-        <v>610</v>
-      </c>
-      <c r="C7" s="43" t="s">
+      <c r="D10" s="65" t="s">
         <v>614</v>
       </c>
-      <c r="D7" s="65" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B8" s="68" t="s">
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B14" s="74" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="72" t="s">
+        <v>631</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>632</v>
+      </c>
+      <c r="D15" s="75" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="72" t="s">
+        <v>623</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>616</v>
+      </c>
+      <c r="D16" s="67" t="s">
         <v>617</v>
       </c>
-      <c r="C8" s="43" t="s">
-        <v>618</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="68" t="s">
-        <v>616</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>619</v>
-      </c>
-      <c r="D9" s="65" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="43" t="s">
-        <v>622</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>623</v>
-      </c>
-      <c r="D10" s="67" t="s">
-        <v>624</v>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="66" t="s">
+        <v>628</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>626</v>
+      </c>
+      <c r="D17" s="68" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" s="71" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="71" t="s">
+        <v>634</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>636</v>
+      </c>
+      <c r="D18" s="70" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="66" t="s">
+        <v>635</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>629</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -28496,17 +28610,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="79" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="72"/>
+      <c r="C2" s="79"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="80" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="20"/>
@@ -28514,10 +28628,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="81" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="74"/>
+      <c r="B6" s="81"/>
     </row>
     <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="35" t="s">
@@ -28646,88 +28760,88 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="78" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="78" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="78"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="78" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="78" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="78"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="78" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="78" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="71" t="s">
+      <c r="A28" s="78" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="78" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="79" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="79"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="72" t="s">
+      <c r="A31" s="79" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="71" t="s">
+      <c r="A32" s="78" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="78"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="78" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
Added instructions for creating remote GitHub repository
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07740D13-2D0F-4573-92C7-179B60DBF04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC935DD-4EDB-48D1-B532-0DCACA519EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,10 @@
     <sheet name="touch" sheetId="6" r:id="rId8"/>
     <sheet name="vi" sheetId="5" r:id="rId9"/>
     <sheet name="nmap" sheetId="20" r:id="rId10"/>
-    <sheet name="shells" sheetId="8" r:id="rId11"/>
+    <sheet name="ufw" sheetId="21" r:id="rId11"/>
     <sheet name="tcpdump" sheetId="15" r:id="rId12"/>
-    <sheet name="awk" sheetId="10" r:id="rId13"/>
-    <sheet name="ufw" sheetId="21" r:id="rId14"/>
+    <sheet name="shells" sheetId="8" r:id="rId13"/>
+    <sheet name="awk" sheetId="10" r:id="rId14"/>
     <sheet name="sort" sheetId="11" r:id="rId15"/>
     <sheet name="head" sheetId="13" r:id="rId16"/>
     <sheet name="cut" sheetId="14" r:id="rId17"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="722">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -26486,6 +26486,122 @@
       </rPr>
       <t>CRE flavor of regex</t>
     </r>
+  </si>
+  <si>
+    <t>CREATE NEW REPOSITORY</t>
+  </si>
+  <si>
+    <t>git init -b main</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-b </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= specifys the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>branch</t>
+    </r>
+  </si>
+  <si>
+    <t>initialize local directory as a Git repository</t>
+  </si>
+  <si>
+    <t>add files and stage them for commit</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = stages all files for commit</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "first commit"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-m </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= specifys that you wish to create a message with the commit</t>
+    </r>
+  </si>
+  <si>
+    <t>commit the files that you've staged in your local repository</t>
+  </si>
+  <si>
+    <t>gh auth login</t>
+  </si>
+  <si>
+    <t>follow prompts, use HTTPS for simple login</t>
+  </si>
+  <si>
+    <t>Set up connection to your GitHub account</t>
+  </si>
+  <si>
+    <t>gh repo create</t>
+  </si>
+  <si>
+    <t>push an existing git repository to GitHub</t>
+  </si>
+  <si>
+    <t>follow prompts, select "Push an existing local repo to GitHub"</t>
   </si>
 </sst>
 </file>
@@ -26827,6 +26943,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -26845,26 +26973,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -27393,7 +27509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D4A975-49E6-4D67-87B6-C134DC574AA3}">
   <dimension ref="A2:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -27411,7 +27527,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="409.5">
+    <row r="3" spans="1:13" ht="120">
       <c r="A3" s="28"/>
       <c r="B3" s="3"/>
       <c r="C3" s="39" t="s">
@@ -27461,7 +27577,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="72" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -27475,7 +27591,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="75">
-      <c r="A9" s="69"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -27487,7 +27603,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="30">
-      <c r="A10" s="69"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -27499,7 +27615,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="45">
-      <c r="A11" s="69"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -27511,7 +27627,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="45">
-      <c r="A12" s="69"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -27528,7 +27644,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="60">
-      <c r="A15" s="70" t="s">
+      <c r="A15" s="73" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -27542,7 +27658,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="75">
-      <c r="A16" s="70"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -27554,7 +27670,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="105">
-      <c r="A17" s="70"/>
+      <c r="A17" s="73"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -27566,7 +27682,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="105">
-      <c r="A18" s="70"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -27578,7 +27694,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="60">
-      <c r="A19" s="70" t="s">
+      <c r="A19" s="73" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -27592,7 +27708,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="60">
-      <c r="A20" s="70"/>
+      <c r="A20" s="73"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -27604,7 +27720,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="105">
-      <c r="A21" s="70"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -27616,7 +27732,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="60">
-      <c r="A22" s="70"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -27746,7 +27862,7 @@
       <c r="D29" s="14" t="s">
         <v>642</v>
       </c>
-      <c r="E29" s="71" t="s">
+      <c r="E29" s="62" t="s">
         <v>643</v>
       </c>
     </row>
@@ -27760,7 +27876,7 @@
       <c r="D30" s="14" t="s">
         <v>646</v>
       </c>
-      <c r="E30" s="71" t="s">
+      <c r="E30" s="62" t="s">
         <v>647</v>
       </c>
     </row>
@@ -27774,7 +27890,7 @@
       <c r="D31" s="14" t="s">
         <v>650</v>
       </c>
-      <c r="E31" s="71" t="s">
+      <c r="E31" s="62" t="s">
         <v>651</v>
       </c>
     </row>
@@ -27800,77 +27916,278 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D27781-00F8-4FFB-93E0-B673FC3983D4}">
-  <dimension ref="B3:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BA1D3C-99B5-45E1-9627-8CE6B2A3AF89}">
+  <dimension ref="B3:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="27"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="4" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5">
-      <c r="B3" s="68" t="s">
-        <v>359</v>
-      </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-    </row>
-    <row r="4" spans="2:5">
+    <row r="3" spans="2:4">
+      <c r="B3" s="27" t="s">
+        <v>655</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>656</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
       <c r="B4" s="27" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="64" t="s">
-        <v>360</v>
-      </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-    </row>
-    <row r="6" spans="2:5">
+        <v>658</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="27" t="s">
+        <v>661</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>662</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
       <c r="B6" s="27" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
+        <v>664</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>665</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
       <c r="B7" s="27" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
+        <v>667</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>668</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
       <c r="B8" s="27" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="68" t="s">
-        <v>365</v>
-      </c>
-      <c r="C11" s="68"/>
+        <v>670</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>671</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="27" t="s">
+        <v>673</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>674</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="27" t="s">
+        <v>676</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>677</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="27" t="s">
+        <v>679</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>680</v>
+      </c>
       <c r="D11" s="27" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="68" t="s">
-        <v>366</v>
-      </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="27" t="s">
-        <v>368</v>
-      </c>
+        <v>681</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="27" t="s">
+        <v>682</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>683</v>
+      </c>
+      <c r="D12" s="27"/>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="27" t="s">
+        <v>684</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="63" t="s">
+        <v>685</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>686</v>
+      </c>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="63" t="s">
+        <v>687</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>688</v>
+      </c>
+      <c r="D17" s="27"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="63" t="s">
+        <v>689</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="27"/>
+      <c r="C19" s="75" t="s">
+        <v>690</v>
+      </c>
+      <c r="D19" s="75"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="27"/>
+      <c r="C20" s="75" t="s">
+        <v>691</v>
+      </c>
+      <c r="D20" s="75"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="27"/>
+      <c r="C21" s="75" t="s">
+        <v>692</v>
+      </c>
+      <c r="D21" s="75"/>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="27"/>
+      <c r="C22" s="75" t="s">
+        <v>693</v>
+      </c>
+      <c r="D22" s="75"/>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="27"/>
+      <c r="C23" s="75" t="s">
+        <v>694</v>
+      </c>
+      <c r="D23" s="75"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="63" t="s">
+        <v>695</v>
+      </c>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="63" t="s">
+        <v>696</v>
+      </c>
+      <c r="C25" s="75" t="s">
+        <v>697</v>
+      </c>
+      <c r="D25" s="75"/>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="27"/>
+      <c r="C26" s="75" t="s">
+        <v>698</v>
+      </c>
+      <c r="D26" s="75"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="27"/>
+      <c r="C27" s="75" t="s">
+        <v>699</v>
+      </c>
+      <c r="D27" s="75"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="27"/>
+      <c r="C28" s="75" t="s">
+        <v>700</v>
+      </c>
+      <c r="D28" s="75"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="27"/>
+      <c r="C29" s="75" t="s">
+        <v>701</v>
+      </c>
+      <c r="D29" s="75"/>
+    </row>
+    <row r="30" spans="2:4" ht="38.25">
+      <c r="B30" s="27" t="s">
+        <v>702</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>703</v>
+      </c>
+      <c r="D30" s="64"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="27" t="s">
+        <v>704</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>705</v>
+      </c>
+      <c r="D31" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B11:C11"/>
+  <mergeCells count="10">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C25:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28215,6 +28532,83 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17D27781-00F8-4FFB-93E0-B673FC3983D4}">
+  <dimension ref="B3:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="8.85546875" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5">
+      <c r="B3" s="74" t="s">
+        <v>359</v>
+      </c>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="27" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="68" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="27" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="27" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="27" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="74" t="s">
+        <v>365</v>
+      </c>
+      <c r="C11" s="74"/>
+      <c r="D11" s="27" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="74" t="s">
+        <v>366</v>
+      </c>
+      <c r="C12" s="74"/>
+      <c r="D12" s="27" t="s">
+        <v>368</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B11:C11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43823669-EFD8-43EB-A359-D7480668BEF6}">
   <dimension ref="A3:C6"/>
   <sheetViews>
@@ -28255,284 +28649,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BA1D3C-99B5-45E1-9627-8CE6B2A3AF89}">
-  <dimension ref="B3:D31"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="4" width="53.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:4">
-      <c r="B3" s="27" t="s">
-        <v>655</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>656</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="27" t="s">
-        <v>658</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>659</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="27" t="s">
-        <v>661</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>662</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="27" t="s">
-        <v>664</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>665</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4">
-      <c r="B7" s="27" t="s">
-        <v>667</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>668</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="27" t="s">
-        <v>670</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>671</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="27" t="s">
-        <v>673</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>674</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="27" t="s">
-        <v>676</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>677</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11" s="27" t="s">
-        <v>679</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>680</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="27" t="s">
-        <v>682</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>683</v>
-      </c>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15" s="27" t="s">
-        <v>684</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="72" t="s">
-        <v>685</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>686</v>
-      </c>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="72" t="s">
-        <v>687</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>688</v>
-      </c>
-      <c r="D17" s="27"/>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="72" t="s">
-        <v>689</v>
-      </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="27"/>
-      <c r="C19" s="73" t="s">
-        <v>690</v>
-      </c>
-      <c r="D19" s="73"/>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="27"/>
-      <c r="C20" s="73" t="s">
-        <v>691</v>
-      </c>
-      <c r="D20" s="73"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="27"/>
-      <c r="C21" s="73" t="s">
-        <v>692</v>
-      </c>
-      <c r="D21" s="73"/>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="27"/>
-      <c r="C22" s="73" t="s">
-        <v>693</v>
-      </c>
-      <c r="D22" s="73"/>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="27"/>
-      <c r="C23" s="73" t="s">
-        <v>694</v>
-      </c>
-      <c r="D23" s="73"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="72" t="s">
-        <v>695</v>
-      </c>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="72" t="s">
-        <v>696</v>
-      </c>
-      <c r="C25" s="73" t="s">
-        <v>697</v>
-      </c>
-      <c r="D25" s="73"/>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="27"/>
-      <c r="C26" s="73" t="s">
-        <v>698</v>
-      </c>
-      <c r="D26" s="73"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="27"/>
-      <c r="C27" s="73" t="s">
-        <v>699</v>
-      </c>
-      <c r="D27" s="73"/>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="27"/>
-      <c r="C28" s="73" t="s">
-        <v>700</v>
-      </c>
-      <c r="D28" s="73"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="27"/>
-      <c r="C29" s="73" t="s">
-        <v>701</v>
-      </c>
-      <c r="D29" s="73"/>
-    </row>
-    <row r="30" spans="2:4" ht="38.25">
-      <c r="B30" s="27" t="s">
-        <v>702</v>
-      </c>
-      <c r="C30" s="74" t="s">
-        <v>703</v>
-      </c>
-      <c r="D30" s="75"/>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="27" t="s">
-        <v>704</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>705</v>
-      </c>
-      <c r="D31" s="27"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C25:D25"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -28741,7 +28857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0B4C89-AE87-4187-8C18-5F20544A3D88}">
   <dimension ref="A3:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -30027,14 +30143,14 @@
       <c r="D18" s="14" t="s">
         <v>583</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="66" t="s">
         <v>584</v>
       </c>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63"/>
-      <c r="I18" s="63"/>
-      <c r="J18" s="63"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
     </row>
     <row r="19" spans="2:13" ht="231.95" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -30046,17 +30162,17 @@
       <c r="D19" s="14" t="s">
         <v>587</v>
       </c>
-      <c r="E19" s="62" t="s">
+      <c r="E19" s="66" t="s">
         <v>588</v>
       </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="62"/>
-      <c r="M19" s="62"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="66"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
     </row>
     <row r="20" spans="2:13" ht="30">
       <c r="B20" s="7" t="s">
@@ -30092,10 +30208,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D19"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -30240,6 +30356,66 @@
       </c>
       <c r="D19" s="21" t="s">
         <v>622</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="60" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="27" t="s">
+        <v>710</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>708</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="27" t="s">
+        <v>711</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>618</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="30">
+      <c r="B26" s="38" t="s">
+        <v>715</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="27" t="s">
+        <v>718</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>716</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="27" t="s">
+        <v>720</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>719</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>721</v>
       </c>
     </row>
   </sheetData>
@@ -30417,17 +30593,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="69" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="65"/>
+      <c r="C2" s="69"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="70" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -30435,10 +30611,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="71" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="67"/>
+      <c r="B6" s="71"/>
     </row>
     <row r="7" spans="1:4" ht="45">
       <c r="A7" s="35" t="s">
@@ -30567,88 +30743,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="68" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="68"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="68" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="68"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="68" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="68"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="68" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="68"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="68" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="68" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="68"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="68" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="68"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="64" t="s">
+      <c r="A29" s="68" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="65" t="s">
+      <c r="A30" s="69" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="65"/>
-      <c r="C30" s="65"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="65" t="s">
+      <c r="A31" s="69" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="65"/>
-      <c r="C31" s="65"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="68" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="64" t="s">
+      <c r="A33" s="68" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
added info to ss tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC935DD-4EDB-48D1-B532-0DCACA519EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833F5B16-02B4-477C-B17C-B3B668C43DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="723">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -24554,55 +24554,6 @@
     <t>ss -i</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ss</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = socket statistics
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-i</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = show internal TCP information</t>
-    </r>
-  </si>
-  <si>
     <t>git commands</t>
   </si>
   <si>
@@ -26602,6 +26553,123 @@
   </si>
   <si>
     <t>follow prompts, select "Push an existing local repo to GitHub"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ss</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = socket statistics
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-i</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = show internal TCP information
+format: &lt;congestion_algorithm&gt;, wscale:&lt;snd&gt;:&lt;rcv&gt;, rto: &lt;value&gt;, </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cubic:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if you see this, this is the socket's congestion algorithm (algorithm that makes sure clients/servers don't send too much data at once)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">wscale:&lt;snd&gt;:&lt;rcv&gt;: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">window scale; client/server must agree on how many segments (chunks of data) to send/receive at one time
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">rto: &lt;icsk_rto&gt;: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> value is in millseconds; TCP starts timer when outbound segment is handed to IP layer. If no 'ack' is received for the data in a given segment before the timer expires, the segment is retransmitted.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -26979,11 +27047,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -27306,11 +27374,11 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -27345,7 +27413,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="29">
       <c r="A8" s="7" t="s">
         <v>63</v>
       </c>
@@ -27356,7 +27424,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="165">
+    <row r="9" spans="1:3" ht="159.5">
       <c r="A9" s="7" t="s">
         <v>66</v>
       </c>
@@ -27367,7 +27435,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="59.45" customHeight="1">
+    <row r="10" spans="1:3" ht="59.5" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>82</v>
       </c>
@@ -27378,7 +27446,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="60">
+    <row r="11" spans="1:3" ht="58">
       <c r="A11" s="8" t="s">
         <v>67</v>
       </c>
@@ -27389,7 +27457,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="60">
+    <row r="12" spans="1:3" ht="58">
       <c r="A12" s="8" t="s">
         <v>68</v>
       </c>
@@ -27411,7 +27479,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3">
       <c r="A14" s="8" t="s">
         <v>170</v>
       </c>
@@ -27422,7 +27490,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30">
+    <row r="15" spans="1:3" ht="29">
       <c r="A15" s="8" t="s">
         <v>169</v>
       </c>
@@ -27455,7 +27523,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="8" t="s">
         <v>78</v>
       </c>
@@ -27513,11 +27581,11 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="4" width="55.7109375" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="4" width="55.7265625" customWidth="1"/>
+    <col min="5" max="5" width="59.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
@@ -27527,7 +27595,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="120">
+    <row r="3" spans="1:13" ht="101.5">
       <c r="A3" s="28"/>
       <c r="B3" s="3"/>
       <c r="C3" s="39" t="s">
@@ -27590,7 +27658,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="75">
+    <row r="9" spans="1:13" ht="72.5">
       <c r="A9" s="72"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
@@ -27602,7 +27670,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30">
+    <row r="10" spans="1:13" ht="29">
       <c r="A10" s="72"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
@@ -27614,7 +27682,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45">
+    <row r="11" spans="1:13" ht="43.5">
       <c r="A11" s="72"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
@@ -27626,7 +27694,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45">
+    <row r="12" spans="1:13" ht="43.5">
       <c r="A12" s="72"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
@@ -27643,7 +27711,7 @@
       <c r="C14" s="9"/>
       <c r="D14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="60">
+    <row r="15" spans="1:13" ht="43.5">
       <c r="A15" s="73" t="s">
         <v>415</v>
       </c>
@@ -27657,7 +27725,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="75">
+    <row r="16" spans="1:13" ht="72.5">
       <c r="A16" s="73"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
@@ -27669,7 +27737,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="105">
+    <row r="17" spans="1:13" ht="87">
       <c r="A17" s="73"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
@@ -27681,7 +27749,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="105">
+    <row r="18" spans="1:13" ht="87">
       <c r="A18" s="73"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
@@ -27693,7 +27761,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="60">
+    <row r="19" spans="1:13" ht="58">
       <c r="A19" s="73" t="s">
         <v>415</v>
       </c>
@@ -27707,7 +27775,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="60">
+    <row r="20" spans="1:13" ht="58">
       <c r="A20" s="73"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
@@ -27719,7 +27787,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="105">
+    <row r="21" spans="1:13" ht="101.5">
       <c r="A21" s="73"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
@@ -27731,7 +27799,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="60">
+    <row r="22" spans="1:13" ht="58">
       <c r="A22" s="73"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
@@ -27765,7 +27833,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:13" ht="150">
+    <row r="25" spans="1:13" ht="130.5">
       <c r="B25" s="11" t="s">
         <v>538</v>
       </c>
@@ -27787,19 +27855,19 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" ht="150">
+    <row r="26" spans="1:13" ht="145">
       <c r="A26" s="28"/>
       <c r="B26" s="11" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>539</v>
       </c>
       <c r="D26" s="36" t="s">
+        <v>630</v>
+      </c>
+      <c r="E26" s="14" t="s">
         <v>631</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>632</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -27810,15 +27878,15 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" ht="165">
+    <row r="27" spans="1:13" ht="145">
       <c r="B27" s="11" t="s">
+        <v>632</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>633</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="D27" s="14" t="s">
         <v>634</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>635</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -27830,18 +27898,18 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" ht="200.1" customHeight="1">
+    <row r="28" spans="1:13" ht="200.15" customHeight="1">
       <c r="B28" s="11" t="s">
+        <v>635</v>
+      </c>
+      <c r="C28" s="17" t="s">
         <v>636</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="D28" s="14" t="s">
         <v>637</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="E28" s="4" t="s">
         <v>638</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>639</v>
       </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -27854,55 +27922,55 @@
     </row>
     <row r="29" spans="1:13" ht="195" customHeight="1">
       <c r="B29" s="11" t="s">
+        <v>639</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>640</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="D29" s="14" t="s">
         <v>641</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="E29" s="62" t="s">
         <v>642</v>
       </c>
-      <c r="E29" s="62" t="s">
+    </row>
+    <row r="30" spans="1:13" ht="211" customHeight="1">
+      <c r="B30" s="11" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="210.95" customHeight="1">
-      <c r="B30" s="11" t="s">
+      <c r="C30" s="17" t="s">
         <v>644</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="D30" s="14" t="s">
         <v>645</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="E30" s="62" t="s">
         <v>646</v>
       </c>
-      <c r="E30" s="62" t="s">
+    </row>
+    <row r="31" spans="1:13" ht="232">
+      <c r="B31" s="11" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="270">
-      <c r="B31" s="11" t="s">
+      <c r="C31" s="17" t="s">
         <v>648</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="D31" s="14" t="s">
         <v>649</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="E31" s="62" t="s">
         <v>650</v>
       </c>
-      <c r="E31" s="62" t="s">
+    </row>
+    <row r="32" spans="1:13" ht="72.5">
+      <c r="B32" s="11" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="75">
-      <c r="B32" s="11" t="s">
+      <c r="C32" s="17" t="s">
         <v>652</v>
       </c>
-      <c r="C32" s="17" t="s">
+      <c r="D32" s="14" t="s">
         <v>653</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>654</v>
       </c>
     </row>
   </sheetData>
@@ -27923,117 +27991,117 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="4" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.7265625" customWidth="1"/>
+    <col min="3" max="4" width="53.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" s="27" t="s">
+        <v>654</v>
+      </c>
+      <c r="C3" s="43" t="s">
         <v>655</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="D3" s="27" t="s">
         <v>656</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="27" t="s">
+        <v>657</v>
+      </c>
+      <c r="C4" s="43" t="s">
         <v>658</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="D4" s="27" t="s">
         <v>659</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="27" t="s">
+        <v>660</v>
+      </c>
+      <c r="C5" s="43" t="s">
         <v>661</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="D5" s="27" t="s">
         <v>662</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="27" t="s">
+        <v>663</v>
+      </c>
+      <c r="C6" s="43" t="s">
         <v>664</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="D6" s="27" t="s">
         <v>665</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="27" t="s">
+        <v>666</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>667</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="D7" s="27" t="s">
         <v>668</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="27" t="s">
+        <v>669</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>670</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="D8" s="27" t="s">
         <v>671</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="27" t="s">
+        <v>672</v>
+      </c>
+      <c r="C9" s="43" t="s">
         <v>673</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="D9" s="27" t="s">
         <v>674</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="27" t="s">
+        <v>675</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>676</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="D10" s="27" t="s">
         <v>677</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="11" spans="2:4">
       <c r="B11" s="27" t="s">
+        <v>678</v>
+      </c>
+      <c r="C11" s="43" t="s">
         <v>679</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="D11" s="27" t="s">
         <v>680</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="12" spans="2:4">
       <c r="B12" s="27" t="s">
+        <v>681</v>
+      </c>
+      <c r="C12" s="43" t="s">
         <v>682</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>683</v>
       </c>
       <c r="D12" s="27"/>
     </row>
@@ -28049,130 +28117,130 @@
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="27" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C15" s="27"/>
       <c r="D15" s="27"/>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="63" t="s">
+        <v>684</v>
+      </c>
+      <c r="C16" s="43" t="s">
         <v>685</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>686</v>
       </c>
       <c r="D16" s="27"/>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="63" t="s">
+        <v>686</v>
+      </c>
+      <c r="C17" s="43" t="s">
         <v>687</v>
-      </c>
-      <c r="C17" s="43" t="s">
-        <v>688</v>
       </c>
       <c r="D17" s="27"/>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="63" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="75" t="s">
-        <v>690</v>
-      </c>
-      <c r="D19" s="75"/>
+      <c r="C19" s="74" t="s">
+        <v>689</v>
+      </c>
+      <c r="D19" s="74"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="75" t="s">
-        <v>691</v>
-      </c>
-      <c r="D20" s="75"/>
+      <c r="C20" s="74" t="s">
+        <v>690</v>
+      </c>
+      <c r="D20" s="74"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="75" t="s">
-        <v>692</v>
-      </c>
-      <c r="D21" s="75"/>
+      <c r="C21" s="74" t="s">
+        <v>691</v>
+      </c>
+      <c r="D21" s="74"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="75" t="s">
-        <v>693</v>
-      </c>
-      <c r="D22" s="75"/>
+      <c r="C22" s="74" t="s">
+        <v>692</v>
+      </c>
+      <c r="D22" s="74"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="75" t="s">
-        <v>694</v>
-      </c>
-      <c r="D23" s="75"/>
+      <c r="C23" s="74" t="s">
+        <v>693</v>
+      </c>
+      <c r="D23" s="74"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="63" t="s">
+        <v>695</v>
+      </c>
+      <c r="C25" s="74" t="s">
         <v>696</v>
       </c>
-      <c r="C25" s="75" t="s">
-        <v>697</v>
-      </c>
-      <c r="D25" s="75"/>
+      <c r="D25" s="74"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="75" t="s">
-        <v>698</v>
-      </c>
-      <c r="D26" s="75"/>
+      <c r="C26" s="74" t="s">
+        <v>697</v>
+      </c>
+      <c r="D26" s="74"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="75" t="s">
-        <v>699</v>
-      </c>
-      <c r="D27" s="75"/>
+      <c r="C27" s="74" t="s">
+        <v>698</v>
+      </c>
+      <c r="D27" s="74"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="75" t="s">
-        <v>700</v>
-      </c>
-      <c r="D28" s="75"/>
+      <c r="C28" s="74" t="s">
+        <v>699</v>
+      </c>
+      <c r="D28" s="74"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="74" t="s">
+        <v>700</v>
+      </c>
+      <c r="D29" s="74"/>
+    </row>
+    <row r="30" spans="2:4" ht="39">
+      <c r="B30" s="27" t="s">
         <v>701</v>
       </c>
-      <c r="D29" s="75"/>
-    </row>
-    <row r="30" spans="2:4" ht="38.25">
-      <c r="B30" s="27" t="s">
+      <c r="C30" s="65" t="s">
         <v>702</v>
-      </c>
-      <c r="C30" s="65" t="s">
-        <v>703</v>
       </c>
       <c r="D30" s="64"/>
     </row>
     <row r="31" spans="2:4">
       <c r="B31" s="27" t="s">
+        <v>703</v>
+      </c>
+      <c r="C31" s="43" t="s">
         <v>704</v>
-      </c>
-      <c r="C31" s="43" t="s">
-        <v>705</v>
       </c>
       <c r="D31" s="27"/>
     </row>
@@ -28201,16 +28269,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="27"/>
-    <col min="2" max="2" width="43.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="27" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="42.42578125" style="27" customWidth="1"/>
-    <col min="7" max="8" width="40.5703125" style="27" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="8.81640625" style="27"/>
+    <col min="2" max="2" width="43.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="27" customWidth="1"/>
+    <col min="5" max="5" width="34.453125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" style="27" customWidth="1"/>
+    <col min="7" max="8" width="40.54296875" style="27" customWidth="1"/>
+    <col min="9" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -28223,7 +28291,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="29.45" customHeight="1">
+    <row r="5" spans="2:8" ht="29.5" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>466</v>
       </c>
@@ -28247,7 +28315,7 @@
       </c>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="2:8" ht="29.1" customHeight="1">
+    <row r="7" spans="2:8" ht="29.15" customHeight="1">
       <c r="C7" s="27" t="s">
         <v>465</v>
       </c>
@@ -28256,7 +28324,7 @@
       </c>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="2:8" ht="45">
+    <row r="8" spans="2:8" ht="43.5">
       <c r="C8" s="27" t="s">
         <v>467</v>
       </c>
@@ -28273,7 +28341,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="2:8" ht="30">
+    <row r="11" spans="2:8" ht="29">
       <c r="B11" s="10" t="s">
         <v>477</v>
       </c>
@@ -28285,7 +28353,7 @@
       </c>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="2:8" ht="115.35" customHeight="1">
+    <row r="12" spans="2:8" ht="115.4" customHeight="1">
       <c r="B12" s="10" t="s">
         <v>472</v>
       </c>
@@ -28297,7 +28365,7 @@
       </c>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="2:8" ht="45">
+    <row r="13" spans="2:8" ht="43.5">
       <c r="B13" s="46" t="s">
         <v>459</v>
       </c>
@@ -28309,7 +28377,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="2:8" ht="30">
+    <row r="14" spans="2:8" ht="29">
       <c r="B14" s="46" t="s">
         <v>478</v>
       </c>
@@ -28321,7 +28389,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="2:8" ht="101.1" customHeight="1">
+    <row r="15" spans="2:8" ht="101.15" customHeight="1">
       <c r="B15" s="8" t="s">
         <v>481</v>
       </c>
@@ -28333,7 +28401,7 @@
       </c>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="2:8" ht="75">
+    <row r="16" spans="2:8" ht="72.5">
       <c r="B16" s="8" t="s">
         <v>495</v>
       </c>
@@ -28356,7 +28424,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="90">
+    <row r="17" spans="2:8" ht="58">
       <c r="B17" s="8" t="s">
         <v>494</v>
       </c>
@@ -28371,7 +28439,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="2:8" ht="45">
+    <row r="18" spans="2:8" ht="43.5">
       <c r="B18" s="8" t="s">
         <v>491</v>
       </c>
@@ -28386,7 +28454,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="2:8" ht="75">
+    <row r="19" spans="2:8" ht="72.5">
       <c r="B19" s="8" t="s">
         <v>496</v>
       </c>
@@ -28401,7 +28469,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="2:8" ht="120">
+    <row r="20" spans="2:8" ht="116">
       <c r="B20" s="8" t="s">
         <v>501</v>
       </c>
@@ -28418,7 +28486,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="2:8" ht="43.35" customHeight="1">
+    <row r="21" spans="2:8" ht="43.4" customHeight="1">
       <c r="B21" s="8" t="s">
         <v>504</v>
       </c>
@@ -28433,7 +28501,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="2:8" ht="90">
+    <row r="22" spans="2:8" ht="87">
       <c r="B22" s="8" t="s">
         <v>510</v>
       </c>
@@ -28448,7 +28516,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="2:8" ht="30">
+    <row r="23" spans="2:8">
       <c r="B23" s="8" t="s">
         <v>543</v>
       </c>
@@ -28477,7 +28545,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="2:8" ht="30">
+    <row r="26" spans="2:8" ht="29">
       <c r="B26" s="10" t="s">
         <v>505</v>
       </c>
@@ -28513,7 +28581,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="2:8" ht="30">
+    <row r="30" spans="2:8" ht="29">
       <c r="B30" s="46" t="s">
         <v>509</v>
       </c>
@@ -28524,7 +28592,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="14.45" customHeight="1"/>
+    <row r="32" spans="2:8" ht="14.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4294967295" r:id="rId1"/>
@@ -28539,18 +28607,18 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="75" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -28580,19 +28648,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="75" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="74"/>
+      <c r="C11" s="75"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="75" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="74"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -28616,12 +28684,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="16.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -28629,13 +28697,13 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="29">
       <c r="B4" s="39" t="s">
         <v>419</v>
       </c>
       <c r="C4" s="38"/>
     </row>
-    <row r="6" spans="1:3" ht="90">
+    <row r="6" spans="1:3" ht="87">
       <c r="A6" s="44" t="s">
         <v>420</v>
       </c>
@@ -28660,12 +28728,12 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -28678,7 +28746,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>430</v>
       </c>
@@ -28713,12 +28781,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -28731,7 +28799,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>438</v>
       </c>
@@ -28742,7 +28810,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="46" t="s">
         <v>441</v>
       </c>
@@ -28766,12 +28834,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="38" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="38" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="38" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="38"/>
+    <col min="1" max="1" width="23.54296875" style="38" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="38" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="38"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -28779,12 +28847,12 @@
         <v>444</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="29">
       <c r="B4" s="39" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>446</v>
       </c>
@@ -28795,7 +28863,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="46" t="s">
         <v>448</v>
       </c>
@@ -28819,12 +28887,12 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="43.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -28832,12 +28900,12 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45">
+    <row r="4" spans="1:3" ht="43.5">
       <c r="B4" s="39" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>426</v>
       </c>
@@ -28861,12 +28929,12 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.453125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="63.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -28875,7 +28943,7 @@
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="43.5">
       <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
@@ -28896,7 +28964,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45">
+    <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -28908,7 +28976,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="43.5">
       <c r="A8" s="7" t="s">
         <v>87</v>
       </c>
@@ -28920,7 +28988,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="90">
+    <row r="9" spans="1:4" ht="72.5">
       <c r="A9" s="8" t="s">
         <v>269</v>
       </c>
@@ -28932,7 +29000,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="43.5">
       <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
@@ -28944,7 +29012,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="75">
+    <row r="11" spans="1:4" ht="58">
       <c r="A11" s="8" t="s">
         <v>264</v>
       </c>
@@ -28956,7 +29024,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" s="12" customFormat="1" ht="45">
+    <row r="12" spans="1:4" s="12" customFormat="1" ht="43.5">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -28968,7 +29036,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" s="12" customFormat="1" ht="45">
+    <row r="13" spans="1:4" s="12" customFormat="1" ht="43.5">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -28980,7 +29048,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="45">
+    <row r="14" spans="1:4" ht="43.5">
       <c r="A14" s="8" t="s">
         <v>275</v>
       </c>
@@ -28992,7 +29060,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" ht="45">
+    <row r="15" spans="1:4" s="3" customFormat="1" ht="43.5">
       <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
@@ -29004,7 +29072,7 @@
       </c>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" ht="45">
+    <row r="16" spans="1:4" ht="43.5">
       <c r="A16" s="8" t="s">
         <v>218</v>
       </c>
@@ -29016,7 +29084,7 @@
       </c>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="60">
+    <row r="17" spans="1:4" ht="43.5">
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
@@ -29028,7 +29096,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="60">
+    <row r="18" spans="1:4" ht="43.5">
       <c r="A18" s="7" t="s">
         <v>21</v>
       </c>
@@ -29040,7 +29108,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="75">
+    <row r="19" spans="1:4" ht="72.5">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -29052,7 +29120,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="90">
+    <row r="20" spans="1:4" ht="87">
       <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
@@ -29064,7 +29132,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" ht="60">
+    <row r="21" spans="1:4" ht="58">
       <c r="A21" s="30" t="s">
         <v>224</v>
       </c>
@@ -29076,7 +29144,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="29">
       <c r="A22" s="12" t="s">
         <v>22</v>
       </c>
@@ -29088,7 +29156,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" ht="30">
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="29">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -29107,10 +29175,10 @@
         <v>321</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="75">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="72.5">
       <c r="A25" s="8" t="s">
         <v>227</v>
       </c>
@@ -29122,7 +29190,7 @@
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" ht="120">
+    <row r="26" spans="1:4" ht="87">
       <c r="A26" s="6" t="s">
         <v>229</v>
       </c>
@@ -29134,7 +29202,7 @@
       </c>
       <c r="D26" s="12"/>
     </row>
-    <row r="27" spans="1:4" ht="60">
+    <row r="27" spans="1:4" ht="58">
       <c r="A27" s="6" t="s">
         <v>231</v>
       </c>
@@ -29182,11 +29250,11 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.54296875" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
@@ -29208,7 +29276,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="45">
+    <row r="5" spans="1:6" ht="43.5">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -29219,7 +29287,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
+    <row r="6" spans="1:6" ht="43.5">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -29230,7 +29298,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60">
+    <row r="7" spans="1:6" ht="58">
       <c r="A7" s="6" t="s">
         <v>104</v>
       </c>
@@ -29241,7 +29309,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="43.5">
       <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
@@ -29255,7 +29323,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="195">
+    <row r="9" spans="1:6" ht="174">
       <c r="A9" s="8" t="s">
         <v>119</v>
       </c>
@@ -29266,7 +29334,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45">
+    <row r="10" spans="1:6" ht="43.5">
       <c r="A10" s="8" t="s">
         <v>90</v>
       </c>
@@ -29277,7 +29345,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="75">
+    <row r="11" spans="1:6" ht="72.5">
       <c r="A11" s="8" t="s">
         <v>92</v>
       </c>
@@ -29288,7 +29356,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60">
+    <row r="12" spans="1:6" ht="58">
       <c r="A12" s="8" t="s">
         <v>93</v>
       </c>
@@ -29299,7 +29367,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="75">
+    <row r="13" spans="1:6" ht="72.5">
       <c r="A13" s="8" t="s">
         <v>97</v>
       </c>
@@ -29310,7 +29378,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="90">
+    <row r="14" spans="1:6" ht="72.5">
       <c r="A14" s="8" t="s">
         <v>98</v>
       </c>
@@ -29321,7 +29389,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60">
+    <row r="15" spans="1:6" ht="58">
       <c r="A15" s="8" t="s">
         <v>99</v>
       </c>
@@ -29332,7 +29400,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="90">
+    <row r="16" spans="1:6" ht="87">
       <c r="A16" s="8" t="s">
         <v>103</v>
       </c>
@@ -29343,7 +29411,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="75">
+    <row r="17" spans="1:3" ht="72.5">
       <c r="A17" s="8" t="s">
         <v>101</v>
       </c>
@@ -29354,7 +29422,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="105">
+    <row r="18" spans="1:3" ht="87">
       <c r="A18" s="8" t="s">
         <v>196</v>
       </c>
@@ -29365,7 +29433,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90">
+    <row r="19" spans="1:3" ht="87">
       <c r="A19" s="8" t="s">
         <v>102</v>
       </c>
@@ -29376,7 +29444,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="60">
+    <row r="20" spans="1:3" ht="43.5">
       <c r="A20" s="8" t="s">
         <v>203</v>
       </c>
@@ -29387,7 +29455,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="90">
+    <row r="21" spans="1:3" ht="87">
       <c r="A21" s="8" t="s">
         <v>106</v>
       </c>
@@ -29398,7 +29466,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="8" t="s">
         <v>108</v>
       </c>
@@ -29409,7 +29477,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="90">
+    <row r="23" spans="1:3" ht="87">
       <c r="A23" s="8" t="s">
         <v>109</v>
       </c>
@@ -29420,7 +29488,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="105">
+    <row r="24" spans="1:3" ht="87">
       <c r="A24" s="8" t="s">
         <v>110</v>
       </c>
@@ -29442,7 +29510,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="90">
+    <row r="26" spans="1:3" ht="72.5">
       <c r="A26" s="8" t="s">
         <v>111</v>
       </c>
@@ -29453,7 +29521,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="90">
+    <row r="27" spans="1:3" ht="87">
       <c r="A27" s="8" t="s">
         <v>113</v>
       </c>
@@ -29464,7 +29532,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="75">
+    <row r="28" spans="1:3" ht="72.5">
       <c r="A28" s="8" t="s">
         <v>114</v>
       </c>
@@ -29475,7 +29543,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="120">
+    <row r="29" spans="1:3" ht="116">
       <c r="A29" s="8" t="s">
         <v>115</v>
       </c>
@@ -29486,7 +29554,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="195">
+    <row r="30" spans="1:3" ht="174">
       <c r="A30" s="6" t="s">
         <v>116</v>
       </c>
@@ -29497,7 +29565,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="210">
+    <row r="31" spans="1:3" ht="159.5">
       <c r="A31" s="6" t="s">
         <v>117</v>
       </c>
@@ -29508,7 +29576,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="240">
+    <row r="32" spans="1:3" ht="203">
       <c r="A32" s="9" t="s">
         <v>60</v>
       </c>
@@ -29544,11 +29612,11 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -29573,7 +29641,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="27"/>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="29">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -29584,7 +29652,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60">
+    <row r="6" spans="1:3" ht="43.5">
       <c r="A6" s="3" t="s">
         <v>135</v>
       </c>
@@ -29595,7 +29663,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="10" t="s">
         <v>136</v>
       </c>
@@ -29606,7 +29674,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="29">
       <c r="A8" s="10" t="s">
         <v>139</v>
       </c>
@@ -29617,7 +29685,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45">
+    <row r="9" spans="1:3" ht="43.5">
       <c r="A9" s="10" t="s">
         <v>140</v>
       </c>
@@ -29628,7 +29696,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45">
+    <row r="10" spans="1:3" ht="43.5">
       <c r="A10" s="10" t="s">
         <v>142</v>
       </c>
@@ -29650,7 +29718,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="43.5">
       <c r="A12" s="10" t="s">
         <v>152</v>
       </c>
@@ -29661,7 +29729,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45">
+    <row r="13" spans="1:3" ht="43.5">
       <c r="A13" s="8" t="s">
         <v>156</v>
       </c>
@@ -29672,7 +29740,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="43.5">
       <c r="A14" s="8" t="s">
         <v>161</v>
       </c>
@@ -29683,7 +29751,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="75">
+    <row r="15" spans="1:3" ht="72.5">
       <c r="A15" s="8" t="s">
         <v>166</v>
       </c>
@@ -29694,7 +29762,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45">
+    <row r="16" spans="1:3" ht="43.5">
       <c r="A16" s="8" t="s">
         <v>175</v>
       </c>
@@ -29705,7 +29773,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="43.5">
       <c r="A17" s="8" t="s">
         <v>177</v>
       </c>
@@ -29716,7 +29784,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45">
+    <row r="18" spans="1:3" ht="43.5">
       <c r="A18" s="8" t="s">
         <v>178</v>
       </c>
@@ -29727,7 +29795,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45">
+    <row r="19" spans="1:3" ht="43.5">
       <c r="A19" s="8" t="s">
         <v>181</v>
       </c>
@@ -29738,7 +29806,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="60">
+    <row r="20" spans="1:3" ht="58">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
@@ -29749,7 +29817,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="90">
+    <row r="21" spans="1:3" ht="72.5">
       <c r="A21" s="10" t="s">
         <v>150</v>
       </c>
@@ -29760,7 +29828,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="8" t="s">
         <v>183</v>
       </c>
@@ -29771,7 +29839,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60">
+    <row r="23" spans="1:3" ht="58">
       <c r="A23" s="10" t="s">
         <v>67</v>
       </c>
@@ -29782,7 +29850,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="90">
+    <row r="24" spans="1:3" ht="87">
       <c r="A24" s="8" t="s">
         <v>186</v>
       </c>
@@ -29793,7 +29861,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="120">
+    <row r="25" spans="1:3" ht="101.5">
       <c r="A25" s="10" t="s">
         <v>232</v>
       </c>
@@ -29804,7 +29872,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="90">
+    <row r="26" spans="1:3" ht="72.5">
       <c r="A26" s="8" t="s">
         <v>234</v>
       </c>
@@ -29815,7 +29883,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="75">
+    <row r="27" spans="1:3" ht="72.5">
       <c r="A27" s="10" t="s">
         <v>236</v>
       </c>
@@ -29826,7 +29894,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="45">
+    <row r="28" spans="1:3" ht="43.5">
       <c r="A28" s="7" t="s">
         <v>240</v>
       </c>
@@ -29837,7 +29905,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="75">
+    <row r="29" spans="1:3" ht="58">
       <c r="A29" s="7" t="s">
         <v>242</v>
       </c>
@@ -29848,7 +29916,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="45.6" customHeight="1">
+    <row r="30" spans="1:3" ht="45.65" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>245</v>
       </c>
@@ -29859,7 +29927,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="45">
+    <row r="31" spans="1:3" ht="43.5">
       <c r="A31" s="7" t="s">
         <v>247</v>
       </c>
@@ -29870,7 +29938,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="45">
+    <row r="32" spans="1:3" ht="43.5">
       <c r="A32" s="7" t="s">
         <v>251</v>
       </c>
@@ -29881,7 +29949,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="45">
+    <row r="33" spans="1:3" ht="43.5">
       <c r="A33" s="8" t="s">
         <v>148</v>
       </c>
@@ -29892,7 +29960,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="60">
+    <row r="34" spans="1:3" ht="58">
       <c r="A34" s="8" t="s">
         <v>148</v>
       </c>
@@ -29981,17 +30049,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F8480C-E8CD-45AC-8F81-8D4ABFF602C5}">
   <dimension ref="B2:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="28"/>
-    <col min="2" max="2" width="30.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="28"/>
+    <col min="1" max="1" width="8.81640625" style="28"/>
+    <col min="2" max="2" width="30.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -29999,7 +30067,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="60">
+    <row r="3" spans="2:4" ht="58">
       <c r="C3" s="37" t="s">
         <v>545</v>
       </c>
@@ -30023,7 +30091,7 @@
       <c r="B7" s="59"/>
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="2:4" ht="30">
+    <row r="8" spans="2:4" ht="29">
       <c r="B8" s="11" t="s">
         <v>560</v>
       </c>
@@ -30034,7 +30102,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30">
+    <row r="9" spans="2:4" ht="29">
       <c r="B9" s="7" t="s">
         <v>553</v>
       </c>
@@ -30045,7 +30113,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30">
+    <row r="10" spans="2:4" ht="29">
       <c r="B10" s="7" t="s">
         <v>556</v>
       </c>
@@ -30056,7 +30124,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="30">
+    <row r="11" spans="2:4" ht="29">
       <c r="B11" s="11" t="s">
         <v>559</v>
       </c>
@@ -30067,7 +30135,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="30">
+    <row r="12" spans="2:4" ht="29">
       <c r="B12" s="11" t="s">
         <v>563</v>
       </c>
@@ -30078,7 +30146,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="45">
+    <row r="13" spans="2:4" ht="43.5">
       <c r="B13" s="11" t="s">
         <v>565</v>
       </c>
@@ -30089,7 +30157,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="45">
+    <row r="14" spans="2:4" ht="43.5">
       <c r="B14" s="11" t="s">
         <v>569</v>
       </c>
@@ -30100,7 +30168,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="45">
+    <row r="15" spans="2:4" ht="43.5">
       <c r="B15" s="11" t="s">
         <v>571</v>
       </c>
@@ -30111,7 +30179,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="30">
+    <row r="16" spans="2:4" ht="29">
       <c r="B16" s="7" t="s">
         <v>574</v>
       </c>
@@ -30122,7 +30190,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="165">
+    <row r="17" spans="2:13" ht="159.5">
       <c r="B17" s="7" t="s">
         <v>578</v>
       </c>
@@ -30133,7 +30201,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="144.94999999999999" customHeight="1">
+    <row r="18" spans="2:13" ht="145" customHeight="1">
       <c r="B18" s="11" t="s">
         <v>581</v>
       </c>
@@ -30152,7 +30220,7 @@
       <c r="I18" s="67"/>
       <c r="J18" s="67"/>
     </row>
-    <row r="19" spans="2:13" ht="231.95" customHeight="1">
+    <row r="19" spans="2:13" ht="232" customHeight="1">
       <c r="B19" s="7" t="s">
         <v>585</v>
       </c>
@@ -30174,7 +30242,7 @@
       <c r="L19" s="66"/>
       <c r="M19" s="66"/>
     </row>
-    <row r="20" spans="2:13" ht="30">
+    <row r="20" spans="2:13" ht="29">
       <c r="B20" s="7" t="s">
         <v>589</v>
       </c>
@@ -30185,7 +30253,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="30">
+    <row r="21" spans="2:13" ht="105" customHeight="1">
       <c r="B21" s="7" t="s">
         <v>592</v>
       </c>
@@ -30193,13 +30261,25 @@
         <v>593</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>594</v>
-      </c>
+        <v>721</v>
+      </c>
+      <c r="E21" s="69" t="s">
+        <v>722</v>
+      </c>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E18:J18"/>
     <mergeCell ref="E19:M19"/>
+    <mergeCell ref="E21:M21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -30210,212 +30290,212 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="27"/>
-    <col min="2" max="3" width="43.5703125" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="27"/>
+    <col min="1" max="1" width="8.7265625" style="27"/>
+    <col min="2" max="3" width="43.54296875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
       <c r="B2" s="43" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="4" spans="2:4">
       <c r="B4" s="60" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="27" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C5" s="43" t="s">
+        <v>597</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>598</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="27" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C6" s="43" t="s">
+        <v>595</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>596</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="45" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C7" s="43" t="s">
+        <v>599</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>600</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="8" spans="2:4">
       <c r="B8" s="45" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C8" s="43" t="s">
+        <v>601</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>602</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="9" spans="2:4">
       <c r="B9" s="45" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C9" s="43" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="45" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C10" s="43" t="s">
+        <v>604</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>605</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="60" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="27" t="s">
+        <v>622</v>
+      </c>
+      <c r="C15" s="43" t="s">
         <v>623</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="D15" s="61" t="s">
         <v>624</v>
-      </c>
-      <c r="D15" s="61" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="27" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C16" s="43" t="s">
+        <v>607</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>608</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17" s="27" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C17" s="43" t="s">
+        <v>617</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>618</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="27" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C18" s="43" t="s">
+        <v>627</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>628</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C19" s="43" t="s">
+        <v>620</v>
+      </c>
+      <c r="D19" s="21" t="s">
         <v>621</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="60" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="27" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="C24" s="43" t="s">
+        <v>707</v>
+      </c>
+      <c r="D24" s="45" t="s">
         <v>708</v>
-      </c>
-      <c r="D24" s="45" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="27" t="s">
+        <v>710</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>617</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>711</v>
       </c>
-      <c r="C25" s="43" t="s">
-        <v>618</v>
-      </c>
-      <c r="D25" s="27" t="s">
+    </row>
+    <row r="26" spans="2:4" ht="29">
+      <c r="B26" s="38" t="s">
+        <v>714</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" ht="30">
-      <c r="B26" s="38" t="s">
-        <v>715</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="46" t="s">
         <v>713</v>
-      </c>
-      <c r="D26" s="46" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C27" s="43" t="s">
+        <v>715</v>
+      </c>
+      <c r="D27" s="27" t="s">
         <v>716</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27" t="s">
+        <v>719</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>718</v>
+      </c>
+      <c r="D28" s="27" t="s">
         <v>720</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>719</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>721</v>
       </c>
     </row>
   </sheetData>
@@ -30432,13 +30512,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="27"/>
-    <col min="2" max="2" width="30.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="8.81640625" style="27"/>
+    <col min="2" max="2" width="30.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -30466,7 +30546,7 @@
       <c r="B6" s="45"/>
       <c r="C6" s="43"/>
     </row>
-    <row r="7" spans="2:4" ht="30">
+    <row r="7" spans="2:4" ht="29">
       <c r="B7" s="46" t="s">
         <v>550</v>
       </c>
@@ -30478,7 +30558,7 @@
     <row r="9" spans="2:4">
       <c r="B9" s="45"/>
     </row>
-    <row r="10" spans="2:4" ht="101.45" customHeight="1">
+    <row r="10" spans="2:4" ht="101.5" customHeight="1">
       <c r="B10" s="45"/>
       <c r="C10" s="43"/>
       <c r="D10" s="38"/>
@@ -30500,10 +30580,10 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -30542,7 +30622,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="101.45" customHeight="1">
+    <row r="9" spans="1:3" ht="101.5" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>295</v>
       </c>
@@ -30575,13 +30655,13 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="28"/>
+    <col min="1" max="1" width="30.453125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="48.81640625" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -30616,7 +30696,7 @@
       </c>
       <c r="B6" s="71"/>
     </row>
-    <row r="7" spans="1:4" ht="45">
+    <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="35" t="s">
         <v>345</v>
       </c>
@@ -30649,7 +30729,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="90">
+    <row r="10" spans="1:4" ht="72.5">
       <c r="A10" s="9" t="s">
         <v>351</v>
       </c>
@@ -30709,7 +30789,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="4" t="s">
         <v>355</v>
       </c>
@@ -30731,7 +30811,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75">
+    <row r="20" spans="1:3" ht="58">
       <c r="A20" s="4" t="s">
         <v>369</v>
       </c>

</xml_diff>

<commit_message>
added more info to the ss tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833F5B16-02B4-477C-B17C-B3B668C43DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F15CD9A-8784-4FEA-BFF1-2B41446C7055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -26601,13 +26601,14 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> = show internal TCP information
-format: &lt;congestion_algorithm&gt;, wscale:&lt;snd&gt;:&lt;rcv&gt;, rto: &lt;value&gt;, </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
+format: &lt;congestion_algorithm&gt;, wscale:&lt;snd&gt;:&lt;rcv&gt;, rto: &lt;value&gt;, rtt: &lt;value&gt;/&lt;avg deviation&gt;, mss: &lt;value&gt;, pmtu: &lt;value&gt;, </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -26618,6 +26619,7 @@
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -26630,6 +26632,7 @@
     <r>
       <rPr>
         <b/>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -26640,6 +26643,7 @@
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -26652,23 +26656,121 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">rto: &lt;icsk_rto&gt;: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> value is in millseconds; TCP starts timer when outbound segment is handed to IP layer. If no 'ack' is received for the data in a given segment before the timer expires, the segment is retransmitted.</t>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">rto: &lt;value&gt;: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> value is in millseconds; TCP starts timer when outbound segment is handed to IP layer. If no 'ack' is received for the data in a given segment before the timer expires, the segment is retransmitted
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rtt: &lt;value&gt;/&lt;avg deviation&gt;:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> average round trip time in milliseconds (from client to server and back again); The first value is the avg round trip time, the second value is the avg deviation from the from the average round trip time
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mss: &lt;value&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: maximum segment size; the largest segment the local host will accept
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pmtu: &lt;value&gt;: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">path MTU value; path MTU is the largest packet size that can traverse this path without suffering fragmentation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>note 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'segment' is the Protocol Data Unit (PDU) at the Transport layer (layer 4)</t>
     </r>
   </si>
 </sst>
@@ -26836,7 +26938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -27030,10 +27132,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -27052,6 +27154,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -28626,11 +28731,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="69" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -28697,7 +28802,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29">
+    <row r="4" spans="1:3">
       <c r="B4" s="39" t="s">
         <v>419</v>
       </c>
@@ -30050,7 +30155,7 @@
   <dimension ref="B2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="E18" sqref="E18:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -30197,7 +30302,7 @@
       <c r="C17" s="17" t="s">
         <v>579</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="76" t="s">
         <v>580</v>
       </c>
     </row>
@@ -30208,7 +30313,7 @@
       <c r="C18" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="76" t="s">
         <v>583</v>
       </c>
       <c r="E18" s="66" t="s">
@@ -30220,14 +30325,14 @@
       <c r="I18" s="67"/>
       <c r="J18" s="67"/>
     </row>
-    <row r="19" spans="2:13" ht="232" customHeight="1">
+    <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
         <v>585</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>586</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="76" t="s">
         <v>587</v>
       </c>
       <c r="E19" s="66" t="s">
@@ -30253,27 +30358,27 @@
         <v>591</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="105" customHeight="1">
+    <row r="21" spans="2:13" ht="210" customHeight="1">
       <c r="B21" s="7" t="s">
         <v>592</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>593</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="76" t="s">
         <v>721</v>
       </c>
-      <c r="E21" s="69" t="s">
+      <c r="E21" s="66" t="s">
         <v>722</v>
       </c>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -30673,10 +30778,10 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="68" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="69"/>
+      <c r="C2" s="68"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="70" t="s">
@@ -30823,88 +30928,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="69" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="69" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="68" t="s">
+      <c r="A24" s="69" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="68" t="s">
+      <c r="A25" s="69" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="68"/>
-      <c r="C25" s="68"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="68" t="s">
+      <c r="A26" s="69" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="68"/>
-      <c r="C26" s="68"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="68" t="s">
+      <c r="A27" s="69" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="69" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="68" t="s">
+      <c r="A29" s="69" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="68"/>
-      <c r="C29" s="68"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="68" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="68" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="68"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="68" t="s">
+      <c r="A32" s="69" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="68"/>
-      <c r="C32" s="68"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="68" t="s">
+      <c r="A33" s="69" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
added hard local repo reset
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134283AF-06E4-45CB-A3A5-0F1EB9808360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F903833E-F261-476F-AE87-77154A82E371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="740">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -27219,6 +27219,21 @@
   </si>
   <si>
     <t>sets the default action to 'ACCEPT' for the 'INPUT' policy</t>
+  </si>
+  <si>
+    <t>OVERWRITE LOCAL REPOSITORY WITH REMOTE</t>
+  </si>
+  <si>
+    <t>git fetch --all</t>
+  </si>
+  <si>
+    <t>git reset --hard origin</t>
+  </si>
+  <si>
+    <t>fetch all remote repo differences</t>
+  </si>
+  <si>
+    <t>reset local repository with remote repo</t>
   </si>
 </sst>
 </file>
@@ -27581,6 +27596,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -27604,9 +27622,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -28154,17 +28169,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="70"/>
+      <c r="C2" s="71"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="72" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -28172,10 +28187,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="73" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="72"/>
+      <c r="B6" s="73"/>
     </row>
     <row r="7" spans="1:4" ht="45">
       <c r="A7" s="35" t="s">
@@ -28304,88 +28319,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="69" t="s">
+      <c r="A22" s="70" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
+      <c r="B22" s="70"/>
+      <c r="C22" s="70"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="70" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="70" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="69" t="s">
+      <c r="A25" s="70" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="69" t="s">
+      <c r="A26" s="70" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="70" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="70" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="70" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="70"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="71" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="70" t="s">
+      <c r="A31" s="71" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="70"/>
-      <c r="C31" s="70"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="70" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="70" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
+      <c r="B33" s="70"/>
+      <c r="C33" s="70"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">
@@ -28574,7 +28589,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="74" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -28588,7 +28603,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="75">
-      <c r="A9" s="73"/>
+      <c r="A9" s="74"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -28600,7 +28615,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="30">
-      <c r="A10" s="73"/>
+      <c r="A10" s="74"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -28612,7 +28627,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="45">
-      <c r="A11" s="73"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -28624,7 +28639,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="45">
-      <c r="A12" s="73"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -28641,7 +28656,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="60">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="75" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -28655,7 +28670,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="75">
-      <c r="A16" s="74"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -28667,7 +28682,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="105">
-      <c r="A17" s="74"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -28679,7 +28694,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="105">
-      <c r="A18" s="74"/>
+      <c r="A18" s="75"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -28691,7 +28706,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="60">
-      <c r="A19" s="74" t="s">
+      <c r="A19" s="75" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -28705,7 +28720,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="60">
-      <c r="A20" s="74"/>
+      <c r="A20" s="75"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -28717,7 +28732,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="105">
-      <c r="A21" s="74"/>
+      <c r="A21" s="75"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -28729,7 +28744,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="60">
-      <c r="A22" s="74"/>
+      <c r="A22" s="75"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -29078,38 +29093,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="76" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="75"/>
+      <c r="D19" s="76"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="76" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="75"/>
+      <c r="D20" s="76"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="76" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="75"/>
+      <c r="D21" s="76"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="76" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="75"/>
+      <c r="D22" s="76"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="76" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="75"/>
+      <c r="D23" s="76"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -29122,38 +29137,38 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="76" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="75"/>
+      <c r="D25" s="76"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="76" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="75"/>
+      <c r="D26" s="76"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="75" t="s">
+      <c r="C27" s="76" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="75"/>
+      <c r="D27" s="76"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="75" t="s">
+      <c r="C28" s="76" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="75"/>
+      <c r="D28" s="76"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="76" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="75"/>
+      <c r="D29" s="76"/>
     </row>
     <row r="30" spans="2:4" ht="38.25">
       <c r="B30" s="27" t="s">
@@ -29542,12 +29557,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="77" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -29555,11 +29570,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="70" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -29577,19 +29592,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="76" t="s">
+      <c r="B11" s="77" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="76"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="77" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="76"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -30978,7 +30993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F8480C-E8CD-45AC-8F81-8D4ABFF602C5}">
   <dimension ref="B2:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="E18" sqref="E18:J18"/>
     </sheetView>
   </sheetViews>
@@ -31239,17 +31254,17 @@
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
       <c r="B4" s="27"/>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="69" t="s">
         <v>724</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="69"/>
     </row>
     <row r="5" spans="2:4" ht="90" customHeight="1">
       <c r="B5" s="27"/>
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="69" t="s">
         <v>725</v>
       </c>
-      <c r="D5" s="77"/>
+      <c r="D5" s="69"/>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="27"/>
@@ -31300,10 +31315,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D28"/>
+  <dimension ref="B2:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -31508,6 +31523,27 @@
       </c>
       <c r="D28" s="27" t="s">
         <v>720</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="60" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3">
+      <c r="B33" s="27" t="s">
+        <v>738</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3">
+      <c r="B34" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="C34" s="43" t="s">
+        <v>737</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more info to iptables tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D7A1B2-7DE7-4F27-A9F9-864E68933C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC373F3-4175-4284-AD28-AAED8ABB7638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="745">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -26779,6 +26779,257 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-A </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>append</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a rule to the end of a selected chain</t>
+    </r>
+  </si>
+  <si>
+    <t>iptables -A INPUT -s 10.10.10.10 -j DROP</t>
+  </si>
+  <si>
+    <r>
+      <t>Append (attach) this new rule to the INPUT chain; anything from source 10.10.10.10, DROP the data'
+'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-A: appends</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (attaches) the rule to the end of the INPUT chain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-s: source</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; where the data is coming from
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-j: jump</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; as in 'jump to the DROP action'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-L</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>list</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> all rules in selected chain</t>
+    </r>
+  </si>
+  <si>
+    <t>iptables -L</t>
+  </si>
+  <si>
+    <t>lists all rules on all chains</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">--policy &lt;CHAIN&gt; &lt;ACTION&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= sets the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>policy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for an iptables chain</t>
+    </r>
+  </si>
+  <si>
+    <t>OVERWRITE LOCAL REPOSITORY WITH REMOTE</t>
+  </si>
+  <si>
+    <t>git fetch --all</t>
+  </si>
+  <si>
+    <t>fetch all remote repo differences</t>
+  </si>
+  <si>
+    <t>reset local repository with remote repo</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">host firewall installed by default on Linux systems. 
 It uses 3 lists or 'chains':
 Input chain: </t>
@@ -26834,8 +27085,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">list for incoming connections not meant for the local system but rather being passed through 
-or 'forwarded' on to another destination
+      <t xml:space="preserve">list that controls incoming connections not meant for the local system but rather just being passed through or 'forwarded' on to another destination
 </t>
     </r>
     <r>
@@ -26857,7 +27107,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">list that tells iptables how to handle data being sent </t>
+      <t xml:space="preserve">list that controls how data being sent </t>
     </r>
     <r>
       <rPr>
@@ -26878,7 +27128,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">of the local host to another destination
+      <t xml:space="preserve">of the local host to another destination is handled
 </t>
     </r>
     <r>
@@ -26972,20 +27222,177 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>block data flow without giving an explanation to the sender. Use if you don't want the sender to know that the system exists.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-A </t>
+      <t>block data flow without giving an explanation to the sender. Use if you don't want the sender to know that they are being blocked by a firewall, or that a system exists.</t>
+    </r>
+  </si>
+  <si>
+    <t>iptables -L -v</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>verbose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> output</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">lists all rules on all chains in verbose mode; which displays the interface name, rule options (if any) and TOS masks
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-L</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>List</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> all rules
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-v</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>verbose</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> output</t>
+    </r>
+  </si>
+  <si>
+    <t>iptables --policy INPUT ACCEPT
+iptables --policy OUTPUT ACCEPT
+iptables --policy FORWARD ACCEPT</t>
+  </si>
+  <si>
+    <t>sets the default action to 'ACCEPT' for the 'INPUT' policy
+sets the default action to 'ACCEPT' for the 'OUTPUT' policy
+sets the default action to 'ACCEPT' for the 'FORWARD' policy
+setting the default policy for these 3 lists or 'chains' sets the default policy to 'ACCEPT' for the entire firewall</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-I &lt;CHAIN&gt; &lt;NUMBER&gt; </t>
     </r>
     <r>
       <rPr>
@@ -27006,234 +27413,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>append</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> a rule to the end of a selected chain</t>
-    </r>
-  </si>
-  <si>
-    <t>iptables -A INPUT -s 10.10.10.10 -j DROP</t>
-  </si>
-  <si>
-    <r>
-      <t>Append (attach) this new rule to the INPUT chain; anything from source 10.10.10.10, DROP the data'
-'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-A: appends</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (attaches) the rule to the end of the INPUT chain
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-s: source</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">; where the data is coming from
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-j: jump</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>; as in 'jump to the DROP action'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-L</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>list</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> all rules in selected chain</t>
-    </r>
-  </si>
-  <si>
-    <t>iptables -L</t>
-  </si>
-  <si>
-    <t>lists all rules on all chains</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">--policy &lt;CHAIN&gt; &lt;ACTION&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= sets the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>default</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>policy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for an iptables chain</t>
-    </r>
-  </si>
-  <si>
-    <t>iptables --policy INPUT ACCEPT</t>
-  </si>
-  <si>
-    <t>sets the default action to 'ACCEPT' for the 'INPUT' policy</t>
-  </si>
-  <si>
-    <t>OVERWRITE LOCAL REPOSITORY WITH REMOTE</t>
-  </si>
-  <si>
-    <t>git fetch --all</t>
-  </si>
-  <si>
-    <t>git reset --hard origin</t>
-  </si>
-  <si>
-    <t>fetch all remote repo differences</t>
-  </si>
-  <si>
-    <t>reset local repository with remote repo</t>
+      <t>inserts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a new rule on a specific chain at a specific location in the chain</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">iptables -I </t>
+  </si>
+  <si>
+    <t>CHAIN CONCEPT (important!)
+firewall 'chains' are made up of 'rules'
+'Rules' are evaluated sequentially in a waterfall operation; e.g. rule 1 is evaluated, then rule 2, then rule 3, then rule 4 etc.</t>
   </si>
 </sst>
 </file>
@@ -31232,84 +31431,104 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
-  <dimension ref="B3:D9"/>
+  <dimension ref="B3:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="27"/>
+    <col min="2" max="2" width="43.7109375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" s="43" t="s">
         <v>723</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="B4" s="27"/>
       <c r="C4" s="69" t="s">
+        <v>735</v>
+      </c>
+      <c r="D4" s="69"/>
+    </row>
+    <row r="5" spans="2:4" ht="90" customHeight="1">
+      <c r="C5" s="69" t="s">
+        <v>736</v>
+      </c>
+      <c r="D5" s="69"/>
+    </row>
+    <row r="6" spans="2:4" ht="90" customHeight="1">
+      <c r="C6" s="69" t="s">
+        <v>744</v>
+      </c>
+      <c r="D6" s="69"/>
+    </row>
+    <row r="8" spans="2:4" ht="75" customHeight="1">
+      <c r="B8" s="10" t="s">
         <v>724</v>
       </c>
-      <c r="D4" s="69"/>
-    </row>
-    <row r="5" spans="2:4" ht="90" customHeight="1">
-      <c r="B5" s="27"/>
-      <c r="C5" s="69" t="s">
+      <c r="C8" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="D5" s="69"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-    </row>
-    <row r="7" spans="2:4" ht="90">
-      <c r="B7" s="10" t="s">
+      <c r="D8" s="26" t="s">
         <v>726</v>
       </c>
-      <c r="C7" s="2" t="s">
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="45" t="s">
         <v>727</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="C9" s="43" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="45" t="s">
+      <c r="D9" s="21" t="s">
         <v>729</v>
       </c>
-      <c r="C8" s="43" t="s">
+    </row>
+    <row r="10" spans="2:4" ht="75">
+      <c r="B10" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="30">
-      <c r="B9" s="46" t="s">
-        <v>732</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>733</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>734</v>
+      <c r="C10" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="60">
+      <c r="B11" s="10" t="s">
+        <v>738</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="30">
+      <c r="B12" s="46" t="s">
+        <v>742</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>743</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31317,7 +31536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
   <dimension ref="B2:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -31527,23 +31746,23 @@
     </row>
     <row r="32" spans="2:4">
       <c r="B32" s="60" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="33" spans="2:3">
       <c r="B33" s="27" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="34" spans="2:3">
       <c r="B34" s="27" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>737</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added info about creating new branch in git
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC373F3-4175-4284-AD28-AAED8ABB7638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30D3501-B5FD-49C8-BE28-7E0BCED43151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="754">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -27433,6 +27433,35 @@
     <t>CHAIN CONCEPT (important!)
 firewall 'chains' are made up of 'rules'
 'Rules' are evaluated sequentially in a waterfall operation; e.g. rule 1 is evaluated, then rule 2, then rule 3, then rule 4 etc.</t>
+  </si>
+  <si>
+    <t>CREATE NEW BRANCH FOR MERGE INTO MAIN</t>
+  </si>
+  <si>
+    <t>create a new branch</t>
+  </si>
+  <si>
+    <t>git checkout -b my-new-branch</t>
+  </si>
+  <si>
+    <t>create, edit, and/or delete files, then stage and commit them</t>
+  </si>
+  <si>
+    <t>git add .
+git commit -m "my commit message"</t>
+  </si>
+  <si>
+    <t>push your new branch to GitLab</t>
+  </si>
+  <si>
+    <t>git push origin my-new-branch</t>
+  </si>
+  <si>
+    <t>GitLab will then prompt you with a direct link for creating a merge request</t>
+  </si>
+  <si>
+    <t>remote: To create a merge request for &lt;branch&gt;, visit:
+&lt;gitLab URL&gt;</t>
   </si>
 </sst>
 </file>
@@ -27599,7 +27628,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -27789,6 +27818,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -27821,6 +27856,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -28143,11 +28181,11 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -28182,7 +28220,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="29">
       <c r="A8" s="7" t="s">
         <v>63</v>
       </c>
@@ -28193,7 +28231,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="165">
+    <row r="9" spans="1:3" ht="159.5">
       <c r="A9" s="7" t="s">
         <v>66</v>
       </c>
@@ -28204,7 +28242,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="59.45" customHeight="1">
+    <row r="10" spans="1:3" ht="59.5" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>82</v>
       </c>
@@ -28215,7 +28253,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="60">
+    <row r="11" spans="1:3" ht="58">
       <c r="A11" s="8" t="s">
         <v>67</v>
       </c>
@@ -28226,7 +28264,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="60">
+    <row r="12" spans="1:3" ht="58">
       <c r="A12" s="8" t="s">
         <v>68</v>
       </c>
@@ -28248,7 +28286,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3">
       <c r="A14" s="8" t="s">
         <v>170</v>
       </c>
@@ -28259,7 +28297,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30">
+    <row r="15" spans="1:3" ht="29">
       <c r="A15" s="8" t="s">
         <v>169</v>
       </c>
@@ -28292,7 +28330,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="8" t="s">
         <v>78</v>
       </c>
@@ -28350,13 +28388,13 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="28"/>
+    <col min="1" max="1" width="30.453125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="48.81640625" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -28368,17 +28406,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="73" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="71"/>
+      <c r="C2" s="73"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="74" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -28386,12 +28424,12 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="75" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="73"/>
-    </row>
-    <row r="7" spans="1:4" ht="45">
+      <c r="B6" s="75"/>
+    </row>
+    <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="35" t="s">
         <v>345</v>
       </c>
@@ -28424,7 +28462,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="90">
+    <row r="10" spans="1:4" ht="72.5">
       <c r="A10" s="9" t="s">
         <v>351</v>
       </c>
@@ -28484,7 +28522,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="4" t="s">
         <v>355</v>
       </c>
@@ -28506,7 +28544,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75">
+    <row r="20" spans="1:3" ht="58">
       <c r="A20" s="4" t="s">
         <v>369</v>
       </c>
@@ -28518,88 +28556,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="70"/>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="70" t="s">
+      <c r="A23" s="72" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="72" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="72" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="70"/>
-      <c r="C25" s="70"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="72" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="70"/>
-      <c r="C26" s="70"/>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="70" t="s">
+      <c r="A27" s="72" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="70"/>
-      <c r="C27" s="70"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="70" t="s">
+      <c r="A28" s="72" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="70"/>
-      <c r="C28" s="70"/>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="70" t="s">
+      <c r="A29" s="72" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="71" t="s">
+      <c r="A30" s="73" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="73"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="71" t="s">
+      <c r="A31" s="73" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="70" t="s">
+      <c r="A32" s="72" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="70" t="s">
+      <c r="A33" s="72" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="70"/>
-      <c r="C33" s="70"/>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">
@@ -28724,11 +28762,11 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="4" width="55.7109375" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="4" width="55.7265625" customWidth="1"/>
+    <col min="5" max="5" width="59.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
@@ -28738,7 +28776,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="120">
+    <row r="3" spans="1:13" ht="101.5">
       <c r="A3" s="28"/>
       <c r="B3" s="3"/>
       <c r="C3" s="39" t="s">
@@ -28788,7 +28826,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="76" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -28801,8 +28839,8 @@
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="75">
-      <c r="A9" s="74"/>
+    <row r="9" spans="1:13" ht="72.5">
+      <c r="A9" s="76"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -28813,8 +28851,8 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30">
-      <c r="A10" s="74"/>
+    <row r="10" spans="1:13" ht="29">
+      <c r="A10" s="76"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -28825,8 +28863,8 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45">
-      <c r="A11" s="74"/>
+    <row r="11" spans="1:13" ht="43.5">
+      <c r="A11" s="76"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -28837,8 +28875,8 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45">
-      <c r="A12" s="74"/>
+    <row r="12" spans="1:13" ht="43.5">
+      <c r="A12" s="76"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -28854,8 +28892,8 @@
       <c r="C14" s="9"/>
       <c r="D14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="60">
-      <c r="A15" s="75" t="s">
+    <row r="15" spans="1:13" ht="43.5">
+      <c r="A15" s="77" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -28868,8 +28906,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="75">
-      <c r="A16" s="75"/>
+    <row r="16" spans="1:13" ht="72.5">
+      <c r="A16" s="77"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -28880,8 +28918,8 @@
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="105">
-      <c r="A17" s="75"/>
+    <row r="17" spans="1:13" ht="87">
+      <c r="A17" s="77"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -28892,8 +28930,8 @@
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="105">
-      <c r="A18" s="75"/>
+    <row r="18" spans="1:13" ht="87">
+      <c r="A18" s="77"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -28904,8 +28942,8 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="60">
-      <c r="A19" s="75" t="s">
+    <row r="19" spans="1:13" ht="58">
+      <c r="A19" s="77" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -28918,8 +28956,8 @@
         <v>526</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="60">
-      <c r="A20" s="75"/>
+    <row r="20" spans="1:13" ht="58">
+      <c r="A20" s="77"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -28930,8 +28968,8 @@
         <v>529</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="105">
-      <c r="A21" s="75"/>
+    <row r="21" spans="1:13" ht="101.5">
+      <c r="A21" s="77"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -28942,8 +28980,8 @@
         <v>541</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="60">
-      <c r="A22" s="75"/>
+    <row r="22" spans="1:13" ht="58">
+      <c r="A22" s="77"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -28976,7 +29014,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:13" ht="150">
+    <row r="25" spans="1:13" ht="130.5">
       <c r="B25" s="11" t="s">
         <v>538</v>
       </c>
@@ -28998,7 +29036,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" ht="150">
+    <row r="26" spans="1:13" ht="145">
       <c r="A26" s="28"/>
       <c r="B26" s="11" t="s">
         <v>629</v>
@@ -29021,7 +29059,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" ht="165">
+    <row r="27" spans="1:13" ht="145">
       <c r="B27" s="11" t="s">
         <v>632</v>
       </c>
@@ -29041,7 +29079,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" ht="200.1" customHeight="1">
+    <row r="28" spans="1:13" ht="200.15" customHeight="1">
       <c r="B28" s="11" t="s">
         <v>635</v>
       </c>
@@ -29077,7 +29115,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="210.95" customHeight="1">
+    <row r="30" spans="1:13" ht="211" customHeight="1">
       <c r="B30" s="11" t="s">
         <v>643</v>
       </c>
@@ -29091,7 +29129,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="270">
+    <row r="31" spans="1:13" ht="232">
       <c r="B31" s="11" t="s">
         <v>647</v>
       </c>
@@ -29105,7 +29143,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="75">
+    <row r="32" spans="1:13" ht="72.5">
       <c r="B32" s="11" t="s">
         <v>651</v>
       </c>
@@ -29134,10 +29172,10 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="4" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.7265625" customWidth="1"/>
+    <col min="3" max="4" width="53.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
@@ -29292,38 +29330,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="76" t="s">
+      <c r="C19" s="78" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="76"/>
+      <c r="D19" s="78"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="76" t="s">
+      <c r="C20" s="78" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="76"/>
+      <c r="D20" s="78"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="76" t="s">
+      <c r="C21" s="78" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="76"/>
+      <c r="D21" s="78"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="76" t="s">
+      <c r="C22" s="78" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="76"/>
+      <c r="D22" s="78"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="76" t="s">
+      <c r="C23" s="78" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="76"/>
+      <c r="D23" s="78"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -29336,40 +29374,40 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="76" t="s">
+      <c r="C25" s="78" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="76"/>
+      <c r="D25" s="78"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="76" t="s">
+      <c r="C26" s="78" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="76"/>
+      <c r="D26" s="78"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="76" t="s">
+      <c r="C27" s="78" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="76"/>
+      <c r="D27" s="78"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="76" t="s">
+      <c r="C28" s="78" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="76"/>
+      <c r="D28" s="78"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="76" t="s">
+      <c r="C29" s="78" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="76"/>
-    </row>
-    <row r="30" spans="2:4" ht="38.25">
+      <c r="D29" s="78"/>
+    </row>
+    <row r="30" spans="2:4" ht="39">
       <c r="B30" s="27" t="s">
         <v>701</v>
       </c>
@@ -29412,16 +29450,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="27"/>
-    <col min="2" max="2" width="43.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="27" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="42.42578125" style="27" customWidth="1"/>
-    <col min="7" max="8" width="40.5703125" style="27" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="8.81640625" style="27"/>
+    <col min="2" max="2" width="43.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="27" customWidth="1"/>
+    <col min="5" max="5" width="34.453125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" style="27" customWidth="1"/>
+    <col min="7" max="8" width="40.54296875" style="27" customWidth="1"/>
+    <col min="9" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -29434,7 +29472,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="29.45" customHeight="1">
+    <row r="5" spans="2:8" ht="29.5" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>466</v>
       </c>
@@ -29458,7 +29496,7 @@
       </c>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="2:8" ht="29.1" customHeight="1">
+    <row r="7" spans="2:8" ht="29.15" customHeight="1">
       <c r="C7" s="27" t="s">
         <v>465</v>
       </c>
@@ -29467,7 +29505,7 @@
       </c>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="2:8" ht="45">
+    <row r="8" spans="2:8" ht="43.5">
       <c r="C8" s="27" t="s">
         <v>467</v>
       </c>
@@ -29484,7 +29522,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="2:8" ht="30">
+    <row r="11" spans="2:8" ht="29">
       <c r="B11" s="10" t="s">
         <v>477</v>
       </c>
@@ -29496,7 +29534,7 @@
       </c>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="2:8" ht="115.35" customHeight="1">
+    <row r="12" spans="2:8" ht="115.4" customHeight="1">
       <c r="B12" s="10" t="s">
         <v>472</v>
       </c>
@@ -29508,7 +29546,7 @@
       </c>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="2:8" ht="45">
+    <row r="13" spans="2:8" ht="43.5">
       <c r="B13" s="46" t="s">
         <v>459</v>
       </c>
@@ -29520,7 +29558,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="2:8" ht="30">
+    <row r="14" spans="2:8" ht="29">
       <c r="B14" s="46" t="s">
         <v>478</v>
       </c>
@@ -29532,7 +29570,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="2:8" ht="101.1" customHeight="1">
+    <row r="15" spans="2:8" ht="101.15" customHeight="1">
       <c r="B15" s="8" t="s">
         <v>481</v>
       </c>
@@ -29544,7 +29582,7 @@
       </c>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="2:8" ht="75">
+    <row r="16" spans="2:8" ht="72.5">
       <c r="B16" s="8" t="s">
         <v>495</v>
       </c>
@@ -29567,7 +29605,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="90">
+    <row r="17" spans="2:8" ht="58">
       <c r="B17" s="8" t="s">
         <v>494</v>
       </c>
@@ -29582,7 +29620,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="2:8" ht="45">
+    <row r="18" spans="2:8" ht="43.5">
       <c r="B18" s="8" t="s">
         <v>491</v>
       </c>
@@ -29597,7 +29635,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="2:8" ht="75">
+    <row r="19" spans="2:8" ht="72.5">
       <c r="B19" s="8" t="s">
         <v>496</v>
       </c>
@@ -29612,7 +29650,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="2:8" ht="120">
+    <row r="20" spans="2:8" ht="116">
       <c r="B20" s="8" t="s">
         <v>501</v>
       </c>
@@ -29629,7 +29667,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="2:8" ht="43.35" customHeight="1">
+    <row r="21" spans="2:8" ht="43.4" customHeight="1">
       <c r="B21" s="8" t="s">
         <v>504</v>
       </c>
@@ -29644,7 +29682,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="2:8" ht="90">
+    <row r="22" spans="2:8" ht="87">
       <c r="B22" s="8" t="s">
         <v>510</v>
       </c>
@@ -29659,7 +29697,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="2:8" ht="30">
+    <row r="23" spans="2:8">
       <c r="B23" s="8" t="s">
         <v>543</v>
       </c>
@@ -29688,7 +29726,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="2:8" ht="30">
+    <row r="26" spans="2:8" ht="29">
       <c r="B26" s="10" t="s">
         <v>505</v>
       </c>
@@ -29724,7 +29762,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="2:8" ht="30">
+    <row r="30" spans="2:8" ht="29">
       <c r="B30" s="46" t="s">
         <v>509</v>
       </c>
@@ -29735,7 +29773,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="14.45" customHeight="1"/>
+    <row r="32" spans="2:8" ht="14.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4294967295" r:id="rId1"/>
@@ -29750,18 +29788,18 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="79" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -29769,11 +29807,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="70" t="s">
+      <c r="B5" s="72" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -29791,19 +29829,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="79" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="77"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="79" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="77"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -29827,12 +29865,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="16.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -29840,13 +29878,13 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3">
       <c r="B4" s="39" t="s">
         <v>419</v>
       </c>
       <c r="C4" s="38"/>
     </row>
-    <row r="6" spans="1:3" ht="90">
+    <row r="6" spans="1:3" ht="87">
       <c r="A6" s="44" t="s">
         <v>420</v>
       </c>
@@ -29871,12 +29909,12 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -29889,7 +29927,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>430</v>
       </c>
@@ -29924,12 +29962,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -29942,7 +29980,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>438</v>
       </c>
@@ -29953,7 +29991,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="46" t="s">
         <v>441</v>
       </c>
@@ -29977,12 +30015,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="38" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="38" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="38" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="38"/>
+    <col min="1" max="1" width="23.54296875" style="38" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="38" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="38"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -29990,12 +30028,12 @@
         <v>444</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="29">
       <c r="B4" s="39" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>446</v>
       </c>
@@ -30006,7 +30044,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="46" t="s">
         <v>448</v>
       </c>
@@ -30030,12 +30068,12 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="43.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -30043,12 +30081,12 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45">
+    <row r="4" spans="1:3" ht="43.5">
       <c r="B4" s="39" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>426</v>
       </c>
@@ -30072,12 +30110,12 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.453125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="63.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -30086,7 +30124,7 @@
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="43.5">
       <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
@@ -30107,7 +30145,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45">
+    <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -30119,7 +30157,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="43.5">
       <c r="A8" s="7" t="s">
         <v>87</v>
       </c>
@@ -30131,7 +30169,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="90">
+    <row r="9" spans="1:4" ht="72.5">
       <c r="A9" s="8" t="s">
         <v>269</v>
       </c>
@@ -30143,7 +30181,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="43.5">
       <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
@@ -30155,7 +30193,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="75">
+    <row r="11" spans="1:4" ht="58">
       <c r="A11" s="8" t="s">
         <v>264</v>
       </c>
@@ -30167,7 +30205,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" s="12" customFormat="1" ht="45">
+    <row r="12" spans="1:4" s="12" customFormat="1" ht="43.5">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -30179,7 +30217,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" s="12" customFormat="1" ht="45">
+    <row r="13" spans="1:4" s="12" customFormat="1" ht="43.5">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -30191,7 +30229,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="45">
+    <row r="14" spans="1:4" ht="43.5">
       <c r="A14" s="8" t="s">
         <v>275</v>
       </c>
@@ -30203,7 +30241,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" ht="45">
+    <row r="15" spans="1:4" s="3" customFormat="1" ht="43.5">
       <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
@@ -30215,7 +30253,7 @@
       </c>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" ht="45">
+    <row r="16" spans="1:4" ht="43.5">
       <c r="A16" s="8" t="s">
         <v>218</v>
       </c>
@@ -30227,7 +30265,7 @@
       </c>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="60">
+    <row r="17" spans="1:4" ht="43.5">
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
@@ -30239,7 +30277,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="60">
+    <row r="18" spans="1:4" ht="43.5">
       <c r="A18" s="7" t="s">
         <v>21</v>
       </c>
@@ -30251,7 +30289,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="75">
+    <row r="19" spans="1:4" ht="72.5">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -30263,7 +30301,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="90">
+    <row r="20" spans="1:4" ht="87">
       <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
@@ -30275,7 +30313,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" ht="60">
+    <row r="21" spans="1:4" ht="58">
       <c r="A21" s="30" t="s">
         <v>224</v>
       </c>
@@ -30287,7 +30325,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="29">
       <c r="A22" s="12" t="s">
         <v>22</v>
       </c>
@@ -30299,7 +30337,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" ht="30">
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="29">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -30321,7 +30359,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="75">
+    <row r="25" spans="1:4" ht="72.5">
       <c r="A25" s="8" t="s">
         <v>227</v>
       </c>
@@ -30333,7 +30371,7 @@
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" ht="120">
+    <row r="26" spans="1:4" ht="87">
       <c r="A26" s="6" t="s">
         <v>229</v>
       </c>
@@ -30345,7 +30383,7 @@
       </c>
       <c r="D26" s="12"/>
     </row>
-    <row r="27" spans="1:4" ht="60">
+    <row r="27" spans="1:4" ht="58">
       <c r="A27" s="6" t="s">
         <v>231</v>
       </c>
@@ -30393,11 +30431,11 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.54296875" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
@@ -30419,7 +30457,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="45">
+    <row r="5" spans="1:6" ht="43.5">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -30430,7 +30468,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
+    <row r="6" spans="1:6" ht="43.5">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -30441,7 +30479,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60">
+    <row r="7" spans="1:6" ht="58">
       <c r="A7" s="6" t="s">
         <v>104</v>
       </c>
@@ -30452,7 +30490,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="43.5">
       <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
@@ -30466,7 +30504,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="195">
+    <row r="9" spans="1:6" ht="174">
       <c r="A9" s="8" t="s">
         <v>119</v>
       </c>
@@ -30477,7 +30515,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45">
+    <row r="10" spans="1:6" ht="43.5">
       <c r="A10" s="8" t="s">
         <v>90</v>
       </c>
@@ -30488,7 +30526,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="75">
+    <row r="11" spans="1:6" ht="72.5">
       <c r="A11" s="8" t="s">
         <v>92</v>
       </c>
@@ -30499,7 +30537,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60">
+    <row r="12" spans="1:6" ht="58">
       <c r="A12" s="8" t="s">
         <v>93</v>
       </c>
@@ -30510,7 +30548,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="75">
+    <row r="13" spans="1:6" ht="72.5">
       <c r="A13" s="8" t="s">
         <v>97</v>
       </c>
@@ -30521,7 +30559,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="90">
+    <row r="14" spans="1:6" ht="72.5">
       <c r="A14" s="8" t="s">
         <v>98</v>
       </c>
@@ -30532,7 +30570,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60">
+    <row r="15" spans="1:6" ht="58">
       <c r="A15" s="8" t="s">
         <v>99</v>
       </c>
@@ -30543,7 +30581,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="90">
+    <row r="16" spans="1:6" ht="87">
       <c r="A16" s="8" t="s">
         <v>103</v>
       </c>
@@ -30554,7 +30592,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="75">
+    <row r="17" spans="1:3" ht="72.5">
       <c r="A17" s="8" t="s">
         <v>101</v>
       </c>
@@ -30565,7 +30603,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="105">
+    <row r="18" spans="1:3" ht="87">
       <c r="A18" s="8" t="s">
         <v>196</v>
       </c>
@@ -30576,7 +30614,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90">
+    <row r="19" spans="1:3" ht="87">
       <c r="A19" s="8" t="s">
         <v>102</v>
       </c>
@@ -30587,7 +30625,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="60">
+    <row r="20" spans="1:3" ht="43.5">
       <c r="A20" s="8" t="s">
         <v>203</v>
       </c>
@@ -30598,7 +30636,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="90">
+    <row r="21" spans="1:3" ht="87">
       <c r="A21" s="8" t="s">
         <v>106</v>
       </c>
@@ -30609,7 +30647,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="8" t="s">
         <v>108</v>
       </c>
@@ -30620,7 +30658,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="90">
+    <row r="23" spans="1:3" ht="87">
       <c r="A23" s="8" t="s">
         <v>109</v>
       </c>
@@ -30631,7 +30669,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="105">
+    <row r="24" spans="1:3" ht="87">
       <c r="A24" s="8" t="s">
         <v>110</v>
       </c>
@@ -30653,7 +30691,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="90">
+    <row r="26" spans="1:3" ht="72.5">
       <c r="A26" s="8" t="s">
         <v>111</v>
       </c>
@@ -30664,7 +30702,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="90">
+    <row r="27" spans="1:3" ht="87">
       <c r="A27" s="8" t="s">
         <v>113</v>
       </c>
@@ -30675,7 +30713,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="75">
+    <row r="28" spans="1:3" ht="72.5">
       <c r="A28" s="8" t="s">
         <v>114</v>
       </c>
@@ -30686,7 +30724,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="120">
+    <row r="29" spans="1:3" ht="116">
       <c r="A29" s="8" t="s">
         <v>115</v>
       </c>
@@ -30697,7 +30735,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="195">
+    <row r="30" spans="1:3" ht="174">
       <c r="A30" s="6" t="s">
         <v>116</v>
       </c>
@@ -30708,7 +30746,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="210">
+    <row r="31" spans="1:3" ht="159.5">
       <c r="A31" s="6" t="s">
         <v>117</v>
       </c>
@@ -30719,7 +30757,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="240">
+    <row r="32" spans="1:3" ht="203">
       <c r="A32" s="9" t="s">
         <v>60</v>
       </c>
@@ -30755,11 +30793,11 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -30784,7 +30822,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="27"/>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="29">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -30795,7 +30833,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60">
+    <row r="6" spans="1:3" ht="43.5">
       <c r="A6" s="3" t="s">
         <v>135</v>
       </c>
@@ -30806,7 +30844,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="10" t="s">
         <v>136</v>
       </c>
@@ -30817,7 +30855,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="29">
       <c r="A8" s="10" t="s">
         <v>139</v>
       </c>
@@ -30828,7 +30866,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45">
+    <row r="9" spans="1:3" ht="43.5">
       <c r="A9" s="10" t="s">
         <v>140</v>
       </c>
@@ -30839,7 +30877,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45">
+    <row r="10" spans="1:3" ht="43.5">
       <c r="A10" s="10" t="s">
         <v>142</v>
       </c>
@@ -30861,7 +30899,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="43.5">
       <c r="A12" s="10" t="s">
         <v>152</v>
       </c>
@@ -30872,7 +30910,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45">
+    <row r="13" spans="1:3" ht="43.5">
       <c r="A13" s="8" t="s">
         <v>156</v>
       </c>
@@ -30883,7 +30921,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="43.5">
       <c r="A14" s="8" t="s">
         <v>161</v>
       </c>
@@ -30894,7 +30932,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="75">
+    <row r="15" spans="1:3" ht="72.5">
       <c r="A15" s="8" t="s">
         <v>166</v>
       </c>
@@ -30905,7 +30943,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45">
+    <row r="16" spans="1:3" ht="43.5">
       <c r="A16" s="8" t="s">
         <v>175</v>
       </c>
@@ -30916,7 +30954,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="43.5">
       <c r="A17" s="8" t="s">
         <v>177</v>
       </c>
@@ -30927,7 +30965,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45">
+    <row r="18" spans="1:3" ht="43.5">
       <c r="A18" s="8" t="s">
         <v>178</v>
       </c>
@@ -30938,7 +30976,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45">
+    <row r="19" spans="1:3" ht="43.5">
       <c r="A19" s="8" t="s">
         <v>181</v>
       </c>
@@ -30949,7 +30987,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="60">
+    <row r="20" spans="1:3" ht="58">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
@@ -30960,7 +30998,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="90">
+    <row r="21" spans="1:3" ht="72.5">
       <c r="A21" s="10" t="s">
         <v>150</v>
       </c>
@@ -30971,7 +31009,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="8" t="s">
         <v>183</v>
       </c>
@@ -30982,7 +31020,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60">
+    <row r="23" spans="1:3" ht="58">
       <c r="A23" s="10" t="s">
         <v>67</v>
       </c>
@@ -30993,7 +31031,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="90">
+    <row r="24" spans="1:3" ht="87">
       <c r="A24" s="8" t="s">
         <v>186</v>
       </c>
@@ -31004,7 +31042,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="120">
+    <row r="25" spans="1:3" ht="101.5">
       <c r="A25" s="10" t="s">
         <v>232</v>
       </c>
@@ -31015,7 +31053,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="90">
+    <row r="26" spans="1:3" ht="72.5">
       <c r="A26" s="8" t="s">
         <v>234</v>
       </c>
@@ -31026,7 +31064,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="75">
+    <row r="27" spans="1:3" ht="72.5">
       <c r="A27" s="10" t="s">
         <v>236</v>
       </c>
@@ -31037,7 +31075,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="45">
+    <row r="28" spans="1:3" ht="43.5">
       <c r="A28" s="7" t="s">
         <v>240</v>
       </c>
@@ -31048,7 +31086,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="75">
+    <row r="29" spans="1:3" ht="58">
       <c r="A29" s="7" t="s">
         <v>242</v>
       </c>
@@ -31059,7 +31097,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="45.6" customHeight="1">
+    <row r="30" spans="1:3" ht="45.65" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>245</v>
       </c>
@@ -31070,7 +31108,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="45">
+    <row r="31" spans="1:3" ht="43.5">
       <c r="A31" s="7" t="s">
         <v>247</v>
       </c>
@@ -31081,7 +31119,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="45">
+    <row r="32" spans="1:3" ht="43.5">
       <c r="A32" s="7" t="s">
         <v>251</v>
       </c>
@@ -31092,7 +31130,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="45">
+    <row r="33" spans="1:3" ht="43.5">
       <c r="A33" s="8" t="s">
         <v>148</v>
       </c>
@@ -31103,7 +31141,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="60">
+    <row r="34" spans="1:3" ht="58">
       <c r="A34" s="8" t="s">
         <v>148</v>
       </c>
@@ -31196,13 +31234,13 @@
       <selection activeCell="E18" sqref="E18:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="28"/>
-    <col min="2" max="2" width="30.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="28"/>
+    <col min="1" max="1" width="8.81640625" style="28"/>
+    <col min="2" max="2" width="30.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -31210,7 +31248,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="60">
+    <row r="3" spans="2:4" ht="58">
       <c r="C3" s="37" t="s">
         <v>545</v>
       </c>
@@ -31234,7 +31272,7 @@
       <c r="B7" s="59"/>
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="2:4" ht="30">
+    <row r="8" spans="2:4" ht="29">
       <c r="B8" s="11" t="s">
         <v>560</v>
       </c>
@@ -31245,7 +31283,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30">
+    <row r="9" spans="2:4" ht="29">
       <c r="B9" s="7" t="s">
         <v>553</v>
       </c>
@@ -31256,7 +31294,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30">
+    <row r="10" spans="2:4" ht="29">
       <c r="B10" s="7" t="s">
         <v>556</v>
       </c>
@@ -31267,7 +31305,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="30">
+    <row r="11" spans="2:4" ht="29">
       <c r="B11" s="11" t="s">
         <v>559</v>
       </c>
@@ -31278,7 +31316,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="30">
+    <row r="12" spans="2:4" ht="29">
       <c r="B12" s="11" t="s">
         <v>563</v>
       </c>
@@ -31289,7 +31327,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="45">
+    <row r="13" spans="2:4" ht="43.5">
       <c r="B13" s="11" t="s">
         <v>565</v>
       </c>
@@ -31300,7 +31338,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="45">
+    <row r="14" spans="2:4" ht="43.5">
       <c r="B14" s="11" t="s">
         <v>569</v>
       </c>
@@ -31311,7 +31349,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="45">
+    <row r="15" spans="2:4" ht="43.5">
       <c r="B15" s="11" t="s">
         <v>571</v>
       </c>
@@ -31322,7 +31360,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="30">
+    <row r="16" spans="2:4" ht="29">
       <c r="B16" s="7" t="s">
         <v>574</v>
       </c>
@@ -31333,7 +31371,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="165">
+    <row r="17" spans="2:13" ht="159.5">
       <c r="B17" s="7" t="s">
         <v>578</v>
       </c>
@@ -31344,7 +31382,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="144.94999999999999" customHeight="1">
+    <row r="18" spans="2:13" ht="145" customHeight="1">
       <c r="B18" s="11" t="s">
         <v>581</v>
       </c>
@@ -31354,14 +31392,14 @@
       <c r="D18" s="66" t="s">
         <v>583</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="69" t="s">
         <v>584</v>
       </c>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -31373,19 +31411,19 @@
       <c r="D19" s="66" t="s">
         <v>587</v>
       </c>
-      <c r="E19" s="67" t="s">
+      <c r="E19" s="69" t="s">
         <v>588</v>
       </c>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
-    </row>
-    <row r="20" spans="2:13" ht="30">
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+    </row>
+    <row r="20" spans="2:13" ht="29">
       <c r="B20" s="7" t="s">
         <v>589</v>
       </c>
@@ -31406,17 +31444,17 @@
       <c r="D21" s="66" t="s">
         <v>721</v>
       </c>
-      <c r="E21" s="67" t="s">
+      <c r="E21" s="69" t="s">
         <v>722</v>
       </c>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="67"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -31433,17 +31471,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
   <dimension ref="B3:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="27"/>
-    <col min="2" max="2" width="43.7109375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="1" width="9.1796875" style="27"/>
+    <col min="2" max="2" width="43.7265625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="46.7265625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.7265625" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
@@ -31452,22 +31490,22 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="71" t="s">
         <v>735</v>
       </c>
-      <c r="D4" s="69"/>
+      <c r="D4" s="71"/>
     </row>
     <row r="5" spans="2:4" ht="90" customHeight="1">
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="71" t="s">
         <v>736</v>
       </c>
-      <c r="D5" s="69"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="71" t="s">
         <v>744</v>
       </c>
-      <c r="D6" s="69"/>
+      <c r="D6" s="71"/>
     </row>
     <row r="8" spans="2:4" ht="75" customHeight="1">
       <c r="B8" s="10" t="s">
@@ -31491,7 +31529,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="75">
+    <row r="10" spans="2:4" ht="72.5">
       <c r="B10" s="8" t="s">
         <v>730</v>
       </c>
@@ -31502,7 +31540,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="60">
+    <row r="11" spans="2:4" ht="58">
       <c r="B11" s="10" t="s">
         <v>738</v>
       </c>
@@ -31513,7 +31551,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="30">
+    <row r="12" spans="2:4" ht="29">
       <c r="B12" s="46" t="s">
         <v>742</v>
       </c>
@@ -31534,18 +31572,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D34"/>
+  <dimension ref="B2:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="27"/>
-    <col min="2" max="3" width="43.5703125" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="27"/>
+    <col min="1" max="1" width="8.7265625" style="27"/>
+    <col min="2" max="3" width="43.54296875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -31711,7 +31749,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="30">
+    <row r="26" spans="2:4" ht="29">
       <c r="B26" s="38" t="s">
         <v>714</v>
       </c>
@@ -31749,7 +31787,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:4">
       <c r="B33" s="27" t="s">
         <v>733</v>
       </c>
@@ -31757,7 +31795,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:4">
       <c r="B34" s="27" t="s">
         <v>734</v>
       </c>
@@ -31765,7 +31803,48 @@
         <v>105</v>
       </c>
     </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="60" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="27" t="s">
+        <v>746</v>
+      </c>
+      <c r="C39" s="43" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="29">
+      <c r="B40" s="68" t="s">
+        <v>748</v>
+      </c>
+      <c r="C40" s="67" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="27" t="s">
+        <v>750</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="29">
+      <c r="B42" s="68" t="s">
+        <v>752</v>
+      </c>
+      <c r="C42" s="71" t="s">
+        <v>753</v>
+      </c>
+      <c r="D42" s="80"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C42:D42"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
@@ -31779,13 +31858,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="27"/>
-    <col min="2" max="2" width="30.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="8.81640625" style="27"/>
+    <col min="2" max="2" width="30.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -31813,7 +31892,7 @@
       <c r="B6" s="45"/>
       <c r="C6" s="43"/>
     </row>
-    <row r="7" spans="2:4" ht="30">
+    <row r="7" spans="2:4" ht="29">
       <c r="B7" s="46" t="s">
         <v>550</v>
       </c>
@@ -31825,7 +31904,7 @@
     <row r="9" spans="2:4">
       <c r="B9" s="45"/>
     </row>
-    <row r="10" spans="2:4" ht="101.45" customHeight="1">
+    <row r="10" spans="2:4" ht="101.5" customHeight="1">
       <c r="B10" s="45"/>
       <c r="C10" s="43"/>
       <c r="D10" s="38"/>
@@ -31847,10 +31926,10 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -31889,7 +31968,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="101.45" customHeight="1">
+    <row r="9" spans="1:3" ht="101.5" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>295</v>
       </c>

</xml_diff>

<commit_message>
Cleaning up 'git' tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30D3501-B5FD-49C8-BE28-7E0BCED43151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90394E2C-224C-41D5-8851-539F7C4B9662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="758">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -27017,16 +27017,7 @@
     </r>
   </si>
   <si>
-    <t>OVERWRITE LOCAL REPOSITORY WITH REMOTE</t>
-  </si>
-  <si>
-    <t>git fetch --all</t>
-  </si>
-  <si>
     <t>fetch all remote repo differences</t>
-  </si>
-  <si>
-    <t>reset local repository with remote repo</t>
   </si>
   <si>
     <r>
@@ -27462,6 +27453,27 @@
   <si>
     <t>remote: To create a merge request for &lt;branch&gt;, visit:
 &lt;gitLab URL&gt;</t>
+  </si>
+  <si>
+    <t>git config -h</t>
+  </si>
+  <si>
+    <t>show help for git config</t>
+  </si>
+  <si>
+    <t>displays some helpful tips for the 'git config' command</t>
+  </si>
+  <si>
+    <t>UPDATE REMOTE REPOSITORY WITH LOCAL CHANGES</t>
+  </si>
+  <si>
+    <t>git pull origin main</t>
+  </si>
+  <si>
+    <t>OVERWRITE LOCAL REPO WITH REMOTE REPO</t>
+  </si>
+  <si>
+    <t>CREATE NEW LOCAL REPO FROM REMOTE REPO</t>
   </si>
 </sst>
 </file>
@@ -27628,7 +27640,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -27825,6 +27837,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -27832,6 +27853,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -27857,7 +27881,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -28181,11 +28205,11 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -28220,7 +28244,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="29">
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="7" t="s">
         <v>63</v>
       </c>
@@ -28231,7 +28255,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="159.5">
+    <row r="9" spans="1:3" ht="165">
       <c r="A9" s="7" t="s">
         <v>66</v>
       </c>
@@ -28242,7 +28266,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="59.5" customHeight="1">
+    <row r="10" spans="1:3" ht="59.45" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>82</v>
       </c>
@@ -28253,7 +28277,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="58">
+    <row r="11" spans="1:3" ht="60">
       <c r="A11" s="8" t="s">
         <v>67</v>
       </c>
@@ -28264,7 +28288,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="58">
+    <row r="12" spans="1:3" ht="60">
       <c r="A12" s="8" t="s">
         <v>68</v>
       </c>
@@ -28286,7 +28310,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" ht="30">
       <c r="A14" s="8" t="s">
         <v>170</v>
       </c>
@@ -28297,7 +28321,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29">
+    <row r="15" spans="1:3" ht="30">
       <c r="A15" s="8" t="s">
         <v>169</v>
       </c>
@@ -28330,7 +28354,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29">
+    <row r="18" spans="1:3" ht="30">
       <c r="A18" s="8" t="s">
         <v>78</v>
       </c>
@@ -28388,13 +28412,13 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.453125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="48.81640625" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="28"/>
+    <col min="1" max="1" width="30.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -28406,17 +28430,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="77" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="73"/>
+      <c r="C2" s="77"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="78" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -28424,12 +28448,12 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="79" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="75"/>
-    </row>
-    <row r="7" spans="1:4" ht="43.5">
+      <c r="B6" s="79"/>
+    </row>
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="35" t="s">
         <v>345</v>
       </c>
@@ -28462,7 +28486,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="72.5">
+    <row r="10" spans="1:4" ht="90">
       <c r="A10" s="9" t="s">
         <v>351</v>
       </c>
@@ -28522,7 +28546,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29">
+    <row r="18" spans="1:3" ht="30">
       <c r="A18" s="4" t="s">
         <v>355</v>
       </c>
@@ -28544,7 +28568,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="58">
+    <row r="20" spans="1:3" ht="75">
       <c r="A20" s="4" t="s">
         <v>369</v>
       </c>
@@ -28556,88 +28580,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="76" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="76" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
+      <c r="B23" s="76"/>
+      <c r="C23" s="76"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="76" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
+      <c r="B24" s="76"/>
+      <c r="C24" s="76"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="76" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="76"/>
+      <c r="C25" s="76"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="76" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="76" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="72" t="s">
+      <c r="A28" s="76" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="76"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="72" t="s">
+      <c r="A29" s="76" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="B29" s="76"/>
+      <c r="C29" s="76"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="77" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="73"/>
-      <c r="C30" s="73"/>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="73" t="s">
+      <c r="A31" s="77" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="72" t="s">
+      <c r="A32" s="76" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="76"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="76" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">
@@ -28762,11 +28786,11 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.7265625" customWidth="1"/>
-    <col min="3" max="4" width="55.7265625" customWidth="1"/>
-    <col min="5" max="5" width="59.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="55.7109375" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
@@ -28776,7 +28800,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="101.5">
+    <row r="3" spans="1:13" ht="120">
       <c r="A3" s="28"/>
       <c r="B3" s="3"/>
       <c r="C3" s="39" t="s">
@@ -28826,7 +28850,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="80" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -28839,8 +28863,8 @@
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="72.5">
-      <c r="A9" s="76"/>
+    <row r="9" spans="1:13" ht="75">
+      <c r="A9" s="80"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -28851,8 +28875,8 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="29">
-      <c r="A10" s="76"/>
+    <row r="10" spans="1:13" ht="30">
+      <c r="A10" s="80"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -28863,8 +28887,8 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="43.5">
-      <c r="A11" s="76"/>
+    <row r="11" spans="1:13" ht="45">
+      <c r="A11" s="80"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -28875,8 +28899,8 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="43.5">
-      <c r="A12" s="76"/>
+    <row r="12" spans="1:13" ht="45">
+      <c r="A12" s="80"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -28892,8 +28916,8 @@
       <c r="C14" s="9"/>
       <c r="D14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="43.5">
-      <c r="A15" s="77" t="s">
+    <row r="15" spans="1:13" ht="60">
+      <c r="A15" s="81" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -28906,8 +28930,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="72.5">
-      <c r="A16" s="77"/>
+    <row r="16" spans="1:13" ht="75">
+      <c r="A16" s="81"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -28918,8 +28942,8 @@
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="87">
-      <c r="A17" s="77"/>
+    <row r="17" spans="1:13" ht="105">
+      <c r="A17" s="81"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -28930,8 +28954,8 @@
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="87">
-      <c r="A18" s="77"/>
+    <row r="18" spans="1:13" ht="105">
+      <c r="A18" s="81"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -28942,8 +28966,8 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="58">
-      <c r="A19" s="77" t="s">
+    <row r="19" spans="1:13" ht="60">
+      <c r="A19" s="81" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -28956,8 +28980,8 @@
         <v>526</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="58">
-      <c r="A20" s="77"/>
+    <row r="20" spans="1:13" ht="60">
+      <c r="A20" s="81"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -28968,8 +28992,8 @@
         <v>529</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="101.5">
-      <c r="A21" s="77"/>
+    <row r="21" spans="1:13" ht="105">
+      <c r="A21" s="81"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -28980,8 +29004,8 @@
         <v>541</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="58">
-      <c r="A22" s="77"/>
+    <row r="22" spans="1:13" ht="60">
+      <c r="A22" s="81"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -29014,7 +29038,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:13" ht="130.5">
+    <row r="25" spans="1:13" ht="150">
       <c r="B25" s="11" t="s">
         <v>538</v>
       </c>
@@ -29036,7 +29060,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" ht="145">
+    <row r="26" spans="1:13" ht="150">
       <c r="A26" s="28"/>
       <c r="B26" s="11" t="s">
         <v>629</v>
@@ -29059,7 +29083,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" ht="145">
+    <row r="27" spans="1:13" ht="165">
       <c r="B27" s="11" t="s">
         <v>632</v>
       </c>
@@ -29079,7 +29103,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" ht="200.15" customHeight="1">
+    <row r="28" spans="1:13" ht="200.1" customHeight="1">
       <c r="B28" s="11" t="s">
         <v>635</v>
       </c>
@@ -29115,7 +29139,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="211" customHeight="1">
+    <row r="30" spans="1:13" ht="210.95" customHeight="1">
       <c r="B30" s="11" t="s">
         <v>643</v>
       </c>
@@ -29129,7 +29153,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="232">
+    <row r="31" spans="1:13" ht="270">
       <c r="B31" s="11" t="s">
         <v>647</v>
       </c>
@@ -29143,7 +29167,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="72.5">
+    <row r="32" spans="1:13" ht="75">
       <c r="B32" s="11" t="s">
         <v>651</v>
       </c>
@@ -29172,10 +29196,10 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.7265625" customWidth="1"/>
-    <col min="3" max="4" width="53.7265625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="4" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
@@ -29330,38 +29354,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="78" t="s">
+      <c r="C19" s="82" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="78"/>
+      <c r="D19" s="82"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="82" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="78"/>
+      <c r="D20" s="82"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="78" t="s">
+      <c r="C21" s="82" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="78"/>
+      <c r="D21" s="82"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="82" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="78"/>
+      <c r="D22" s="82"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="78" t="s">
+      <c r="C23" s="82" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="78"/>
+      <c r="D23" s="82"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -29374,40 +29398,40 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="78" t="s">
+      <c r="C25" s="82" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="78"/>
+      <c r="D25" s="82"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="78" t="s">
+      <c r="C26" s="82" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="78"/>
+      <c r="D26" s="82"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="82" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="78"/>
+      <c r="D27" s="82"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="78" t="s">
+      <c r="C28" s="82" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="78"/>
+      <c r="D28" s="82"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="78" t="s">
+      <c r="C29" s="82" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="78"/>
-    </row>
-    <row r="30" spans="2:4" ht="39">
+      <c r="D29" s="82"/>
+    </row>
+    <row r="30" spans="2:4" ht="38.25">
       <c r="B30" s="27" t="s">
         <v>701</v>
       </c>
@@ -29450,16 +29474,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="27"/>
-    <col min="2" max="2" width="43.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.54296875" style="27" customWidth="1"/>
-    <col min="5" max="5" width="34.453125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="42.453125" style="27" customWidth="1"/>
-    <col min="7" max="8" width="40.54296875" style="27" customWidth="1"/>
-    <col min="9" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="8.85546875" style="27"/>
+    <col min="2" max="2" width="43.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="27" customWidth="1"/>
+    <col min="7" max="8" width="40.5703125" style="27" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -29472,7 +29496,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="29.5" customHeight="1">
+    <row r="5" spans="2:8" ht="29.45" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>466</v>
       </c>
@@ -29496,7 +29520,7 @@
       </c>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="2:8" ht="29.15" customHeight="1">
+    <row r="7" spans="2:8" ht="29.1" customHeight="1">
       <c r="C7" s="27" t="s">
         <v>465</v>
       </c>
@@ -29505,7 +29529,7 @@
       </c>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="2:8" ht="43.5">
+    <row r="8" spans="2:8" ht="45">
       <c r="C8" s="27" t="s">
         <v>467</v>
       </c>
@@ -29522,7 +29546,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="2:8" ht="29">
+    <row r="11" spans="2:8" ht="30">
       <c r="B11" s="10" t="s">
         <v>477</v>
       </c>
@@ -29534,7 +29558,7 @@
       </c>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="2:8" ht="115.4" customHeight="1">
+    <row r="12" spans="2:8" ht="115.35" customHeight="1">
       <c r="B12" s="10" t="s">
         <v>472</v>
       </c>
@@ -29546,7 +29570,7 @@
       </c>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="2:8" ht="43.5">
+    <row r="13" spans="2:8" ht="45">
       <c r="B13" s="46" t="s">
         <v>459</v>
       </c>
@@ -29558,7 +29582,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="2:8" ht="29">
+    <row r="14" spans="2:8" ht="30">
       <c r="B14" s="46" t="s">
         <v>478</v>
       </c>
@@ -29570,7 +29594,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="2:8" ht="101.15" customHeight="1">
+    <row r="15" spans="2:8" ht="101.1" customHeight="1">
       <c r="B15" s="8" t="s">
         <v>481</v>
       </c>
@@ -29582,7 +29606,7 @@
       </c>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="2:8" ht="72.5">
+    <row r="16" spans="2:8" ht="75">
       <c r="B16" s="8" t="s">
         <v>495</v>
       </c>
@@ -29605,7 +29629,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="58">
+    <row r="17" spans="2:8" ht="90">
       <c r="B17" s="8" t="s">
         <v>494</v>
       </c>
@@ -29620,7 +29644,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="2:8" ht="43.5">
+    <row r="18" spans="2:8" ht="45">
       <c r="B18" s="8" t="s">
         <v>491</v>
       </c>
@@ -29635,7 +29659,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="2:8" ht="72.5">
+    <row r="19" spans="2:8" ht="75">
       <c r="B19" s="8" t="s">
         <v>496</v>
       </c>
@@ -29650,7 +29674,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="2:8" ht="116">
+    <row r="20" spans="2:8" ht="120">
       <c r="B20" s="8" t="s">
         <v>501</v>
       </c>
@@ -29667,7 +29691,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="2:8" ht="43.4" customHeight="1">
+    <row r="21" spans="2:8" ht="43.35" customHeight="1">
       <c r="B21" s="8" t="s">
         <v>504</v>
       </c>
@@ -29682,7 +29706,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="2:8" ht="87">
+    <row r="22" spans="2:8" ht="90">
       <c r="B22" s="8" t="s">
         <v>510</v>
       </c>
@@ -29697,7 +29721,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" ht="30">
       <c r="B23" s="8" t="s">
         <v>543</v>
       </c>
@@ -29726,7 +29750,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="2:8" ht="29">
+    <row r="26" spans="2:8" ht="30">
       <c r="B26" s="10" t="s">
         <v>505</v>
       </c>
@@ -29762,7 +29786,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="2:8" ht="29">
+    <row r="30" spans="2:8" ht="30">
       <c r="B30" s="46" t="s">
         <v>509</v>
       </c>
@@ -29773,7 +29797,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="14.5" customHeight="1"/>
+    <row r="32" spans="2:8" ht="14.45" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4294967295" r:id="rId1"/>
@@ -29788,18 +29812,18 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="83" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -29807,11 +29831,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="76" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -29829,19 +29853,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="83" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="79"/>
+      <c r="C11" s="83"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="83" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="79"/>
+      <c r="C12" s="83"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -29865,12 +29889,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="16.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -29878,13 +29902,13 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="30">
       <c r="B4" s="39" t="s">
         <v>419</v>
       </c>
       <c r="C4" s="38"/>
     </row>
-    <row r="6" spans="1:3" ht="87">
+    <row r="6" spans="1:3" ht="90">
       <c r="A6" s="44" t="s">
         <v>420</v>
       </c>
@@ -29909,12 +29933,12 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -29927,7 +29951,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="46" t="s">
         <v>430</v>
       </c>
@@ -29962,12 +29986,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -29980,7 +30004,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="46" t="s">
         <v>438</v>
       </c>
@@ -29991,7 +30015,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29">
+    <row r="7" spans="1:3" ht="30">
       <c r="A7" s="46" t="s">
         <v>441</v>
       </c>
@@ -30015,12 +30039,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="38" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="38" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="38"/>
+    <col min="1" max="1" width="23.5703125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="38" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="38"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -30028,12 +30052,12 @@
         <v>444</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29">
+    <row r="4" spans="1:3" ht="30">
       <c r="B4" s="39" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="46" t="s">
         <v>446</v>
       </c>
@@ -30044,7 +30068,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29">
+    <row r="7" spans="1:3" ht="30">
       <c r="A7" s="46" t="s">
         <v>448</v>
       </c>
@@ -30068,12 +30092,12 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -30081,12 +30105,12 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.5">
+    <row r="4" spans="1:3" ht="45">
       <c r="B4" s="39" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="46" t="s">
         <v>426</v>
       </c>
@@ -30110,12 +30134,12 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.453125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="63.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -30124,7 +30148,7 @@
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="43.5">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
@@ -30145,7 +30169,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.5">
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -30157,7 +30181,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="43.5">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" s="7" t="s">
         <v>87</v>
       </c>
@@ -30169,7 +30193,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="72.5">
+    <row r="9" spans="1:4" ht="90">
       <c r="A9" s="8" t="s">
         <v>269</v>
       </c>
@@ -30181,7 +30205,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="43.5">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
@@ -30193,7 +30217,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="58">
+    <row r="11" spans="1:4" ht="75">
       <c r="A11" s="8" t="s">
         <v>264</v>
       </c>
@@ -30205,7 +30229,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" s="12" customFormat="1" ht="43.5">
+    <row r="12" spans="1:4" s="12" customFormat="1" ht="45">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -30217,7 +30241,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" s="12" customFormat="1" ht="43.5">
+    <row r="13" spans="1:4" s="12" customFormat="1" ht="45">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -30229,7 +30253,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="43.5">
+    <row r="14" spans="1:4" ht="45">
       <c r="A14" s="8" t="s">
         <v>275</v>
       </c>
@@ -30241,7 +30265,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" ht="43.5">
+    <row r="15" spans="1:4" s="3" customFormat="1" ht="45">
       <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
@@ -30253,7 +30277,7 @@
       </c>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" ht="43.5">
+    <row r="16" spans="1:4" ht="45">
       <c r="A16" s="8" t="s">
         <v>218</v>
       </c>
@@ -30265,7 +30289,7 @@
       </c>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="43.5">
+    <row r="17" spans="1:4" ht="60">
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
@@ -30277,7 +30301,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="43.5">
+    <row r="18" spans="1:4" ht="60">
       <c r="A18" s="7" t="s">
         <v>21</v>
       </c>
@@ -30289,7 +30313,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="72.5">
+    <row r="19" spans="1:4" ht="75">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -30301,7 +30325,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="87">
+    <row r="20" spans="1:4" ht="90">
       <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
@@ -30313,7 +30337,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" ht="58">
+    <row r="21" spans="1:4" ht="60">
       <c r="A21" s="30" t="s">
         <v>224</v>
       </c>
@@ -30325,7 +30349,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="29">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" s="12" t="s">
         <v>22</v>
       </c>
@@ -30337,7 +30361,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" ht="29">
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="30">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -30359,7 +30383,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="72.5">
+    <row r="25" spans="1:4" ht="75">
       <c r="A25" s="8" t="s">
         <v>227</v>
       </c>
@@ -30371,7 +30395,7 @@
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" ht="87">
+    <row r="26" spans="1:4" ht="120">
       <c r="A26" s="6" t="s">
         <v>229</v>
       </c>
@@ -30383,7 +30407,7 @@
       </c>
       <c r="D26" s="12"/>
     </row>
-    <row r="27" spans="1:4" ht="58">
+    <row r="27" spans="1:4" ht="60">
       <c r="A27" s="6" t="s">
         <v>231</v>
       </c>
@@ -30431,11 +30455,11 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.54296875" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
@@ -30457,7 +30481,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="43.5">
+    <row r="5" spans="1:6" ht="45">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -30468,7 +30492,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.5">
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -30479,7 +30503,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="58">
+    <row r="7" spans="1:6" ht="60">
       <c r="A7" s="6" t="s">
         <v>104</v>
       </c>
@@ -30490,7 +30514,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.5">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
@@ -30504,7 +30528,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="174">
+    <row r="9" spans="1:6" ht="195">
       <c r="A9" s="8" t="s">
         <v>119</v>
       </c>
@@ -30515,7 +30539,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.5">
+    <row r="10" spans="1:6" ht="45">
       <c r="A10" s="8" t="s">
         <v>90</v>
       </c>
@@ -30526,7 +30550,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="72.5">
+    <row r="11" spans="1:6" ht="75">
       <c r="A11" s="8" t="s">
         <v>92</v>
       </c>
@@ -30537,7 +30561,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="58">
+    <row r="12" spans="1:6" ht="60">
       <c r="A12" s="8" t="s">
         <v>93</v>
       </c>
@@ -30548,7 +30572,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="72.5">
+    <row r="13" spans="1:6" ht="75">
       <c r="A13" s="8" t="s">
         <v>97</v>
       </c>
@@ -30559,7 +30583,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="72.5">
+    <row r="14" spans="1:6" ht="90">
       <c r="A14" s="8" t="s">
         <v>98</v>
       </c>
@@ -30570,7 +30594,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="58">
+    <row r="15" spans="1:6" ht="60">
       <c r="A15" s="8" t="s">
         <v>99</v>
       </c>
@@ -30581,7 +30605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="87">
+    <row r="16" spans="1:6" ht="90">
       <c r="A16" s="8" t="s">
         <v>103</v>
       </c>
@@ -30592,7 +30616,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="72.5">
+    <row r="17" spans="1:3" ht="75">
       <c r="A17" s="8" t="s">
         <v>101</v>
       </c>
@@ -30603,7 +30627,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="87">
+    <row r="18" spans="1:3" ht="105">
       <c r="A18" s="8" t="s">
         <v>196</v>
       </c>
@@ -30614,7 +30638,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="87">
+    <row r="19" spans="1:3" ht="90">
       <c r="A19" s="8" t="s">
         <v>102</v>
       </c>
@@ -30625,7 +30649,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="43.5">
+    <row r="20" spans="1:3" ht="60">
       <c r="A20" s="8" t="s">
         <v>203</v>
       </c>
@@ -30636,7 +30660,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="87">
+    <row r="21" spans="1:3" ht="90">
       <c r="A21" s="8" t="s">
         <v>106</v>
       </c>
@@ -30647,7 +30671,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5">
+    <row r="22" spans="1:3" ht="75">
       <c r="A22" s="8" t="s">
         <v>108</v>
       </c>
@@ -30658,7 +30682,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="87">
+    <row r="23" spans="1:3" ht="90">
       <c r="A23" s="8" t="s">
         <v>109</v>
       </c>
@@ -30669,7 +30693,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="87">
+    <row r="24" spans="1:3" ht="105">
       <c r="A24" s="8" t="s">
         <v>110</v>
       </c>
@@ -30691,7 +30715,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="72.5">
+    <row r="26" spans="1:3" ht="90">
       <c r="A26" s="8" t="s">
         <v>111</v>
       </c>
@@ -30702,7 +30726,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="87">
+    <row r="27" spans="1:3" ht="90">
       <c r="A27" s="8" t="s">
         <v>113</v>
       </c>
@@ -30713,7 +30737,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="72.5">
+    <row r="28" spans="1:3" ht="75">
       <c r="A28" s="8" t="s">
         <v>114</v>
       </c>
@@ -30724,7 +30748,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="116">
+    <row r="29" spans="1:3" ht="120">
       <c r="A29" s="8" t="s">
         <v>115</v>
       </c>
@@ -30735,7 +30759,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="174">
+    <row r="30" spans="1:3" ht="195">
       <c r="A30" s="6" t="s">
         <v>116</v>
       </c>
@@ -30746,7 +30770,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="159.5">
+    <row r="31" spans="1:3" ht="210">
       <c r="A31" s="6" t="s">
         <v>117</v>
       </c>
@@ -30757,7 +30781,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="203">
+    <row r="32" spans="1:3" ht="240">
       <c r="A32" s="9" t="s">
         <v>60</v>
       </c>
@@ -30793,11 +30817,11 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -30822,7 +30846,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="27"/>
     </row>
-    <row r="5" spans="1:3" ht="29">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -30833,7 +30857,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.5">
+    <row r="6" spans="1:3" ht="60">
       <c r="A6" s="3" t="s">
         <v>135</v>
       </c>
@@ -30844,7 +30868,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29">
+    <row r="7" spans="1:3" ht="30">
       <c r="A7" s="10" t="s">
         <v>136</v>
       </c>
@@ -30855,7 +30879,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="29">
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="10" t="s">
         <v>139</v>
       </c>
@@ -30866,7 +30890,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.5">
+    <row r="9" spans="1:3" ht="45">
       <c r="A9" s="10" t="s">
         <v>140</v>
       </c>
@@ -30877,7 +30901,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.5">
+    <row r="10" spans="1:3" ht="45">
       <c r="A10" s="10" t="s">
         <v>142</v>
       </c>
@@ -30899,7 +30923,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.5">
+    <row r="12" spans="1:3" ht="45">
       <c r="A12" s="10" t="s">
         <v>152</v>
       </c>
@@ -30910,7 +30934,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="43.5">
+    <row r="13" spans="1:3" ht="45">
       <c r="A13" s="8" t="s">
         <v>156</v>
       </c>
@@ -30921,7 +30945,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="43.5">
+    <row r="14" spans="1:3" ht="45">
       <c r="A14" s="8" t="s">
         <v>161</v>
       </c>
@@ -30932,7 +30956,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="72.5">
+    <row r="15" spans="1:3" ht="75">
       <c r="A15" s="8" t="s">
         <v>166</v>
       </c>
@@ -30943,7 +30967,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="43.5">
+    <row r="16" spans="1:3" ht="45">
       <c r="A16" s="8" t="s">
         <v>175</v>
       </c>
@@ -30954,7 +30978,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="43.5">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" s="8" t="s">
         <v>177</v>
       </c>
@@ -30965,7 +30989,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="43.5">
+    <row r="18" spans="1:3" ht="45">
       <c r="A18" s="8" t="s">
         <v>178</v>
       </c>
@@ -30976,7 +31000,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="43.5">
+    <row r="19" spans="1:3" ht="45">
       <c r="A19" s="8" t="s">
         <v>181</v>
       </c>
@@ -30987,7 +31011,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="58">
+    <row r="20" spans="1:3" ht="60">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
@@ -30998,7 +31022,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="72.5">
+    <row r="21" spans="1:3" ht="90">
       <c r="A21" s="10" t="s">
         <v>150</v>
       </c>
@@ -31009,7 +31033,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5">
+    <row r="22" spans="1:3" ht="75">
       <c r="A22" s="8" t="s">
         <v>183</v>
       </c>
@@ -31020,7 +31044,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="58">
+    <row r="23" spans="1:3" ht="60">
       <c r="A23" s="10" t="s">
         <v>67</v>
       </c>
@@ -31031,7 +31055,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="87">
+    <row r="24" spans="1:3" ht="90">
       <c r="A24" s="8" t="s">
         <v>186</v>
       </c>
@@ -31042,7 +31066,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="101.5">
+    <row r="25" spans="1:3" ht="120">
       <c r="A25" s="10" t="s">
         <v>232</v>
       </c>
@@ -31053,7 +31077,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="72.5">
+    <row r="26" spans="1:3" ht="90">
       <c r="A26" s="8" t="s">
         <v>234</v>
       </c>
@@ -31064,7 +31088,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="72.5">
+    <row r="27" spans="1:3" ht="75">
       <c r="A27" s="10" t="s">
         <v>236</v>
       </c>
@@ -31075,7 +31099,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="43.5">
+    <row r="28" spans="1:3" ht="45">
       <c r="A28" s="7" t="s">
         <v>240</v>
       </c>
@@ -31086,7 +31110,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="58">
+    <row r="29" spans="1:3" ht="75">
       <c r="A29" s="7" t="s">
         <v>242</v>
       </c>
@@ -31097,7 +31121,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="45.65" customHeight="1">
+    <row r="30" spans="1:3" ht="45.6" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>245</v>
       </c>
@@ -31108,7 +31132,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="43.5">
+    <row r="31" spans="1:3" ht="45">
       <c r="A31" s="7" t="s">
         <v>247</v>
       </c>
@@ -31119,7 +31143,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="43.5">
+    <row r="32" spans="1:3" ht="45">
       <c r="A32" s="7" t="s">
         <v>251</v>
       </c>
@@ -31130,7 +31154,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="43.5">
+    <row r="33" spans="1:3" ht="45">
       <c r="A33" s="8" t="s">
         <v>148</v>
       </c>
@@ -31141,7 +31165,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="58">
+    <row r="34" spans="1:3" ht="60">
       <c r="A34" s="8" t="s">
         <v>148</v>
       </c>
@@ -31234,13 +31258,13 @@
       <selection activeCell="E18" sqref="E18:J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="28"/>
-    <col min="2" max="2" width="30.54296875" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1796875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="52.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="28"/>
+    <col min="1" max="1" width="8.85546875" style="28"/>
+    <col min="2" max="2" width="30.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="28"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -31248,7 +31272,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="58">
+    <row r="3" spans="2:4" ht="60">
       <c r="C3" s="37" t="s">
         <v>545</v>
       </c>
@@ -31272,7 +31296,7 @@
       <c r="B7" s="59"/>
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="2:4" ht="29">
+    <row r="8" spans="2:4" ht="30">
       <c r="B8" s="11" t="s">
         <v>560</v>
       </c>
@@ -31283,7 +31307,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="29">
+    <row r="9" spans="2:4" ht="30">
       <c r="B9" s="7" t="s">
         <v>553</v>
       </c>
@@ -31294,7 +31318,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="29">
+    <row r="10" spans="2:4" ht="30">
       <c r="B10" s="7" t="s">
         <v>556</v>
       </c>
@@ -31305,7 +31329,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="29">
+    <row r="11" spans="2:4" ht="30">
       <c r="B11" s="11" t="s">
         <v>559</v>
       </c>
@@ -31316,7 +31340,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="29">
+    <row r="12" spans="2:4" ht="30">
       <c r="B12" s="11" t="s">
         <v>563</v>
       </c>
@@ -31327,7 +31351,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="43.5">
+    <row r="13" spans="2:4" ht="45">
       <c r="B13" s="11" t="s">
         <v>565</v>
       </c>
@@ -31338,7 +31362,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="43.5">
+    <row r="14" spans="2:4" ht="45">
       <c r="B14" s="11" t="s">
         <v>569</v>
       </c>
@@ -31349,7 +31373,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="43.5">
+    <row r="15" spans="2:4" ht="45">
       <c r="B15" s="11" t="s">
         <v>571</v>
       </c>
@@ -31360,7 +31384,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="29">
+    <row r="16" spans="2:4" ht="30">
       <c r="B16" s="7" t="s">
         <v>574</v>
       </c>
@@ -31371,7 +31395,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="159.5">
+    <row r="17" spans="2:13" ht="165">
       <c r="B17" s="7" t="s">
         <v>578</v>
       </c>
@@ -31382,7 +31406,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="145" customHeight="1">
+    <row r="18" spans="2:13" ht="144.94999999999999" customHeight="1">
       <c r="B18" s="11" t="s">
         <v>581</v>
       </c>
@@ -31392,14 +31416,14 @@
       <c r="D18" s="66" t="s">
         <v>583</v>
       </c>
-      <c r="E18" s="69" t="s">
+      <c r="E18" s="72" t="s">
         <v>584</v>
       </c>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -31411,19 +31435,19 @@
       <c r="D19" s="66" t="s">
         <v>587</v>
       </c>
-      <c r="E19" s="69" t="s">
+      <c r="E19" s="72" t="s">
         <v>588</v>
       </c>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-    </row>
-    <row r="20" spans="2:13" ht="29">
+      <c r="F19" s="72"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
+    </row>
+    <row r="20" spans="2:13" ht="30">
       <c r="B20" s="7" t="s">
         <v>589</v>
       </c>
@@ -31444,17 +31468,17 @@
       <c r="D21" s="66" t="s">
         <v>721</v>
       </c>
-      <c r="E21" s="69" t="s">
+      <c r="E21" s="72" t="s">
         <v>722</v>
       </c>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
+      <c r="K21" s="72"/>
+      <c r="L21" s="72"/>
+      <c r="M21" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -31475,13 +31499,13 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="27"/>
-    <col min="2" max="2" width="43.7265625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="46.7265625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.7265625" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="27"/>
+    <col min="1" max="1" width="9.140625" style="27"/>
+    <col min="2" max="2" width="43.7109375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
@@ -31490,22 +31514,22 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="71" t="s">
-        <v>735</v>
-      </c>
-      <c r="D4" s="71"/>
+      <c r="C4" s="74" t="s">
+        <v>732</v>
+      </c>
+      <c r="D4" s="74"/>
     </row>
     <row r="5" spans="2:4" ht="90" customHeight="1">
-      <c r="C5" s="71" t="s">
-        <v>736</v>
-      </c>
-      <c r="D5" s="71"/>
+      <c r="C5" s="74" t="s">
+        <v>733</v>
+      </c>
+      <c r="D5" s="74"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="71" t="s">
-        <v>744</v>
-      </c>
-      <c r="D6" s="71"/>
+      <c r="C6" s="74" t="s">
+        <v>741</v>
+      </c>
+      <c r="D6" s="74"/>
     </row>
     <row r="8" spans="2:4" ht="75" customHeight="1">
       <c r="B8" s="10" t="s">
@@ -31529,34 +31553,34 @@
         <v>729</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="72.5">
+    <row r="10" spans="2:4" ht="75">
       <c r="B10" s="8" t="s">
         <v>730</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="60">
+      <c r="B11" s="10" t="s">
+        <v>735</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="30">
+      <c r="B12" s="46" t="s">
+        <v>739</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>740</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="58">
-      <c r="B11" s="10" t="s">
-        <v>738</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>737</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="29">
-      <c r="B12" s="46" t="s">
-        <v>742</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>743</v>
       </c>
     </row>
   </sheetData>
@@ -31572,18 +31596,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D42"/>
+  <dimension ref="B2:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44:D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="27"/>
-    <col min="2" max="3" width="43.54296875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="27"/>
+    <col min="1" max="1" width="8.7109375" style="27"/>
+    <col min="2" max="2" width="49" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -31662,188 +31687,214 @@
         <v>605</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
-      <c r="B14" s="60" t="s">
+    <row r="13" spans="2:4">
+      <c r="B13" s="60" t="s">
         <v>616</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" s="71" customFormat="1">
+      <c r="B14" s="84" t="s">
+        <v>752</v>
+      </c>
+      <c r="C14" s="70" t="s">
+        <v>751</v>
+      </c>
+      <c r="D14" s="69" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="15" spans="2:4">
       <c r="B15" s="27" t="s">
+        <v>614</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>607</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" s="71" customFormat="1"/>
+    <row r="18" spans="2:4" s="71" customFormat="1">
+      <c r="B18" s="60" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" s="71" customFormat="1">
+      <c r="B19" s="27" t="s">
         <v>622</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C19" s="43" t="s">
         <v>623</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D19" s="61" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
-      <c r="B16" s="27" t="s">
-        <v>614</v>
-      </c>
-      <c r="C16" s="43" t="s">
-        <v>607</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="27" t="s">
+    <row r="20" spans="2:4" s="71" customFormat="1">
+      <c r="B20" s="60"/>
+    </row>
+    <row r="21" spans="2:4" s="71" customFormat="1"/>
+    <row r="22" spans="2:4" s="71" customFormat="1">
+      <c r="B22" s="60" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" s="71" customFormat="1">
+      <c r="B23" s="71" t="s">
         <v>619</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C23" s="70" t="s">
         <v>617</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D23" s="69" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="27" t="s">
+    <row r="24" spans="2:4" s="71" customFormat="1">
+      <c r="B24" s="71" t="s">
         <v>625</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C24" s="70" t="s">
         <v>627</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D24" s="69" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="27" t="s">
+    <row r="25" spans="2:4">
+      <c r="B25" s="71" t="s">
         <v>626</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C25" s="70" t="s">
         <v>620</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D25" s="69" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="60" t="s">
+    <row r="26" spans="2:4" s="71" customFormat="1">
+      <c r="C26" s="70"/>
+      <c r="D26" s="69"/>
+    </row>
+    <row r="27" spans="2:4" s="71" customFormat="1">
+      <c r="C27" s="70"/>
+      <c r="D27" s="69"/>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="60" t="s">
         <v>706</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="27" t="s">
+    <row r="29" spans="2:4">
+      <c r="B29" s="27" t="s">
         <v>709</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C29" s="43" t="s">
         <v>707</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D29" s="45" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="27" t="s">
+    <row r="30" spans="2:4">
+      <c r="B30" s="27" t="s">
         <v>710</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C30" s="43" t="s">
         <v>617</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D30" s="27" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="29">
-      <c r="B26" s="38" t="s">
+    <row r="31" spans="2:4" ht="30">
+      <c r="B31" s="38" t="s">
         <v>714</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D31" s="46" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="27" t="s">
+    <row r="32" spans="2:4">
+      <c r="B32" s="27" t="s">
         <v>717</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C32" s="43" t="s">
         <v>715</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D32" s="27" t="s">
         <v>716</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="27" t="s">
-        <v>719</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>718</v>
-      </c>
-      <c r="D28" s="27" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="60" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33" s="27" t="s">
-        <v>733</v>
+        <v>719</v>
       </c>
       <c r="C33" s="43" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="27" t="s">
-        <v>734</v>
-      </c>
-      <c r="C34" s="43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="B38" s="60" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="B39" s="27" t="s">
-        <v>746</v>
-      </c>
-      <c r="C39" s="43" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ht="29">
-      <c r="B40" s="68" t="s">
-        <v>748</v>
-      </c>
-      <c r="C40" s="67" t="s">
-        <v>749</v>
+        <v>718</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="60" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="27" t="s">
+        <v>731</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="60" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="27" t="s">
+        <v>743</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="30">
+      <c r="B42" s="68" t="s">
+        <v>745</v>
+      </c>
+      <c r="C42" s="67" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="27" t="s">
+        <v>747</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="30">
+      <c r="B44" s="68" t="s">
+        <v>749</v>
+      </c>
+      <c r="C44" s="74" t="s">
         <v>750</v>
       </c>
-      <c r="C41" s="43" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="29">
-      <c r="B42" s="68" t="s">
-        <v>752</v>
-      </c>
-      <c r="C42" s="71" t="s">
-        <v>753</v>
-      </c>
-      <c r="D42" s="80"/>
+      <c r="D44" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C44:D44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -31858,13 +31909,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="27"/>
-    <col min="2" max="2" width="30.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1796875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="52.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="8.85546875" style="27"/>
+    <col min="2" max="2" width="30.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -31892,7 +31943,7 @@
       <c r="B6" s="45"/>
       <c r="C6" s="43"/>
     </row>
-    <row r="7" spans="2:4" ht="29">
+    <row r="7" spans="2:4" ht="30">
       <c r="B7" s="46" t="s">
         <v>550</v>
       </c>
@@ -31904,7 +31955,7 @@
     <row r="9" spans="2:4">
       <c r="B9" s="45"/>
     </row>
-    <row r="10" spans="2:4" ht="101.5" customHeight="1">
+    <row r="10" spans="2:4" ht="101.45" customHeight="1">
       <c r="B10" s="45"/>
       <c r="C10" s="43"/>
       <c r="D10" s="38"/>
@@ -31926,10 +31977,10 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -31968,7 +32019,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="101.5" customHeight="1">
+    <row r="9" spans="1:3" ht="101.45" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>295</v>
       </c>

</xml_diff>

<commit_message>
added more to 'iptables' tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90394E2C-224C-41D5-8851-539F7C4B9662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E0BDDB-E84C-415A-9FB0-686D59061526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="758">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="762">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -26822,9 +26822,6 @@
     </r>
   </si>
   <si>
-    <t>iptables -A INPUT -s 10.10.10.10 -j DROP</t>
-  </si>
-  <si>
     <r>
       <t>Append (attach) this new rule to the INPUT chain; anything from source 10.10.10.10, DROP the data'
 '</t>
@@ -26946,75 +26943,7 @@
     </r>
   </si>
   <si>
-    <t>iptables -L</t>
-  </si>
-  <si>
     <t>lists all rules on all chains</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">--policy &lt;CHAIN&gt; &lt;ACTION&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= sets the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>default</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>policy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for an iptables chain</t>
-    </r>
   </si>
   <si>
     <t>fetch all remote repo differences</t>
@@ -27217,9 +27146,6 @@
     </r>
   </si>
   <si>
-    <t>iptables -L -v</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -27361,11 +27287,6 @@
       </rPr>
       <t xml:space="preserve"> output</t>
     </r>
-  </si>
-  <si>
-    <t>iptables --policy INPUT ACCEPT
-iptables --policy OUTPUT ACCEPT
-iptables --policy FORWARD ACCEPT</t>
   </si>
   <si>
     <t>sets the default action to 'ACCEPT' for the 'INPUT' policy
@@ -27374,58 +27295,6 @@
 setting the default policy for these 3 lists or 'chains' sets the default policy to 'ACCEPT' for the entire firewall</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-I &lt;CHAIN&gt; &lt;NUMBER&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>inserts</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> a new rule on a specific chain at a specific location in the chain</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">iptables -I </t>
-  </si>
-  <si>
-    <t>CHAIN CONCEPT (important!)
-firewall 'chains' are made up of 'rules'
-'Rules' are evaluated sequentially in a waterfall operation; e.g. rule 1 is evaluated, then rule 2, then rule 3, then rule 4 etc.</t>
-  </si>
-  <si>
     <t>CREATE NEW BRANCH FOR MERGE INTO MAIN</t>
   </si>
   <si>
@@ -27474,6 +27343,304 @@
   </si>
   <si>
     <t>CREATE NEW LOCAL REPO FROM REMOTE REPO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CHAIN CONCEPT (important!)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>firewall 'chains' are made up of 'rules'
+'Rules' are evaluated sequentially in a waterfall operation; e.g. rule 1 is evaluated, then rule 2, then rule 3, then rule 4 etc.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">--policy {&lt;CHAIN&gt; &lt;ACTION&gt;} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= sets the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>policy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for an iptables chain</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>READING COMMAND SYNTAX:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">{ } </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= encloses mandatory parameters
+[ ] = encloses optional parameters
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt; &gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = encloses variables where you can input your own value
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = separates two or more items, only one can be chosen
+</t>
+    </r>
+  </si>
+  <si>
+    <t>sudo iptables -L</t>
+  </si>
+  <si>
+    <t>sudo iptables -A INPUT -s 10.10.10.10 -j DROP</t>
+  </si>
+  <si>
+    <t>sudo iptables -L -v</t>
+  </si>
+  <si>
+    <t>sudo iptables -I INPUT 1 -s 10.10.10.20 -j DROP</t>
+  </si>
+  <si>
+    <t>sudo iptables --policy INPUT ACCEPT
+sudo iptables --policy OUTPUT ACCEPT
+sudo iptables --policy FORWARD ACCEPT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-I {&lt;CHAIN&gt;} {&lt;NUMBER&gt;} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inserts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a new rule on a specific chain at a specific location in the chain</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-F [&lt;CHAIN&gt;] [&lt;NUMBER&gt;] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>flush</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (delete) all rules in a chain</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo iptables -F INPUT </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">flushes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(deletes) all rules in the INPUT chain</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -27640,7 +27807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -27830,21 +27997,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -27880,9 +28032,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -28430,17 +28579,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="72" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="77"/>
+      <c r="C2" s="72"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="73" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -28448,10 +28597,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="74" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="79"/>
+      <c r="B6" s="74"/>
     </row>
     <row r="7" spans="1:4" ht="45">
       <c r="A7" s="35" t="s">
@@ -28580,88 +28729,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="76"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="71" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="76"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="76" t="s">
+      <c r="A24" s="71" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="76" t="s">
+      <c r="A25" s="71" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="76"/>
-      <c r="C25" s="76"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="76" t="s">
+      <c r="A26" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="76"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="71" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="76"/>
-      <c r="C27" s="76"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="76" t="s">
+      <c r="A28" s="71" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="76"/>
-      <c r="C28" s="76"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="76" t="s">
+      <c r="A29" s="71" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="72" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="72" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="76" t="s">
+      <c r="A32" s="71" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="71" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">
@@ -28850,7 +28999,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="75" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -28864,7 +29013,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="75">
-      <c r="A9" s="80"/>
+      <c r="A9" s="75"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -28876,7 +29025,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="30">
-      <c r="A10" s="80"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -28888,7 +29037,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="45">
-      <c r="A11" s="80"/>
+      <c r="A11" s="75"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -28900,7 +29049,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="45">
-      <c r="A12" s="80"/>
+      <c r="A12" s="75"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -28917,7 +29066,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="60">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="76" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -28931,7 +29080,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="75">
-      <c r="A16" s="81"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -28943,7 +29092,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="105">
-      <c r="A17" s="81"/>
+      <c r="A17" s="76"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -28955,7 +29104,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="105">
-      <c r="A18" s="81"/>
+      <c r="A18" s="76"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -28967,7 +29116,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="60">
-      <c r="A19" s="81" t="s">
+      <c r="A19" s="76" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -28981,7 +29130,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="60">
-      <c r="A20" s="81"/>
+      <c r="A20" s="76"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -28993,7 +29142,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="105">
-      <c r="A21" s="81"/>
+      <c r="A21" s="76"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -29005,7 +29154,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="60">
-      <c r="A22" s="81"/>
+      <c r="A22" s="76"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -29354,38 +29503,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="77" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="82"/>
+      <c r="D19" s="77"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="82" t="s">
+      <c r="C20" s="77" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="82"/>
+      <c r="D20" s="77"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="77" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="82"/>
+      <c r="D21" s="77"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="82" t="s">
+      <c r="C22" s="77" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="82"/>
+      <c r="D22" s="77"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="77" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="82"/>
+      <c r="D23" s="77"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -29398,38 +29547,38 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="82" t="s">
+      <c r="C25" s="77" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="82"/>
+      <c r="D25" s="77"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="82" t="s">
+      <c r="C26" s="77" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="82"/>
+      <c r="D26" s="77"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="82" t="s">
+      <c r="C27" s="77" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="82"/>
+      <c r="D27" s="77"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="82" t="s">
+      <c r="C28" s="77" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="82"/>
+      <c r="D28" s="77"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="82" t="s">
+      <c r="C29" s="77" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="82"/>
+      <c r="D29" s="77"/>
     </row>
     <row r="30" spans="2:4" ht="38.25">
       <c r="B30" s="27" t="s">
@@ -29818,12 +29967,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="78" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -29831,11 +29980,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="71" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -29853,19 +30002,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="83" t="s">
+      <c r="B11" s="78" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="83"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="78" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="83"/>
+      <c r="C12" s="78"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -31416,14 +31565,14 @@
       <c r="D18" s="66" t="s">
         <v>583</v>
       </c>
-      <c r="E18" s="72" t="s">
+      <c r="E18" s="67" t="s">
         <v>584</v>
       </c>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="73"/>
-      <c r="J18" s="73"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -31435,17 +31584,17 @@
       <c r="D19" s="66" t="s">
         <v>587</v>
       </c>
-      <c r="E19" s="72" t="s">
+      <c r="E19" s="67" t="s">
         <v>588</v>
       </c>
-      <c r="F19" s="72"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
     </row>
     <row r="20" spans="2:13" ht="30">
       <c r="B20" s="7" t="s">
@@ -31468,17 +31617,17 @@
       <c r="D21" s="66" t="s">
         <v>721</v>
       </c>
-      <c r="E21" s="72" t="s">
+      <c r="E21" s="67" t="s">
         <v>722</v>
       </c>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-      <c r="J21" s="72"/>
-      <c r="K21" s="72"/>
-      <c r="L21" s="72"/>
-      <c r="M21" s="72"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
+      <c r="L21" s="67"/>
+      <c r="M21" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -31493,10 +31642,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
-  <dimension ref="B3:D12"/>
+  <dimension ref="B3:D14"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -31514,80 +31663,98 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="69" t="s">
+        <v>729</v>
+      </c>
+      <c r="D4" s="69"/>
+    </row>
+    <row r="5" spans="2:4" ht="90" customHeight="1">
+      <c r="C5" s="69" t="s">
+        <v>730</v>
+      </c>
+      <c r="D5" s="69"/>
+    </row>
+    <row r="6" spans="2:4" ht="60" customHeight="1">
+      <c r="C6" s="69" t="s">
+        <v>750</v>
+      </c>
+      <c r="D6" s="69"/>
+    </row>
+    <row r="7" spans="2:4" ht="75" customHeight="1">
+      <c r="C7" s="69" t="s">
+        <v>752</v>
+      </c>
+      <c r="D7" s="69"/>
+    </row>
+    <row r="9" spans="2:4" ht="75" customHeight="1">
+      <c r="B9" s="10" t="s">
+        <v>724</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>754</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="45" t="s">
+        <v>726</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>753</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="75">
+      <c r="B11" s="8" t="s">
+        <v>751</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>757</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="60">
+      <c r="B12" s="10" t="s">
+        <v>731</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>732</v>
       </c>
-      <c r="D4" s="74"/>
-    </row>
-    <row r="5" spans="2:4" ht="90" customHeight="1">
-      <c r="C5" s="74" t="s">
-        <v>733</v>
-      </c>
-      <c r="D5" s="74"/>
-    </row>
-    <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="74" t="s">
-        <v>741</v>
-      </c>
-      <c r="D6" s="74"/>
-    </row>
-    <row r="8" spans="2:4" ht="75" customHeight="1">
-      <c r="B8" s="10" t="s">
-        <v>724</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>725</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="45" t="s">
-        <v>727</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>728</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="75">
-      <c r="B10" s="8" t="s">
-        <v>730</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>737</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="60">
-      <c r="B11" s="10" t="s">
-        <v>735</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>734</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="30">
-      <c r="B12" s="46" t="s">
-        <v>739</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>740</v>
+    </row>
+    <row r="13" spans="2:4" ht="45">
+      <c r="B13" s="46" t="s">
+        <v>758</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="30">
+      <c r="B14" s="46" t="s">
+        <v>759</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>761</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31598,7 +31765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
   <dimension ref="B2:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C44" sqref="C44:D44"/>
     </sheetView>
   </sheetViews>
@@ -31692,15 +31859,15 @@
         <v>616</v>
       </c>
     </row>
-    <row r="14" spans="2:4" s="71" customFormat="1">
-      <c r="B14" s="84" t="s">
-        <v>752</v>
-      </c>
-      <c r="C14" s="70" t="s">
-        <v>751</v>
-      </c>
-      <c r="D14" s="69" t="s">
-        <v>753</v>
+    <row r="14" spans="2:4">
+      <c r="B14" s="27" t="s">
+        <v>744</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>743</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -31714,13 +31881,12 @@
         <v>608</v>
       </c>
     </row>
-    <row r="17" spans="2:4" s="71" customFormat="1"/>
-    <row r="18" spans="2:4" s="71" customFormat="1">
+    <row r="18" spans="2:4">
       <c r="B18" s="60" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" s="71" customFormat="1">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" s="27" t="s">
         <v>622</v>
       </c>
@@ -31731,55 +31897,54 @@
         <v>624</v>
       </c>
     </row>
-    <row r="20" spans="2:4" s="71" customFormat="1">
+    <row r="20" spans="2:4">
       <c r="B20" s="60"/>
     </row>
-    <row r="21" spans="2:4" s="71" customFormat="1"/>
-    <row r="22" spans="2:4" s="71" customFormat="1">
+    <row r="22" spans="2:4">
       <c r="B22" s="60" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" s="71" customFormat="1">
-      <c r="B23" s="71" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="27" t="s">
         <v>619</v>
       </c>
-      <c r="C23" s="70" t="s">
+      <c r="C23" s="43" t="s">
         <v>617</v>
       </c>
-      <c r="D23" s="69" t="s">
+      <c r="D23" s="21" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="24" spans="2:4" s="71" customFormat="1">
-      <c r="B24" s="71" t="s">
+    <row r="24" spans="2:4">
+      <c r="B24" s="27" t="s">
         <v>625</v>
       </c>
-      <c r="C24" s="70" t="s">
+      <c r="C24" s="43" t="s">
         <v>627</v>
       </c>
-      <c r="D24" s="69" t="s">
+      <c r="D24" s="21" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="25" spans="2:4">
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="27" t="s">
         <v>626</v>
       </c>
-      <c r="C25" s="70" t="s">
+      <c r="C25" s="43" t="s">
         <v>620</v>
       </c>
-      <c r="D25" s="69" t="s">
+      <c r="D25" s="21" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="26" spans="2:4" s="71" customFormat="1">
-      <c r="C26" s="70"/>
-      <c r="D26" s="69"/>
-    </row>
-    <row r="27" spans="2:4" s="71" customFormat="1">
-      <c r="C27" s="70"/>
-      <c r="D27" s="69"/>
+    <row r="26" spans="2:4">
+      <c r="C26" s="43"/>
+      <c r="D26" s="21"/>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="C27" s="43"/>
+      <c r="D27" s="21"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="60" t="s">
@@ -31843,54 +32008,54 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="60" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="27" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="60" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="27" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="30">
-      <c r="B42" s="68" t="s">
-        <v>745</v>
-      </c>
-      <c r="C42" s="67" t="s">
-        <v>746</v>
+      <c r="B42" s="38" t="s">
+        <v>737</v>
+      </c>
+      <c r="C42" s="39" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="27" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="30">
-      <c r="B44" s="68" t="s">
-        <v>749</v>
-      </c>
-      <c r="C44" s="74" t="s">
-        <v>750</v>
-      </c>
-      <c r="D44" s="75"/>
+      <c r="B44" s="38" t="s">
+        <v>741</v>
+      </c>
+      <c r="C44" s="69" t="s">
+        <v>742</v>
+      </c>
+      <c r="D44" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fleshed out some iptables commands
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D858BCD3-1DF0-4DA8-8E4C-7CBE67734ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509A0225-2841-4FDF-A65D-7047E834DB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="763">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -26823,83 +26823,6 @@
   </si>
   <si>
     <r>
-      <t>Append (attach) this new rule to the INPUT chain; anything from source 10.10.10.10, DROP the data'
-'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-A: appends</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (attaches) the rule to the end of the INPUT chain
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-s: source</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">; where the data is coming from
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-j: jump</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>; as in 'jump to the DROP action'</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -26941,9 +26864,6 @@
       </rPr>
       <t xml:space="preserve"> all rules in selected chain</t>
     </r>
-  </si>
-  <si>
-    <t>lists all rules on all chains</t>
   </si>
   <si>
     <t>fetch all remote repo differences</t>
@@ -27087,66 +27007,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">ACTIONS determine what to do with a specific connection. The main actions are:
-ACCEPT: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">allow data to flow
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>REJECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: block data flow, and give the sender an error. Use if you want the sender to know they are being blocked by a firewall</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-DROP: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>block data flow without giving an explanation to the sender. Use if you don't want the sender to know that they are being blocked by a firewall, or that a system exists.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -27180,105 +27040,6 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> output</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">lists all rules on all chains in verbose mode; which displays the interface name, rule options (if any) and TOS masks
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-L</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>List</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> all rules
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-v</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>verbose</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -27639,7 +27400,439 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(deletes) all rules in the INPUT chain</t>
+      <t xml:space="preserve">(deletes) all rules in the INPUT chain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-F</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = flush (delete)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">lists all rules on all chains
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-L =</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>List</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> all rules</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">lists all rules on all chains in verbose mode; which displays the interface name, rule options (if any) and TOS masks
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-L =</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>List</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> all rules
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-v = verbose</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> output</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Append (attach) this new rule to the INPUT chain; anything from source 10.10.10.10, DROP the data'
+'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-A = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">appends (attaches) the rule to the end of the INPUT chain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-s = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">source; where the data is coming from
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-j</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = jump to (go perform this action)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>insert</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> rule into </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chain </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>at line 1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, anything from source 10.10.10.20 jump to DROP action (drop packet without responding to sender)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-I</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = insert rule
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-s </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= source; where the data is coming from
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-j </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= jump to (go perform this action)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ACTIONS determine what to do with the data that matches a rule. The main actions are:
+ACCEPT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">allow data to flow
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>REJECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: block data flow, and give the sender an error. Use if you want the sender to know they are being blocked by a firewall</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+DROP: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>block data flow without giving an explanation to the sender. Use if you don't want the sender to know that they are being blocked by a firewall, or that a system exists.</t>
     </r>
   </si>
 </sst>
@@ -31403,7 +31596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F8480C-E8CD-45AC-8F81-8D4ABFF602C5}">
   <dimension ref="B2:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E18" sqref="E18:J18"/>
     </sheetView>
   </sheetViews>
@@ -31645,7 +31838,7 @@
   <dimension ref="B3:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -31664,25 +31857,25 @@
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
       <c r="C4" s="69" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D4" s="69"/>
     </row>
-    <row r="5" spans="2:4" ht="90" customHeight="1">
+    <row r="5" spans="2:4" ht="60" customHeight="1">
       <c r="C5" s="69" t="s">
-        <v>730</v>
+        <v>746</v>
       </c>
       <c r="D5" s="69"/>
     </row>
-    <row r="6" spans="2:4" ht="60" customHeight="1">
+    <row r="6" spans="2:4" ht="90" customHeight="1">
       <c r="C6" s="69" t="s">
-        <v>750</v>
+        <v>762</v>
       </c>
       <c r="D6" s="69"/>
     </row>
     <row r="7" spans="2:4" ht="75" customHeight="1">
       <c r="C7" s="69" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="D7" s="69"/>
     </row>
@@ -31691,69 +31884,72 @@
         <v>724</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="D9" s="26" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30">
+      <c r="B10" s="45" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10" s="45" t="s">
-        <v>726</v>
-      </c>
       <c r="C10" s="43" t="s">
-        <v>753</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>727</v>
+        <v>749</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="75">
       <c r="B11" s="8" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="60">
       <c r="B12" s="10" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="45">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="90">
       <c r="B13" s="46" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>756</v>
+        <v>752</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>761</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30">
       <c r="B14" s="46" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>760</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>761</v>
+        <v>756</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>757</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31861,13 +32057,13 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="27" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -31883,7 +32079,7 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="60" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -31902,7 +32098,7 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="60" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -32008,52 +32204,52 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="60" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="27" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="60" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="27" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
       <c r="C41" s="43" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="30">
       <c r="B42" s="38" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="27" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
       <c r="C43" s="43" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="30">
       <c r="B44" s="38" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C44" s="69" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="D44" s="70"/>
     </row>

</xml_diff>

<commit_message>
fleshed out some more iptables
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509A0225-2841-4FDF-A65D-7047E834DB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C866CC-9AB6-4894-82F8-6CF6EB11738F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
@@ -27380,55 +27380,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">flushes </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(deletes) all rules in the INPUT chain
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-F</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = flush (delete)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">lists all rules on all chains
 </t>
     </r>
@@ -27833,6 +27784,78 @@
         <scheme val="minor"/>
       </rPr>
       <t>block data flow without giving an explanation to the sender. Use if you don't want the sender to know that they are being blocked by a firewall, or that a system exists.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">flushes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(deletes) all rules in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-F</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = flush (delete)</t>
     </r>
   </si>
 </sst>
@@ -31838,7 +31861,7 @@
   <dimension ref="B3:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -31869,7 +31892,7 @@
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
       <c r="C6" s="69" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D6" s="69"/>
     </row>
@@ -31887,7 +31910,7 @@
         <v>750</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30">
@@ -31898,7 +31921,7 @@
         <v>749</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="75">
@@ -31920,7 +31943,7 @@
         <v>751</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="90">
@@ -31931,7 +31954,7 @@
         <v>752</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30">
@@ -31942,7 +31965,7 @@
         <v>756</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated work on iptables
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C866CC-9AB6-4894-82F8-6CF6EB11738F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C964CC90-9C09-4CD6-BC5A-6106EECCFAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="766">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -26787,50 +26787,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">-A </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>append</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> a rule to the end of a selected chain</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>-L</t>
     </r>
     <r>
@@ -27107,23 +27063,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">CHAIN CONCEPT (important!)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>firewall 'chains' are made up of 'rules'
-'Rules' are evaluated sequentially in a waterfall operation; e.g. rule 1 is evaluated, then rule 2, then rule 3, then rule 4 etc.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -27274,9 +27213,6 @@
     <t>sudo iptables -L</t>
   </si>
   <si>
-    <t>sudo iptables -A INPUT -s 10.10.10.10 -j DROP</t>
-  </si>
-  <si>
     <t>sudo iptables -L -v</t>
   </si>
   <si>
@@ -27508,7 +27444,453 @@
   </si>
   <si>
     <r>
-      <t>Append (attach) this new rule to the INPUT chain; anything from source 10.10.10.10, DROP the data'
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>insert</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> rule into </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chain </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>at line 1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, anything from source 10.10.10.20 jump to DROP action (drop packet without responding to sender)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-I</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = insert rule
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-s </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= source; where the data is coming from
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-j </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= jump to (go perform this action)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ACTIONS determine what to do with the data that matches a rule. The main actions are:
+ACCEPT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">allow data to flow
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>REJECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: block data flow, and give the sender an error. Use if you want the sender to know they are being blocked by a firewall</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+DROP: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>block data flow without giving an explanation to the sender. Use if you don't want the sender to know that they are being blocked by a firewall, or that a system exists.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">flushes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(deletes) all rules in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-F</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = flush (delete)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CHAIN CONCEPT (important!)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>firewall 'chains' are made up of 'rules'
+'Rules' are evaluated sequentially in a waterfall operation; i.e. rule 1 is evaluated, then rule 2, then rule 3, then rule 4 etc.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the first rule that matches will grab the data and perform it's operation on it, and no further evaluations will take place </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(i.e. if the data matches rule 4, rule 5 will not be evaluated. All rule evaluations will stop)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-A {&lt;CHAIN&gt;} [options] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>append</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a rule to the end of a selected chain</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Append</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (attach) this new rule to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chain; anything from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>source</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> subnet 10.10.10.0/24, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DROP</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the data'
 '</t>
     </r>
     <r>
@@ -27584,28 +27966,80 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>insert</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> rule into </t>
+    <t>sudo iptables -A INPUT -s 10.10.10.0/24 -j DROP
+-or-
+sudo iptables -A INPUT -s 10.10.10.0/255.255.255.0 -j DROP</t>
+  </si>
+  <si>
+    <t>sudo -A INPUT -p tcp -s 10.10.10.10 -j DROP</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-p {tcp|udp}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>protocol;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tells iptables what protocol you wish to match on</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>append</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> new rule to </t>
     </r>
     <r>
       <rPr>
@@ -27628,30 +28062,76 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> chain </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>at line 1</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, anything from source 10.10.10.20 jump to DROP action (drop packet without responding to sender)
+      <t xml:space="preserve"> chain, any </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCP</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> traffic from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>source</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 10.10.10.10, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DROP</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the data
 </t>
     </r>
     <r>
@@ -27664,18 +28144,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>-I</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = insert rule
+      <t xml:space="preserve">-p </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= protocol; match on the following protocol value
 </t>
     </r>
     <r>
@@ -27688,18 +28168,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">-s </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= source; where the data is coming from
+      <t>-s</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = source; where the data is coming from
 </t>
     </r>
     <r>
@@ -27712,150 +28192,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">-j </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= jump to (go perform this action)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ACTIONS determine what to do with the data that matches a rule. The main actions are:
-ACCEPT: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">allow data to flow
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>REJECT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: block data flow, and give the sender an error. Use if you want the sender to know they are being blocked by a firewall</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-DROP: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>block data flow without giving an explanation to the sender. Use if you don't want the sender to know that they are being blocked by a firewall, or that a system exists.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">flushes </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(deletes) all rules in the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>INPUT</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> chain
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-F</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = flush (delete)</t>
+      <t>-j</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = jump to (go perform this action)</t>
     </r>
   </si>
 </sst>
@@ -31858,17 +32206,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
-  <dimension ref="B3:D14"/>
+  <dimension ref="B3:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="27"/>
     <col min="2" max="2" width="43.7109375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" style="27" customWidth="1"/>
     <col min="4" max="4" width="56.7109375" style="27" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="27"/>
   </cols>
@@ -31880,92 +32228,103 @@
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
       <c r="C4" s="69" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="D4" s="69"/>
     </row>
-    <row r="5" spans="2:4" ht="60" customHeight="1">
+    <row r="5" spans="2:4" ht="75" customHeight="1">
       <c r="C5" s="69" t="s">
-        <v>746</v>
+        <v>759</v>
       </c>
       <c r="D5" s="69"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
       <c r="C6" s="69" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="D6" s="69"/>
     </row>
     <row r="7" spans="2:4" ht="75" customHeight="1">
       <c r="C7" s="69" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D7" s="69"/>
     </row>
     <row r="9" spans="2:4" ht="75" customHeight="1">
-      <c r="B9" s="10" t="s">
-        <v>724</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>750</v>
+      <c r="B9" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>762</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30">
       <c r="B10" s="45" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="75">
       <c r="B11" s="8" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="60">
       <c r="B12" s="10" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="90">
+      <c r="B13" s="8" t="s">
         <v>751</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="90">
-      <c r="B13" s="46" t="s">
-        <v>754</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30">
       <c r="B14" s="46" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>762</v>
+        <v>758</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="75">
+      <c r="B15" s="8" t="s">
+        <v>764</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>765</v>
       </c>
     </row>
   </sheetData>
@@ -32080,13 +32439,13 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="27" t="s">
+        <v>739</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>738</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>740</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>739</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -32102,7 +32461,7 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="60" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -32121,7 +32480,7 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="60" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -32227,52 +32586,52 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="60" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="27" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="60" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="27" t="s">
+        <v>730</v>
+      </c>
+      <c r="C41" s="43" t="s">
         <v>731</v>
-      </c>
-      <c r="C41" s="43" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="30">
       <c r="B42" s="38" t="s">
+        <v>732</v>
+      </c>
+      <c r="C42" s="39" t="s">
         <v>733</v>
-      </c>
-      <c r="C42" s="39" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="27" t="s">
+        <v>734</v>
+      </c>
+      <c r="C43" s="43" t="s">
         <v>735</v>
-      </c>
-      <c r="C43" s="43" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="30">
       <c r="B44" s="38" t="s">
+        <v>736</v>
+      </c>
+      <c r="C44" s="69" t="s">
         <v>737</v>
-      </c>
-      <c r="C44" s="69" t="s">
-        <v>738</v>
       </c>
       <c r="D44" s="70"/>
     </row>

</xml_diff>

<commit_message>
added more to iptables tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C964CC90-9C09-4CD6-BC5A-6106EECCFAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC0C6EA-8C61-4964-884E-4E09F52ABA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="775">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -27444,149 +27444,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>insert</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> rule into </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>INPUT</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> chain </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>at line 1</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, anything from source 10.10.10.20 jump to DROP action (drop packet without responding to sender)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-I</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = insert rule
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-s </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= source; where the data is coming from
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-j </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= jump to (go perform this action)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">ACTIONS determine what to do with the data that matches a rule. The main actions are:
 ACCEPT: </t>
     </r>
@@ -27797,172 +27654,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> a rule to the end of a selected chain</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Append</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (attach) this new rule to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>INPUT</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> chain; anything from </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>source</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> subnet 10.10.10.0/24, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DROP</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the data'
-'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-A = </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">appends (attaches) the rule to the end of the INPUT chain
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-s = </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">source; where the data is coming from
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-j</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = jump to (go perform this action)</t>
     </r>
   </si>
   <si>
@@ -28018,6 +27709,207 @@
     </r>
   </si>
   <si>
+    <t>RESET WORKING FOLDER FILE TO LAST COMMIT</t>
+  </si>
+  <si>
+    <t>git checkout &lt;fileName&gt;</t>
+  </si>
+  <si>
+    <t>overwrite file in working folder with last local commit</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>insert</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> rule into </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chain </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>at line 1</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, anything from source 10.10.10.20 jump to DROP action (drop packet without responding to sender)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-I</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = insert rule
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-s </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= source; where the data is coming from
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-j </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= jump to (perform this action)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--dport {port|port protocol}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>destination</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> port; use when you want a rule to apply to a specific port</t>
+    </r>
+  </si>
+  <si>
+    <t>sudo iptables -A INPUT -p tcp --dport 22 -j DROP
+-or-
+sudo iptables -A INPUT -p tcp --dport ssh -j DROP</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -28144,7 +28036,31 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">-p </t>
+      <t>-A =</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> append; add to the end of the specified chain</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-p </t>
     </r>
     <r>
       <rPr>
@@ -28203,8 +28119,485 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = jump to (go perform this action)</t>
-    </r>
+      <t xml:space="preserve"> = jump to (perform this action)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>append</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> new rule to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chain, any </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TCP</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> traffic destined for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>port 22 (SSH)</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DROP</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the data
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= append; add to the end of the specified chain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-p </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= protocol; match on the following protocol value
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--dport</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = destination port; match on data destined to this port
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-s </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= source; where the data is coming from
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-j </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= jump to (perform this action)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Append</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (attach) this new rule to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> chain; anything from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>source</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> subnet 10.10.10.0/24, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DROP</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the data'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-A = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">appends (attaches) the rule to the end of the INPUT chain
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-s = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">source; where the data is coming from
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-j</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = jump to (perform this action)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-m {&lt;moduleName&gt;}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>match</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; compare the data to an iptables module and determine if it matches</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'man iptables-extensions' will give you a list of available modules you can match on</t>
+    </r>
+  </si>
+  <si>
+    <t>sudo iptables -A INPUT -p tcp --dport 22 -s 10.10.10.10 -m state --state NEW,ESTABLISHED -j ACCEPT</t>
   </si>
 </sst>
 </file>
@@ -32206,10 +32599,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
-  <dimension ref="B3:D15"/>
+  <dimension ref="B3:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -32234,13 +32627,13 @@
     </row>
     <row r="5" spans="2:4" ht="75" customHeight="1">
       <c r="C5" s="69" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D5" s="69"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
       <c r="C6" s="69" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D6" s="69"/>
     </row>
@@ -32252,13 +32645,13 @@
     </row>
     <row r="9" spans="2:4" ht="75" customHeight="1">
       <c r="B9" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>760</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>762</v>
-      </c>
       <c r="D9" s="26" t="s">
-        <v>761</v>
+        <v>771</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="30">
@@ -32302,7 +32695,7 @@
         <v>749</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>756</v>
+        <v>766</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30">
@@ -32313,18 +32706,40 @@
         <v>753</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="75">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="90">
       <c r="B15" s="8" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>765</v>
+        <v>769</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="105" customHeight="1">
+      <c r="B16" s="8" t="s">
+        <v>767</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>768</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="60">
+      <c r="B17" s="8" t="s">
+        <v>772</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>774</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>773</v>
       </c>
     </row>
   </sheetData>
@@ -32341,10 +32756,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D44"/>
+  <dimension ref="B2:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44:D44"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -32634,6 +33049,19 @@
         <v>737</v>
       </c>
       <c r="D44" s="70"/>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="60" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="27" t="s">
+        <v>765</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>764</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
added more to iptables
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D32524-7F98-4F7C-940B-BA9D60BF025C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6094E4EA-C76B-49CF-AC88-CA16D27A27DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,13 @@
     <sheet name="find" sheetId="3" r:id="rId3"/>
     <sheet name="tree" sheetId="4" r:id="rId4"/>
     <sheet name="ss" sheetId="16" r:id="rId5"/>
-    <sheet name="iptables" sheetId="22" r:id="rId6"/>
-    <sheet name="git" sheetId="18" r:id="rId7"/>
-    <sheet name="mv" sheetId="17" r:id="rId8"/>
-    <sheet name="touch" sheetId="6" r:id="rId9"/>
-    <sheet name="vi" sheetId="5" r:id="rId10"/>
-    <sheet name="nmap" sheetId="20" r:id="rId11"/>
-    <sheet name="ufw" sheetId="21" r:id="rId12"/>
+    <sheet name="git" sheetId="18" r:id="rId6"/>
+    <sheet name="mv" sheetId="17" r:id="rId7"/>
+    <sheet name="touch" sheetId="6" r:id="rId8"/>
+    <sheet name="vi" sheetId="5" r:id="rId9"/>
+    <sheet name="nmap" sheetId="20" r:id="rId10"/>
+    <sheet name="ufw" sheetId="21" r:id="rId11"/>
+    <sheet name="iptables" sheetId="22" r:id="rId12"/>
     <sheet name="tcpdump" sheetId="15" r:id="rId13"/>
     <sheet name="shells" sheetId="8" r:id="rId14"/>
     <sheet name="awk" sheetId="10" r:id="rId15"/>
@@ -29439,6 +29439,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -29465,9 +29468,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -29990,380 +29990,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CADC5F-634D-400C-ABA1-AB65FF79E0C8}">
-  <dimension ref="A1:D48"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.42578125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="28"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="34" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="57" customHeight="1">
-      <c r="A2" s="28" t="s">
-        <v>318</v>
-      </c>
-      <c r="B2" s="72" t="s">
-        <v>329</v>
-      </c>
-      <c r="C2" s="72"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="73" t="s">
-        <v>309</v>
-      </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-    </row>
-    <row r="5" spans="1:4" s="34" customFormat="1">
-      <c r="B5" s="20"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="20"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="74" t="s">
-        <v>323</v>
-      </c>
-      <c r="B6" s="74"/>
-    </row>
-    <row r="7" spans="1:4" ht="45">
-      <c r="A7" s="35" t="s">
-        <v>345</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="34" t="s">
-        <v>348</v>
-      </c>
-      <c r="B8" s="34" t="s">
-        <v>343</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="34" t="s">
-        <v>349</v>
-      </c>
-      <c r="B9" s="34" t="s">
-        <v>344</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="90">
-      <c r="A10" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C10" s="36" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="14" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="32" t="s">
-        <v>314</v>
-      </c>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="34" t="s">
-        <v>353</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>315</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="34" t="s">
-        <v>352</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>354</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30">
-      <c r="A18" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>356</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="37" t="s">
-        <v>389</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>390</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="75">
-      <c r="A20" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>370</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="71" t="s">
-        <v>317</v>
-      </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="71" t="s">
-        <v>320</v>
-      </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="71" t="s">
-        <v>324</v>
-      </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="71" t="s">
-        <v>326</v>
-      </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="71" t="s">
-        <v>328</v>
-      </c>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="71" t="s">
-        <v>330</v>
-      </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="71" t="s">
-        <v>331</v>
-      </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="72" t="s">
-        <v>332</v>
-      </c>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="72" t="s">
-        <v>340</v>
-      </c>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="71" t="s">
-        <v>341</v>
-      </c>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="71" t="s">
-        <v>342</v>
-      </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="27" t="s">
-        <v>377</v>
-      </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="27"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="27" t="s">
-        <v>378</v>
-      </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="27" t="s">
-        <v>379</v>
-      </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="27" t="s">
-        <v>381</v>
-      </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="27" t="s">
-        <v>382</v>
-      </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="27" t="s">
-        <v>383</v>
-      </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="27" t="s">
-        <v>384</v>
-      </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="27" t="s">
-        <v>385</v>
-      </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="27" t="s">
-        <v>386</v>
-      </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="27" t="s">
-        <v>387</v>
-      </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="28" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="28" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="28" t="s">
-        <v>374</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:B6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D4A975-49E6-4D67-87B6-C134DC574AA3}">
   <dimension ref="A2:M32"/>
   <sheetViews>
@@ -30435,7 +30061,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="76" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -30449,7 +30075,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="75">
-      <c r="A9" s="75"/>
+      <c r="A9" s="76"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -30461,7 +30087,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="30">
-      <c r="A10" s="75"/>
+      <c r="A10" s="76"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -30473,7 +30099,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="45">
-      <c r="A11" s="75"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -30485,7 +30111,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="45">
-      <c r="A12" s="75"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -30502,7 +30128,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="60">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="77" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -30516,7 +30142,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="75">
-      <c r="A16" s="76"/>
+      <c r="A16" s="77"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -30528,7 +30154,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="105">
-      <c r="A17" s="76"/>
+      <c r="A17" s="77"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -30540,7 +30166,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="105">
-      <c r="A18" s="76"/>
+      <c r="A18" s="77"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -30552,7 +30178,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="60">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="77" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -30566,7 +30192,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="60">
-      <c r="A20" s="76"/>
+      <c r="A20" s="77"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -30578,7 +30204,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="105">
-      <c r="A21" s="76"/>
+      <c r="A21" s="77"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -30590,7 +30216,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="60">
-      <c r="A22" s="76"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -30773,7 +30399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BA1D3C-99B5-45E1-9627-8CE6B2A3AF89}">
   <dimension ref="B3:D31"/>
   <sheetViews>
@@ -30939,38 +30565,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="78" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="77"/>
+      <c r="D19" s="78"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="78" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="77"/>
+      <c r="D20" s="78"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="78" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="77"/>
+      <c r="D21" s="78"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="78" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="77"/>
+      <c r="D22" s="78"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="78" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="77"/>
+      <c r="D23" s="78"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -30983,38 +30609,38 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="78" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="77"/>
+      <c r="D25" s="78"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="77" t="s">
+      <c r="C26" s="78" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="77"/>
+      <c r="D26" s="78"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="77" t="s">
+      <c r="C27" s="78" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="77"/>
+      <c r="D27" s="78"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="77" t="s">
+      <c r="C28" s="78" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="77"/>
+      <c r="D28" s="78"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="78" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="77"/>
+      <c r="D29" s="78"/>
     </row>
     <row r="30" spans="2:4" ht="38.25">
       <c r="B30" s="27" t="s">
@@ -31048,6 +30674,172 @@
     <mergeCell ref="C25:D25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
+  <dimension ref="B3:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="27"/>
+    <col min="2" max="2" width="43.7109375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4">
+      <c r="B3" s="43" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="120" customHeight="1">
+      <c r="C4" s="69" t="s">
+        <v>726</v>
+      </c>
+      <c r="D4" s="69"/>
+    </row>
+    <row r="5" spans="2:4" ht="75" customHeight="1">
+      <c r="C5" s="69" t="s">
+        <v>758</v>
+      </c>
+      <c r="D5" s="69"/>
+    </row>
+    <row r="6" spans="2:4" ht="90" customHeight="1">
+      <c r="C6" s="69" t="s">
+        <v>756</v>
+      </c>
+      <c r="D6" s="69"/>
+    </row>
+    <row r="7" spans="2:4" ht="75" customHeight="1">
+      <c r="C7" s="69" t="s">
+        <v>746</v>
+      </c>
+      <c r="D7" s="69"/>
+    </row>
+    <row r="9" spans="2:4" ht="75" customHeight="1">
+      <c r="B9" s="8" t="s">
+        <v>759</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30">
+      <c r="B10" s="45" t="s">
+        <v>724</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>747</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="75">
+      <c r="B11" s="8" t="s">
+        <v>745</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="60">
+      <c r="B12" s="10" t="s">
+        <v>727</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="90">
+      <c r="B13" s="8" t="s">
+        <v>751</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="30">
+      <c r="B14" s="46" t="s">
+        <v>752</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="90">
+      <c r="B15" s="8" t="s">
+        <v>762</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="105" customHeight="1">
+      <c r="B16" s="8" t="s">
+        <v>767</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>768</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="180" customHeight="1">
+      <c r="B17" s="8" t="s">
+        <v>772</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>774</v>
+      </c>
+      <c r="E17" s="70" t="s">
+        <v>773</v>
+      </c>
+      <c r="F17" s="67"/>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E17:J17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -31403,12 +31195,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -31416,11 +31208,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="72" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -31438,19 +31230,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="79" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="78"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="79" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="78"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -33077,177 +32869,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
-  <dimension ref="B3:J17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="27"/>
-    <col min="2" max="2" width="43.7109375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="27"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:4">
-      <c r="B3" s="43" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="69" t="s">
-        <v>726</v>
-      </c>
-      <c r="D4" s="69"/>
-    </row>
-    <row r="5" spans="2:4" ht="75" customHeight="1">
-      <c r="C5" s="69" t="s">
-        <v>758</v>
-      </c>
-      <c r="D5" s="69"/>
-    </row>
-    <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="69" t="s">
-        <v>756</v>
-      </c>
-      <c r="D6" s="69"/>
-    </row>
-    <row r="7" spans="2:4" ht="75" customHeight="1">
-      <c r="C7" s="69" t="s">
-        <v>746</v>
-      </c>
-      <c r="D7" s="69"/>
-    </row>
-    <row r="9" spans="2:4" ht="75" customHeight="1">
-      <c r="B9" s="8" t="s">
-        <v>759</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>760</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="30">
-      <c r="B10" s="45" t="s">
-        <v>724</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>747</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="75">
-      <c r="B11" s="8" t="s">
-        <v>745</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>750</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="60">
-      <c r="B12" s="10" t="s">
-        <v>727</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>748</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="90">
-      <c r="B13" s="8" t="s">
-        <v>751</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="30">
-      <c r="B14" s="46" t="s">
-        <v>752</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="90">
-      <c r="B15" s="8" t="s">
-        <v>762</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="105" customHeight="1">
-      <c r="B16" s="8" t="s">
-        <v>767</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>768</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="180" customHeight="1">
-      <c r="B17" s="8" t="s">
-        <v>772</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>775</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>774</v>
-      </c>
-      <c r="E17" s="79" t="s">
-        <v>773</v>
-      </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E17:J17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
   <dimension ref="B2:D48"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -33536,7 +33162,7 @@
       <c r="C44" s="69" t="s">
         <v>737</v>
       </c>
-      <c r="D44" s="70"/>
+      <c r="D44" s="71"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="60" t="s">
@@ -33560,7 +33186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49AC9E2A-F2F8-4B6A-A51F-5B422B308701}">
   <dimension ref="B2:D11"/>
   <sheetViews>
@@ -33628,7 +33254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783B63B9-C5EF-4E1E-9ABB-91855341E3A8}">
   <dimension ref="A2:C10"/>
   <sheetViews>
@@ -33701,4 +33327,378 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CADC5F-634D-400C-ABA1-AB65FF79E0C8}">
+  <dimension ref="A1:D48"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="34" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57" customHeight="1">
+      <c r="A2" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" s="73"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="74" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+    </row>
+    <row r="5" spans="1:4" s="34" customFormat="1">
+      <c r="B5" s="20"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="75" t="s">
+        <v>323</v>
+      </c>
+      <c r="B6" s="75"/>
+    </row>
+    <row r="7" spans="1:4" ht="45">
+      <c r="A7" s="35" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="90">
+      <c r="A10" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="14" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30">
+      <c r="A18" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="37" t="s">
+        <v>389</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>390</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="75">
+      <c r="A20" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>370</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="72" t="s">
+        <v>317</v>
+      </c>
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="72" t="s">
+        <v>320</v>
+      </c>
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="72" t="s">
+        <v>324</v>
+      </c>
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="72" t="s">
+        <v>326</v>
+      </c>
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="72" t="s">
+        <v>327</v>
+      </c>
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="72" t="s">
+        <v>328</v>
+      </c>
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="72" t="s">
+        <v>330</v>
+      </c>
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="72" t="s">
+        <v>331</v>
+      </c>
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="73" t="s">
+        <v>332</v>
+      </c>
+      <c r="B30" s="73"/>
+      <c r="C30" s="73"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="73" t="s">
+        <v>340</v>
+      </c>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="72" t="s">
+        <v>341</v>
+      </c>
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="27" t="s">
+        <v>381</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="27" t="s">
+        <v>383</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="B42" s="27"/>
+      <c r="C42" s="27"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="27" t="s">
+        <v>387</v>
+      </c>
+      <c r="B44" s="27"/>
+      <c r="C44" s="27"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="28" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="28" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="28" t="s">
+        <v>374</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fleshed out 'rcvmss' for 'ss -i' option
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6094E4EA-C76B-49CF-AC88-CA16D27A27DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB21A34-7917-4880-8815-AD71459554E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -26556,225 +26556,6 @@
     <t>follow prompts, select "Push an existing local repo to GitHub"</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ss</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = socket statistics
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-i</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = show internal TCP information
-format: &lt;congestion_algorithm&gt;, wscale:&lt;snd&gt;:&lt;rcv&gt;, rto: &lt;value&gt;, rtt: &lt;value&gt;/&lt;avg deviation&gt;, mss: &lt;value&gt;, pmtu: &lt;value&gt;, </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>cubic:</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> if you see this, this is the socket's congestion algorithm (algorithm that makes sure clients/servers don't send too much data at once)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">wscale:&lt;snd&gt;:&lt;rcv&gt;: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">window scale; client/server must agree on how many segments (chunks of data) to send/receive at one time
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">rto: &lt;value&gt;: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> value is in millseconds; TCP starts timer when outbound segment is handed to IP layer. If no 'ack' is received for the data in a given segment before the timer expires, the segment is retransmitted
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>rtt: &lt;value&gt;/&lt;avg deviation&gt;:</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> average round trip time in milliseconds (from client to server and back again); The first value is the avg round trip time, the second value is the avg deviation from the from the average round trip time
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>mss: &lt;value&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: maximum segment size; the largest segment the local host will accept
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">pmtu: &lt;value&gt;: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">path MTU value; path MTU is the largest packet size that can traverse this path without suffering fragmentation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>note 1:</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 'segment' is the Protocol Data Unit (PDU) at the Transport layer (layer 4)</t>
-    </r>
-  </si>
-  <si>
     <t>linux 'iptables'</t>
   </si>
   <si>
@@ -29074,6 +28855,572 @@
     <t>sudo iptables -A INPUT  -s 10.10.10.10 -m state --state NEW,ESTABLISHED -j ACCEPT
 -and-
 sudo iptables -A OUTPUT -d 10.10.10.10 -m state --state ESTABLISHED -j ACCEPT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ss</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = socket statistics
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-i</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = show internal TCP information
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>format:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+&lt;congestion_algorithm&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wscale:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;snd&gt;:&lt;rcv&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rto:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;value&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rtt:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;value&gt;/&lt;avg deviation&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mss:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;value&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pmtu:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;value&gt;, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rcvmss:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;value&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cubic:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if you see this, this is the socket's congestion algorithm (algorithm that makes sure clients/servers don't send too much data at once)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wscale:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;snd&gt;:&lt;rcv&gt;:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> window scale;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> client/server must agree on how many segments (chunks of data) to send/receive at one time
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">rto: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;value&gt;:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>retransmission timeout</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> value is in millseconds; TCP starts timer when outbound segment is handed to IP layer. If no 'ack' is received for the data in a given segment before the timer expires, the segment is retransmitted
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">rtt: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;value&gt;/&lt;avg deviation&gt;: average </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>round trip time</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in milliseconds (from client to server and back again); The first value is the avg round trip time, the second value is the avg deviation from the from the average round trip time
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">mss: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;value&gt;: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>maximum segment size;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the largest segment the local host will accept
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pmtu: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;value&gt;: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>path maximum transmission unit</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> value; path MTU is the largest packet size that can traverse this path without suffering fragmentation
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">rcvmss: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">&lt;value&gt;: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>receive maximum segment size</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, in bytes, announced to peer nodes
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>note 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'segment' is the Protocol Data Unit (PDU) at the Transport layer (layer 4)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -29439,9 +29786,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -29465,6 +29809,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -29790,11 +30137,11 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -29829,7 +30176,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="29">
       <c r="A8" s="7" t="s">
         <v>63</v>
       </c>
@@ -29840,7 +30187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="165">
+    <row r="9" spans="1:3" ht="159.5">
       <c r="A9" s="7" t="s">
         <v>66</v>
       </c>
@@ -29851,7 +30198,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="59.45" customHeight="1">
+    <row r="10" spans="1:3" ht="59.5" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>82</v>
       </c>
@@ -29862,7 +30209,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="60">
+    <row r="11" spans="1:3" ht="58">
       <c r="A11" s="8" t="s">
         <v>67</v>
       </c>
@@ -29873,7 +30220,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="60">
+    <row r="12" spans="1:3" ht="58">
       <c r="A12" s="8" t="s">
         <v>68</v>
       </c>
@@ -29895,7 +30242,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30">
+    <row r="14" spans="1:3">
       <c r="A14" s="8" t="s">
         <v>170</v>
       </c>
@@ -29906,7 +30253,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30">
+    <row r="15" spans="1:3" ht="29">
       <c r="A15" s="8" t="s">
         <v>169</v>
       </c>
@@ -29939,7 +30286,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="8" t="s">
         <v>78</v>
       </c>
@@ -29993,15 +30340,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D4A975-49E6-4D67-87B6-C134DC574AA3}">
   <dimension ref="A2:M32"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="4" width="55.7109375" customWidth="1"/>
-    <col min="5" max="5" width="59.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="4" width="55.7265625" customWidth="1"/>
+    <col min="5" max="5" width="59.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
@@ -30011,7 +30358,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="120">
+    <row r="3" spans="1:13" ht="101.5">
       <c r="A3" s="28"/>
       <c r="B3" s="3"/>
       <c r="C3" s="39" t="s">
@@ -30061,7 +30408,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="75" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -30074,8 +30421,8 @@
         <v>399</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="75">
-      <c r="A9" s="76"/>
+    <row r="9" spans="1:13" ht="72.5">
+      <c r="A9" s="75"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -30086,8 +30433,8 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="30">
-      <c r="A10" s="76"/>
+    <row r="10" spans="1:13" ht="29">
+      <c r="A10" s="75"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -30098,8 +30445,8 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45">
-      <c r="A11" s="76"/>
+    <row r="11" spans="1:13" ht="43.5">
+      <c r="A11" s="75"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -30110,8 +30457,8 @@
         <v>516</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="45">
-      <c r="A12" s="76"/>
+    <row r="12" spans="1:13" ht="43.5">
+      <c r="A12" s="75"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -30127,8 +30474,8 @@
       <c r="C14" s="9"/>
       <c r="D14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="60">
-      <c r="A15" s="77" t="s">
+    <row r="15" spans="1:13" ht="43.5">
+      <c r="A15" s="76" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -30141,8 +30488,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="75">
-      <c r="A16" s="77"/>
+    <row r="16" spans="1:13" ht="72.5">
+      <c r="A16" s="76"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -30153,8 +30500,8 @@
         <v>523</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="105">
-      <c r="A17" s="77"/>
+    <row r="17" spans="1:13" ht="87">
+      <c r="A17" s="76"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -30165,8 +30512,8 @@
         <v>524</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="105">
-      <c r="A18" s="77"/>
+    <row r="18" spans="1:13" ht="87">
+      <c r="A18" s="76"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -30177,8 +30524,8 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="60">
-      <c r="A19" s="77" t="s">
+    <row r="19" spans="1:13" ht="58">
+      <c r="A19" s="76" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -30191,8 +30538,8 @@
         <v>526</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="60">
-      <c r="A20" s="77"/>
+    <row r="20" spans="1:13" ht="58">
+      <c r="A20" s="76"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -30203,8 +30550,8 @@
         <v>529</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="105">
-      <c r="A21" s="77"/>
+    <row r="21" spans="1:13" ht="101.5">
+      <c r="A21" s="76"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -30215,8 +30562,8 @@
         <v>541</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="60">
-      <c r="A22" s="77"/>
+    <row r="22" spans="1:13" ht="58">
+      <c r="A22" s="76"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -30249,7 +30596,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:13" ht="150">
+    <row r="25" spans="1:13" ht="130.5">
       <c r="B25" s="11" t="s">
         <v>538</v>
       </c>
@@ -30271,7 +30618,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" ht="150">
+    <row r="26" spans="1:13" ht="145">
       <c r="A26" s="28"/>
       <c r="B26" s="11" t="s">
         <v>629</v>
@@ -30294,7 +30641,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" ht="165">
+    <row r="27" spans="1:13" ht="145">
       <c r="B27" s="11" t="s">
         <v>632</v>
       </c>
@@ -30314,7 +30661,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" ht="200.1" customHeight="1">
+    <row r="28" spans="1:13" ht="200.15" customHeight="1">
       <c r="B28" s="11" t="s">
         <v>635</v>
       </c>
@@ -30350,7 +30697,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="210.95" customHeight="1">
+    <row r="30" spans="1:13" ht="211" customHeight="1">
       <c r="B30" s="11" t="s">
         <v>643</v>
       </c>
@@ -30364,7 +30711,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="270">
+    <row r="31" spans="1:13" ht="232">
       <c r="B31" s="11" t="s">
         <v>647</v>
       </c>
@@ -30378,7 +30725,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="75">
+    <row r="32" spans="1:13" ht="72.5">
       <c r="B32" s="11" t="s">
         <v>651</v>
       </c>
@@ -30407,10 +30754,10 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="4" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.7265625" customWidth="1"/>
+    <col min="3" max="4" width="53.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
@@ -30565,38 +30912,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="78" t="s">
+      <c r="C19" s="77" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="78"/>
+      <c r="D19" s="77"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="77" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="78"/>
+      <c r="D20" s="77"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="78" t="s">
+      <c r="C21" s="77" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="78"/>
+      <c r="D21" s="77"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="77" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="78"/>
+      <c r="D22" s="77"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="78" t="s">
+      <c r="C23" s="77" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="78"/>
+      <c r="D23" s="77"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -30609,40 +30956,40 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="78" t="s">
+      <c r="C25" s="77" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="78"/>
+      <c r="D25" s="77"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="78" t="s">
+      <c r="C26" s="77" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="78"/>
+      <c r="D26" s="77"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="77" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="78"/>
+      <c r="D27" s="77"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="78" t="s">
+      <c r="C28" s="77" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="78"/>
+      <c r="D28" s="77"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="78" t="s">
+      <c r="C29" s="77" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="78"/>
-    </row>
-    <row r="30" spans="2:4" ht="38.25">
+      <c r="D29" s="77"/>
+    </row>
+    <row r="30" spans="2:4" ht="39">
       <c r="B30" s="27" t="s">
         <v>701</v>
       </c>
@@ -30681,148 +31028,148 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
   <dimension ref="B3:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="27"/>
-    <col min="2" max="2" width="43.7109375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="51.85546875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="1" width="9.1796875" style="27"/>
+    <col min="2" max="2" width="43.7265625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="51.81640625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.7265625" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" s="43" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
       <c r="C4" s="69" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D4" s="69"/>
     </row>
     <row r="5" spans="2:4" ht="75" customHeight="1">
       <c r="C5" s="69" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="D5" s="69"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
       <c r="C6" s="69" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="D6" s="69"/>
     </row>
     <row r="7" spans="2:4" ht="75" customHeight="1">
       <c r="C7" s="69" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D7" s="69"/>
     </row>
     <row r="9" spans="2:4" ht="75" customHeight="1">
       <c r="B9" s="8" t="s">
+        <v>757</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>758</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="29">
+      <c r="B10" s="45" t="s">
+        <v>722</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>745</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="72.5">
+      <c r="B11" s="8" t="s">
+        <v>743</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="58">
+      <c r="B12" s="10" t="s">
+        <v>725</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>746</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="87">
+      <c r="B13" s="8" t="s">
+        <v>749</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="29">
+      <c r="B14" s="46" t="s">
+        <v>750</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="87">
+      <c r="B15" s="8" t="s">
+        <v>760</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>760</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="30">
-      <c r="B10" s="45" t="s">
-        <v>724</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>747</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="75">
-      <c r="B11" s="8" t="s">
-        <v>745</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>750</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="60">
-      <c r="B12" s="10" t="s">
-        <v>727</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>748</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="90">
-      <c r="B13" s="8" t="s">
-        <v>751</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>749</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="30">
-      <c r="B14" s="46" t="s">
-        <v>752</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>753</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="90">
-      <c r="B15" s="8" t="s">
-        <v>762</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>761</v>
-      </c>
       <c r="D15" s="19" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="105" customHeight="1">
       <c r="B16" s="8" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>766</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>768</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="180" customHeight="1">
       <c r="B17" s="8" t="s">
+        <v>770</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>773</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>772</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>775</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>774</v>
-      </c>
-      <c r="E17" s="70" t="s">
-        <v>773</v>
+      <c r="E17" s="78" t="s">
+        <v>771</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="67"/>
@@ -30851,16 +31198,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="27"/>
-    <col min="2" max="2" width="43.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="27" customWidth="1"/>
-    <col min="5" max="5" width="34.42578125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="42.42578125" style="27" customWidth="1"/>
-    <col min="7" max="8" width="40.5703125" style="27" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="8.81640625" style="27"/>
+    <col min="2" max="2" width="43.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="27" customWidth="1"/>
+    <col min="5" max="5" width="34.453125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="42.453125" style="27" customWidth="1"/>
+    <col min="7" max="8" width="40.54296875" style="27" customWidth="1"/>
+    <col min="9" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -30873,7 +31220,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="29.45" customHeight="1">
+    <row r="5" spans="2:8" ht="29.5" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>466</v>
       </c>
@@ -30897,7 +31244,7 @@
       </c>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="2:8" ht="29.1" customHeight="1">
+    <row r="7" spans="2:8" ht="29.15" customHeight="1">
       <c r="C7" s="27" t="s">
         <v>465</v>
       </c>
@@ -30906,7 +31253,7 @@
       </c>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="2:8" ht="45">
+    <row r="8" spans="2:8" ht="43.5">
       <c r="C8" s="27" t="s">
         <v>467</v>
       </c>
@@ -30923,7 +31270,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="2:8" ht="30">
+    <row r="11" spans="2:8" ht="29">
       <c r="B11" s="10" t="s">
         <v>477</v>
       </c>
@@ -30935,7 +31282,7 @@
       </c>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="2:8" ht="115.35" customHeight="1">
+    <row r="12" spans="2:8" ht="115.4" customHeight="1">
       <c r="B12" s="10" t="s">
         <v>472</v>
       </c>
@@ -30947,7 +31294,7 @@
       </c>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="2:8" ht="45">
+    <row r="13" spans="2:8" ht="43.5">
       <c r="B13" s="46" t="s">
         <v>459</v>
       </c>
@@ -30959,7 +31306,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="2:8" ht="30">
+    <row r="14" spans="2:8" ht="29">
       <c r="B14" s="46" t="s">
         <v>478</v>
       </c>
@@ -30971,7 +31318,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="2:8" ht="101.1" customHeight="1">
+    <row r="15" spans="2:8" ht="101.15" customHeight="1">
       <c r="B15" s="8" t="s">
         <v>481</v>
       </c>
@@ -30983,7 +31330,7 @@
       </c>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="2:8" ht="75">
+    <row r="16" spans="2:8" ht="72.5">
       <c r="B16" s="8" t="s">
         <v>495</v>
       </c>
@@ -31006,7 +31353,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="90">
+    <row r="17" spans="2:8" ht="58">
       <c r="B17" s="8" t="s">
         <v>494</v>
       </c>
@@ -31021,7 +31368,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="2:8" ht="45">
+    <row r="18" spans="2:8" ht="43.5">
       <c r="B18" s="8" t="s">
         <v>491</v>
       </c>
@@ -31036,7 +31383,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="2:8" ht="75">
+    <row r="19" spans="2:8" ht="72.5">
       <c r="B19" s="8" t="s">
         <v>496</v>
       </c>
@@ -31051,7 +31398,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="2:8" ht="120">
+    <row r="20" spans="2:8" ht="116">
       <c r="B20" s="8" t="s">
         <v>501</v>
       </c>
@@ -31068,7 +31415,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="2:8" ht="43.35" customHeight="1">
+    <row r="21" spans="2:8" ht="43.4" customHeight="1">
       <c r="B21" s="8" t="s">
         <v>504</v>
       </c>
@@ -31083,7 +31430,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="2:8" ht="90">
+    <row r="22" spans="2:8" ht="87">
       <c r="B22" s="8" t="s">
         <v>510</v>
       </c>
@@ -31098,7 +31445,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="2:8" ht="30">
+    <row r="23" spans="2:8">
       <c r="B23" s="8" t="s">
         <v>543</v>
       </c>
@@ -31127,7 +31474,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="2:8" ht="30">
+    <row r="26" spans="2:8" ht="29">
       <c r="B26" s="10" t="s">
         <v>505</v>
       </c>
@@ -31163,7 +31510,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="2:8" ht="30">
+    <row r="30" spans="2:8" ht="29">
       <c r="B30" s="46" t="s">
         <v>509</v>
       </c>
@@ -31174,7 +31521,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="14.45" customHeight="1"/>
+    <row r="32" spans="2:8" ht="14.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4294967295" r:id="rId1"/>
@@ -31189,9 +31536,9 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
@@ -31208,11 +31555,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="71" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -31266,12 +31613,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="16.453125" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -31279,13 +31626,13 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="29">
       <c r="B4" s="39" t="s">
         <v>419</v>
       </c>
       <c r="C4" s="38"/>
     </row>
-    <row r="6" spans="1:3" ht="90">
+    <row r="6" spans="1:3" ht="87">
       <c r="A6" s="44" t="s">
         <v>420</v>
       </c>
@@ -31310,12 +31657,12 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -31328,7 +31675,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>430</v>
       </c>
@@ -31363,12 +31710,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -31381,7 +31728,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>438</v>
       </c>
@@ -31392,7 +31739,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="46" t="s">
         <v>441</v>
       </c>
@@ -31416,12 +31763,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="38" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" style="38" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="38" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="38"/>
+    <col min="1" max="1" width="23.54296875" style="38" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="38" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="38"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -31429,12 +31776,12 @@
         <v>444</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="29">
       <c r="B4" s="39" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>446</v>
       </c>
@@ -31445,7 +31792,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="46" t="s">
         <v>448</v>
       </c>
@@ -31469,12 +31816,12 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="43.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -31482,12 +31829,12 @@
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45">
+    <row r="4" spans="1:3" ht="43.5">
       <c r="B4" s="39" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="29">
       <c r="A6" s="46" t="s">
         <v>426</v>
       </c>
@@ -31511,12 +31858,12 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.453125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="63.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -31525,7 +31872,7 @@
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="43.5">
       <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
@@ -31546,7 +31893,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="45">
+    <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -31558,7 +31905,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="45">
+    <row r="8" spans="1:4" ht="43.5">
       <c r="A8" s="7" t="s">
         <v>87</v>
       </c>
@@ -31570,7 +31917,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="90">
+    <row r="9" spans="1:4" ht="72.5">
       <c r="A9" s="8" t="s">
         <v>269</v>
       </c>
@@ -31582,7 +31929,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="45">
+    <row r="10" spans="1:4" ht="43.5">
       <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
@@ -31594,7 +31941,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="75">
+    <row r="11" spans="1:4" ht="58">
       <c r="A11" s="8" t="s">
         <v>264</v>
       </c>
@@ -31606,7 +31953,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" s="12" customFormat="1" ht="45">
+    <row r="12" spans="1:4" s="12" customFormat="1" ht="43.5">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -31618,7 +31965,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" s="12" customFormat="1" ht="45">
+    <row r="13" spans="1:4" s="12" customFormat="1" ht="43.5">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -31630,7 +31977,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="45">
+    <row r="14" spans="1:4" ht="43.5">
       <c r="A14" s="8" t="s">
         <v>275</v>
       </c>
@@ -31642,7 +31989,7 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" ht="45">
+    <row r="15" spans="1:4" s="3" customFormat="1" ht="43.5">
       <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
@@ -31654,7 +32001,7 @@
       </c>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" ht="45">
+    <row r="16" spans="1:4" ht="43.5">
       <c r="A16" s="8" t="s">
         <v>218</v>
       </c>
@@ -31666,7 +32013,7 @@
       </c>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="60">
+    <row r="17" spans="1:4" ht="43.5">
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
@@ -31678,7 +32025,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="60">
+    <row r="18" spans="1:4" ht="43.5">
       <c r="A18" s="7" t="s">
         <v>21</v>
       </c>
@@ -31690,7 +32037,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="75">
+    <row r="19" spans="1:4" ht="72.5">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -31702,7 +32049,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="90">
+    <row r="20" spans="1:4" ht="87">
       <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
@@ -31714,7 +32061,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" ht="60">
+    <row r="21" spans="1:4" ht="58">
       <c r="A21" s="30" t="s">
         <v>224</v>
       </c>
@@ -31726,7 +32073,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="30">
+    <row r="22" spans="1:4" ht="29">
       <c r="A22" s="12" t="s">
         <v>22</v>
       </c>
@@ -31738,7 +32085,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" ht="30">
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="29">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -31760,7 +32107,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="75">
+    <row r="25" spans="1:4" ht="72.5">
       <c r="A25" s="8" t="s">
         <v>227</v>
       </c>
@@ -31772,7 +32119,7 @@
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" ht="120">
+    <row r="26" spans="1:4" ht="87">
       <c r="A26" s="6" t="s">
         <v>229</v>
       </c>
@@ -31784,7 +32131,7 @@
       </c>
       <c r="D26" s="12"/>
     </row>
-    <row r="27" spans="1:4" ht="60">
+    <row r="27" spans="1:4" ht="58">
       <c r="A27" s="6" t="s">
         <v>231</v>
       </c>
@@ -31832,11 +32179,11 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.54296875" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
@@ -31858,7 +32205,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="45">
+    <row r="5" spans="1:6" ht="43.5">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -31869,7 +32216,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45">
+    <row r="6" spans="1:6" ht="43.5">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -31880,7 +32227,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60">
+    <row r="7" spans="1:6" ht="58">
       <c r="A7" s="6" t="s">
         <v>104</v>
       </c>
@@ -31891,7 +32238,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45">
+    <row r="8" spans="1:6" ht="43.5">
       <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
@@ -31905,7 +32252,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="195">
+    <row r="9" spans="1:6" ht="174">
       <c r="A9" s="8" t="s">
         <v>119</v>
       </c>
@@ -31916,7 +32263,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45">
+    <row r="10" spans="1:6" ht="43.5">
       <c r="A10" s="8" t="s">
         <v>90</v>
       </c>
@@ -31927,7 +32274,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="75">
+    <row r="11" spans="1:6" ht="72.5">
       <c r="A11" s="8" t="s">
         <v>92</v>
       </c>
@@ -31938,7 +32285,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60">
+    <row r="12" spans="1:6" ht="58">
       <c r="A12" s="8" t="s">
         <v>93</v>
       </c>
@@ -31949,7 +32296,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="75">
+    <row r="13" spans="1:6" ht="72.5">
       <c r="A13" s="8" t="s">
         <v>97</v>
       </c>
@@ -31960,7 +32307,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="90">
+    <row r="14" spans="1:6" ht="72.5">
       <c r="A14" s="8" t="s">
         <v>98</v>
       </c>
@@ -31971,7 +32318,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60">
+    <row r="15" spans="1:6" ht="58">
       <c r="A15" s="8" t="s">
         <v>99</v>
       </c>
@@ -31982,7 +32329,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="90">
+    <row r="16" spans="1:6" ht="87">
       <c r="A16" s="8" t="s">
         <v>103</v>
       </c>
@@ -31993,7 +32340,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="75">
+    <row r="17" spans="1:3" ht="72.5">
       <c r="A17" s="8" t="s">
         <v>101</v>
       </c>
@@ -32004,7 +32351,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="105">
+    <row r="18" spans="1:3" ht="87">
       <c r="A18" s="8" t="s">
         <v>196</v>
       </c>
@@ -32015,7 +32362,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="90">
+    <row r="19" spans="1:3" ht="87">
       <c r="A19" s="8" t="s">
         <v>102</v>
       </c>
@@ -32026,7 +32373,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="60">
+    <row r="20" spans="1:3" ht="43.5">
       <c r="A20" s="8" t="s">
         <v>203</v>
       </c>
@@ -32037,7 +32384,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="90">
+    <row r="21" spans="1:3" ht="87">
       <c r="A21" s="8" t="s">
         <v>106</v>
       </c>
@@ -32048,7 +32395,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="8" t="s">
         <v>108</v>
       </c>
@@ -32059,7 +32406,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="90">
+    <row r="23" spans="1:3" ht="87">
       <c r="A23" s="8" t="s">
         <v>109</v>
       </c>
@@ -32070,7 +32417,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="105">
+    <row r="24" spans="1:3" ht="87">
       <c r="A24" s="8" t="s">
         <v>110</v>
       </c>
@@ -32092,7 +32439,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="90">
+    <row r="26" spans="1:3" ht="72.5">
       <c r="A26" s="8" t="s">
         <v>111</v>
       </c>
@@ -32103,7 +32450,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="90">
+    <row r="27" spans="1:3" ht="87">
       <c r="A27" s="8" t="s">
         <v>113</v>
       </c>
@@ -32114,7 +32461,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="75">
+    <row r="28" spans="1:3" ht="72.5">
       <c r="A28" s="8" t="s">
         <v>114</v>
       </c>
@@ -32125,7 +32472,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="120">
+    <row r="29" spans="1:3" ht="116">
       <c r="A29" s="8" t="s">
         <v>115</v>
       </c>
@@ -32136,7 +32483,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="195">
+    <row r="30" spans="1:3" ht="174">
       <c r="A30" s="6" t="s">
         <v>116</v>
       </c>
@@ -32147,7 +32494,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="210">
+    <row r="31" spans="1:3" ht="159.5">
       <c r="A31" s="6" t="s">
         <v>117</v>
       </c>
@@ -32158,7 +32505,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="240">
+    <row r="32" spans="1:3" ht="203">
       <c r="A32" s="9" t="s">
         <v>60</v>
       </c>
@@ -32194,11 +32541,11 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -32223,7 +32570,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="27"/>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="29">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -32234,7 +32581,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="60">
+    <row r="6" spans="1:3" ht="43.5">
       <c r="A6" s="3" t="s">
         <v>135</v>
       </c>
@@ -32245,7 +32592,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="29">
       <c r="A7" s="10" t="s">
         <v>136</v>
       </c>
@@ -32256,7 +32603,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30">
+    <row r="8" spans="1:3" ht="29">
       <c r="A8" s="10" t="s">
         <v>139</v>
       </c>
@@ -32267,7 +32614,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="45">
+    <row r="9" spans="1:3" ht="43.5">
       <c r="A9" s="10" t="s">
         <v>140</v>
       </c>
@@ -32278,7 +32625,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45">
+    <row r="10" spans="1:3" ht="43.5">
       <c r="A10" s="10" t="s">
         <v>142</v>
       </c>
@@ -32300,7 +32647,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="43.5">
       <c r="A12" s="10" t="s">
         <v>152</v>
       </c>
@@ -32311,7 +32658,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45">
+    <row r="13" spans="1:3" ht="43.5">
       <c r="A13" s="8" t="s">
         <v>156</v>
       </c>
@@ -32322,7 +32669,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="43.5">
       <c r="A14" s="8" t="s">
         <v>161</v>
       </c>
@@ -32333,7 +32680,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="75">
+    <row r="15" spans="1:3" ht="72.5">
       <c r="A15" s="8" t="s">
         <v>166</v>
       </c>
@@ -32344,7 +32691,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45">
+    <row r="16" spans="1:3" ht="43.5">
       <c r="A16" s="8" t="s">
         <v>175</v>
       </c>
@@ -32355,7 +32702,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="43.5">
       <c r="A17" s="8" t="s">
         <v>177</v>
       </c>
@@ -32366,7 +32713,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45">
+    <row r="18" spans="1:3" ht="43.5">
       <c r="A18" s="8" t="s">
         <v>178</v>
       </c>
@@ -32377,7 +32724,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45">
+    <row r="19" spans="1:3" ht="43.5">
       <c r="A19" s="8" t="s">
         <v>181</v>
       </c>
@@ -32388,7 +32735,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="60">
+    <row r="20" spans="1:3" ht="58">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
@@ -32399,7 +32746,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="90">
+    <row r="21" spans="1:3" ht="72.5">
       <c r="A21" s="10" t="s">
         <v>150</v>
       </c>
@@ -32410,7 +32757,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75">
+    <row r="22" spans="1:3" ht="72.5">
       <c r="A22" s="8" t="s">
         <v>183</v>
       </c>
@@ -32421,7 +32768,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60">
+    <row r="23" spans="1:3" ht="58">
       <c r="A23" s="10" t="s">
         <v>67</v>
       </c>
@@ -32432,7 +32779,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="90">
+    <row r="24" spans="1:3" ht="87">
       <c r="A24" s="8" t="s">
         <v>186</v>
       </c>
@@ -32443,7 +32790,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="120">
+    <row r="25" spans="1:3" ht="101.5">
       <c r="A25" s="10" t="s">
         <v>232</v>
       </c>
@@ -32454,7 +32801,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="90">
+    <row r="26" spans="1:3" ht="72.5">
       <c r="A26" s="8" t="s">
         <v>234</v>
       </c>
@@ -32465,7 +32812,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="75">
+    <row r="27" spans="1:3" ht="72.5">
       <c r="A27" s="10" t="s">
         <v>236</v>
       </c>
@@ -32476,7 +32823,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="45">
+    <row r="28" spans="1:3" ht="43.5">
       <c r="A28" s="7" t="s">
         <v>240</v>
       </c>
@@ -32487,7 +32834,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="75">
+    <row r="29" spans="1:3" ht="58">
       <c r="A29" s="7" t="s">
         <v>242</v>
       </c>
@@ -32498,7 +32845,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="45.6" customHeight="1">
+    <row r="30" spans="1:3" ht="45.65" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>245</v>
       </c>
@@ -32509,7 +32856,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="45">
+    <row r="31" spans="1:3" ht="43.5">
       <c r="A31" s="7" t="s">
         <v>247</v>
       </c>
@@ -32520,7 +32867,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="45">
+    <row r="32" spans="1:3" ht="43.5">
       <c r="A32" s="7" t="s">
         <v>251</v>
       </c>
@@ -32531,7 +32878,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="45">
+    <row r="33" spans="1:3" ht="43.5">
       <c r="A33" s="8" t="s">
         <v>148</v>
       </c>
@@ -32542,7 +32889,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="60">
+    <row r="34" spans="1:3" ht="58">
       <c r="A34" s="8" t="s">
         <v>148</v>
       </c>
@@ -32631,17 +32978,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F8480C-E8CD-45AC-8F81-8D4ABFF602C5}">
   <dimension ref="B2:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:J18"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="28"/>
-    <col min="2" max="2" width="30.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="28"/>
+    <col min="1" max="1" width="8.81640625" style="28"/>
+    <col min="2" max="2" width="30.54296875" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -32649,7 +32996,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="60">
+    <row r="3" spans="2:4" ht="58">
       <c r="C3" s="37" t="s">
         <v>545</v>
       </c>
@@ -32673,7 +33020,7 @@
       <c r="B7" s="59"/>
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="2:4" ht="30">
+    <row r="8" spans="2:4" ht="29">
       <c r="B8" s="11" t="s">
         <v>560</v>
       </c>
@@ -32684,7 +33031,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30">
+    <row r="9" spans="2:4" ht="29">
       <c r="B9" s="7" t="s">
         <v>553</v>
       </c>
@@ -32695,7 +33042,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30">
+    <row r="10" spans="2:4" ht="29">
       <c r="B10" s="7" t="s">
         <v>556</v>
       </c>
@@ -32706,7 +33053,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="30">
+    <row r="11" spans="2:4" ht="29">
       <c r="B11" s="11" t="s">
         <v>559</v>
       </c>
@@ -32717,7 +33064,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="30">
+    <row r="12" spans="2:4" ht="29">
       <c r="B12" s="11" t="s">
         <v>563</v>
       </c>
@@ -32728,7 +33075,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="45">
+    <row r="13" spans="2:4" ht="43.5">
       <c r="B13" s="11" t="s">
         <v>565</v>
       </c>
@@ -32739,7 +33086,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="45">
+    <row r="14" spans="2:4" ht="43.5">
       <c r="B14" s="11" t="s">
         <v>569</v>
       </c>
@@ -32750,7 +33097,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="45">
+    <row r="15" spans="2:4" ht="43.5">
       <c r="B15" s="11" t="s">
         <v>571</v>
       </c>
@@ -32761,7 +33108,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="30">
+    <row r="16" spans="2:4" ht="29">
       <c r="B16" s="7" t="s">
         <v>574</v>
       </c>
@@ -32772,7 +33119,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="165">
+    <row r="17" spans="2:13" ht="159.5">
       <c r="B17" s="7" t="s">
         <v>578</v>
       </c>
@@ -32783,7 +33130,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="144.94999999999999" customHeight="1">
+    <row r="18" spans="2:13" ht="145" customHeight="1">
       <c r="B18" s="11" t="s">
         <v>581</v>
       </c>
@@ -32824,7 +33171,7 @@
       <c r="L19" s="67"/>
       <c r="M19" s="67"/>
     </row>
-    <row r="20" spans="2:13" ht="30">
+    <row r="20" spans="2:13" ht="29">
       <c r="B20" s="7" t="s">
         <v>589</v>
       </c>
@@ -32835,7 +33182,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="210" customHeight="1">
+    <row r="21" spans="2:13" ht="238" customHeight="1">
       <c r="B21" s="7" t="s">
         <v>592</v>
       </c>
@@ -32843,10 +33190,10 @@
         <v>593</v>
       </c>
       <c r="D21" s="66" t="s">
-        <v>721</v>
+        <v>774</v>
       </c>
       <c r="E21" s="67" t="s">
-        <v>722</v>
+        <v>775</v>
       </c>
       <c r="F21" s="67"/>
       <c r="G21" s="67"/>
@@ -32876,13 +33223,13 @@
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="27"/>
+    <col min="1" max="1" width="8.7265625" style="27"/>
     <col min="2" max="2" width="49" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="27"/>
+    <col min="3" max="3" width="43.54296875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -32968,13 +33315,13 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="27" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C14" s="43" t="s">
+        <v>736</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>738</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -32990,7 +33337,7 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" s="60" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -33009,7 +33356,7 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="60" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -33080,7 +33427,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="31" spans="2:4" ht="30">
+    <row r="31" spans="2:4" ht="29">
       <c r="B31" s="38" t="s">
         <v>714</v>
       </c>
@@ -33115,66 +33462,66 @@
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="60" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="27" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="C37" s="43" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40" s="60" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41" s="27" t="s">
+        <v>728</v>
+      </c>
+      <c r="C41" s="43" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="29">
+      <c r="B42" s="38" t="s">
         <v>730</v>
       </c>
-      <c r="C41" s="43" t="s">
+      <c r="C42" s="39" t="s">
         <v>731</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="30">
-      <c r="B42" s="38" t="s">
-        <v>732</v>
-      </c>
-      <c r="C42" s="39" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43" s="27" t="s">
+        <v>732</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="29">
+      <c r="B44" s="38" t="s">
         <v>734</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C44" s="69" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" ht="30">
-      <c r="B44" s="38" t="s">
-        <v>736</v>
-      </c>
-      <c r="C44" s="69" t="s">
-        <v>737</v>
-      </c>
-      <c r="D44" s="71"/>
+      <c r="D44" s="70"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="60" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48" s="27" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C48" s="43" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
   </sheetData>
@@ -33194,13 +33541,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="27"/>
-    <col min="2" max="2" width="30.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="52.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="27"/>
+    <col min="1" max="1" width="8.81640625" style="27"/>
+    <col min="2" max="2" width="30.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1796875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -33228,7 +33575,7 @@
       <c r="B6" s="45"/>
       <c r="C6" s="43"/>
     </row>
-    <row r="7" spans="2:4" ht="30">
+    <row r="7" spans="2:4" ht="29">
       <c r="B7" s="46" t="s">
         <v>550</v>
       </c>
@@ -33240,7 +33587,7 @@
     <row r="9" spans="2:4">
       <c r="B9" s="45"/>
     </row>
-    <row r="10" spans="2:4" ht="101.45" customHeight="1">
+    <row r="10" spans="2:4" ht="101.5" customHeight="1">
       <c r="B10" s="45"/>
       <c r="C10" s="43"/>
       <c r="D10" s="38"/>
@@ -33262,10 +33609,10 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -33304,7 +33651,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="101.45" customHeight="1">
+    <row r="9" spans="1:3" ht="101.5" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>295</v>
       </c>
@@ -33337,13 +33684,13 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="28"/>
+    <col min="1" max="1" width="30.453125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="41.453125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="48.81640625" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -33355,17 +33702,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="72" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="73"/>
+      <c r="C2" s="72"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="73" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="74"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -33373,12 +33720,12 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="74" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="75"/>
-    </row>
-    <row r="7" spans="1:4" ht="45">
+      <c r="B6" s="74"/>
+    </row>
+    <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="35" t="s">
         <v>345</v>
       </c>
@@ -33411,7 +33758,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="90">
+    <row r="10" spans="1:4" ht="72.5">
       <c r="A10" s="9" t="s">
         <v>351</v>
       </c>
@@ -33471,7 +33818,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30">
+    <row r="18" spans="1:3" ht="29">
       <c r="A18" s="4" t="s">
         <v>355</v>
       </c>
@@ -33493,7 +33840,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="75">
+    <row r="20" spans="1:3" ht="58">
       <c r="A20" s="4" t="s">
         <v>369</v>
       </c>
@@ -33505,88 +33852,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="72" t="s">
+      <c r="A22" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="72" t="s">
+      <c r="A23" s="71" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="71" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="71" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="71" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="71" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="72" t="s">
+      <c r="A28" s="71" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="72" t="s">
+      <c r="A29" s="71" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="73" t="s">
+      <c r="A30" s="72" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="73"/>
-      <c r="C30" s="73"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="73" t="s">
+      <c r="A31" s="72" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="72" t="s">
+      <c r="A32" s="71" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
+      <c r="B32" s="71"/>
+      <c r="C32" s="71"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="72" t="s">
+      <c r="A33" s="71" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
+      <c r="B33" s="71"/>
+      <c r="C33" s="71"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
added more to git tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB21A34-7917-4880-8815-AD71459554E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD119DF-C522-486F-B2F0-0576D69B35E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="776">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="782">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -29420,6 +29420,139 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 'segment' is the Protocol Data Unit (PDU) at the Transport layer (layer 4)</t>
+    </r>
+  </si>
+  <si>
+    <t>LOOKING AT GIT DIFFERENCES</t>
+  </si>
+  <si>
+    <t>git diff</t>
+  </si>
+  <si>
+    <t>show differences between file in working folder and file in local repo</t>
+  </si>
+  <si>
+    <t>Basic output guide</t>
+  </si>
+  <si>
+    <t>diff --git a/file.txt b/file.txt
+index f2aa86d..1831a89  100644
+--- a/file.txt
++++ b/file.txt
+@@ -1 +1,2 @@ 
+hello
++added text to line 2
+\ No newline at end of file</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">diff --git a/file b/file </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= comparing 2 versions of same file, 'a' and 'b'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>index f2aa86d..1831a89  100644</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = different hashes for old and new files, plus '100644' is the 'mode' of the file (what functions are allowed on the file)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">--- a/file.txt = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file version 'a' is symbolized by a '-'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
++++ b/file.txt = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">file version 'b' is symbolized by a '+'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@@ -1 +1,2 @@</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =  </t>
     </r>
   </si>
 </sst>
@@ -29587,7 +29720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -29777,6 +29910,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -29815,6 +29957,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -30408,7 +30553,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="78" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -30422,7 +30567,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="72.5">
-      <c r="A9" s="75"/>
+      <c r="A9" s="78"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -30434,7 +30579,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29">
-      <c r="A10" s="75"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -30446,7 +30591,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="43.5">
-      <c r="A11" s="75"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -30458,7 +30603,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5">
-      <c r="A12" s="75"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -30475,7 +30620,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="43.5">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="79" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -30489,7 +30634,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="72.5">
-      <c r="A16" s="76"/>
+      <c r="A16" s="79"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -30501,7 +30646,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="87">
-      <c r="A17" s="76"/>
+      <c r="A17" s="79"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -30513,7 +30658,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="87">
-      <c r="A18" s="76"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -30525,7 +30670,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="58">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="79" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -30539,7 +30684,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="58">
-      <c r="A20" s="76"/>
+      <c r="A20" s="79"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -30551,7 +30696,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="101.5">
-      <c r="A21" s="76"/>
+      <c r="A21" s="79"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -30563,7 +30708,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="58">
-      <c r="A22" s="76"/>
+      <c r="A22" s="79"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -30912,38 +31057,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="80" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="77"/>
+      <c r="D19" s="80"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="77" t="s">
+      <c r="C20" s="80" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="77"/>
+      <c r="D20" s="80"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="80" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="77"/>
+      <c r="D21" s="80"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="80" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="77"/>
+      <c r="D22" s="80"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="77" t="s">
+      <c r="C23" s="80" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="77"/>
+      <c r="D23" s="80"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -30956,38 +31101,38 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="77" t="s">
+      <c r="C25" s="80" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="77"/>
+      <c r="D25" s="80"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="77" t="s">
+      <c r="C26" s="80" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="77"/>
+      <c r="D26" s="80"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="77" t="s">
+      <c r="C27" s="80" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="77"/>
+      <c r="D27" s="80"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="77" t="s">
+      <c r="C28" s="80" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="77"/>
+      <c r="D28" s="80"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="80" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="77"/>
+      <c r="D29" s="80"/>
     </row>
     <row r="30" spans="2:4" ht="39">
       <c r="B30" s="27" t="s">
@@ -31047,28 +31192,28 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="72" t="s">
         <v>724</v>
       </c>
-      <c r="D4" s="69"/>
+      <c r="D4" s="72"/>
     </row>
     <row r="5" spans="2:4" ht="75" customHeight="1">
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="72" t="s">
         <v>756</v>
       </c>
-      <c r="D5" s="69"/>
+      <c r="D5" s="72"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="72" t="s">
         <v>754</v>
       </c>
-      <c r="D6" s="69"/>
+      <c r="D6" s="72"/>
     </row>
     <row r="7" spans="2:4" ht="75" customHeight="1">
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="72" t="s">
         <v>744</v>
       </c>
-      <c r="D7" s="69"/>
+      <c r="D7" s="72"/>
     </row>
     <row r="9" spans="2:4" ht="75" customHeight="1">
       <c r="B9" s="8" t="s">
@@ -31168,14 +31313,14 @@
       <c r="D17" s="18" t="s">
         <v>772</v>
       </c>
-      <c r="E17" s="78" t="s">
+      <c r="E17" s="81" t="s">
         <v>771</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -31542,12 +31687,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="82" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -31555,11 +31700,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="74" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -31577,19 +31722,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="79" t="s">
+      <c r="B11" s="82" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="79"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="79" t="s">
+      <c r="B12" s="82" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="79"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -32978,7 +33123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F8480C-E8CD-45AC-8F81-8D4ABFF602C5}">
   <dimension ref="B2:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
@@ -33140,14 +33285,14 @@
       <c r="D18" s="66" t="s">
         <v>583</v>
       </c>
-      <c r="E18" s="67" t="s">
+      <c r="E18" s="70" t="s">
         <v>584</v>
       </c>
-      <c r="F18" s="68"/>
-      <c r="G18" s="68"/>
-      <c r="H18" s="68"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="68"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -33159,17 +33304,17 @@
       <c r="D19" s="66" t="s">
         <v>587</v>
       </c>
-      <c r="E19" s="67" t="s">
+      <c r="E19" s="70" t="s">
         <v>588</v>
       </c>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
-      <c r="M19" s="67"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
     </row>
     <row r="20" spans="2:13" ht="29">
       <c r="B20" s="7" t="s">
@@ -33192,17 +33337,17 @@
       <c r="D21" s="66" t="s">
         <v>774</v>
       </c>
-      <c r="E21" s="67" t="s">
+      <c r="E21" s="70" t="s">
         <v>775</v>
       </c>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="67"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+      <c r="K21" s="70"/>
+      <c r="L21" s="70"/>
+      <c r="M21" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -33217,10 +33362,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D48"/>
+  <dimension ref="B2:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -33506,10 +33651,10 @@
       <c r="B44" s="38" t="s">
         <v>734</v>
       </c>
-      <c r="C44" s="69" t="s">
+      <c r="C44" s="72" t="s">
         <v>735</v>
       </c>
-      <c r="D44" s="70"/>
+      <c r="D44" s="73"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="60" t="s">
@@ -33522,6 +33667,30 @@
       </c>
       <c r="C48" s="43" t="s">
         <v>762</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="60" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" s="68" customFormat="1" ht="116">
+      <c r="B52" s="83" t="s">
+        <v>779</v>
+      </c>
+      <c r="C52" s="67" t="s">
+        <v>780</v>
+      </c>
+      <c r="D52" s="69" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="29">
+      <c r="C53" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="D53" s="69" t="s">
+        <v>778</v>
       </c>
     </row>
   </sheetData>
@@ -33702,17 +33871,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="75" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="72"/>
+      <c r="C2" s="75"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="76" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -33720,10 +33889,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="77" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="74"/>
+      <c r="B6" s="77"/>
     </row>
     <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="35" t="s">
@@ -33852,88 +34021,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="71" t="s">
+      <c r="A22" s="74" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="71" t="s">
+      <c r="A23" s="74" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="71" t="s">
+      <c r="A24" s="74" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="74"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="74" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="74"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="71" t="s">
+      <c r="A26" s="74" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="74"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="71" t="s">
+      <c r="A27" s="74" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="71"/>
-      <c r="C27" s="71"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="74"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="71" t="s">
+      <c r="A28" s="74" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
+      <c r="B28" s="74"/>
+      <c r="C28" s="74"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="71" t="s">
+      <c r="A29" s="74" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="71"/>
+      <c r="B29" s="74"/>
+      <c r="C29" s="74"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="75" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="72" t="s">
+      <c r="A31" s="75" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="71" t="s">
+      <c r="A32" s="74" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="71"/>
-      <c r="C32" s="71"/>
+      <c r="B32" s="74"/>
+      <c r="C32" s="74"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="71" t="s">
+      <c r="A33" s="74" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="71"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
fleshed out git tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DD119DF-C522-486F-B2F0-0576D69B35E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1DFA90-7A51-4BD7-9748-D2AA2FDC18B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="795">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -26440,122 +26440,6 @@
     </r>
   </si>
   <si>
-    <t>CREATE NEW REPOSITORY</t>
-  </si>
-  <si>
-    <t>git init -b main</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-b </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= specifys the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>branch</t>
-    </r>
-  </si>
-  <si>
-    <t>initialize local directory as a Git repository</t>
-  </si>
-  <si>
-    <t>add files and stage them for commit</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = stages all files for commit</t>
-    </r>
-  </si>
-  <si>
-    <t>git commit -m "first commit"</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-m </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= specifys that you wish to create a message with the commit</t>
-    </r>
-  </si>
-  <si>
-    <t>commit the files that you've staged in your local repository</t>
-  </si>
-  <si>
-    <t>gh auth login</t>
-  </si>
-  <si>
-    <t>follow prompts, use HTTPS for simple login</t>
-  </si>
-  <si>
-    <t>Set up connection to your GitHub account</t>
-  </si>
-  <si>
-    <t>gh repo create</t>
-  </si>
-  <si>
-    <t>push an existing git repository to GitHub</t>
-  </si>
-  <si>
-    <t>follow prompts, select "Push an existing local repo to GitHub"</t>
-  </si>
-  <si>
     <t>linux 'iptables'</t>
   </si>
   <si>
@@ -26823,9 +26707,6 @@
   </si>
   <si>
     <t>git config -h</t>
-  </si>
-  <si>
-    <t>show help for git config</t>
   </si>
   <si>
     <t>displays some helpful tips for the 'git config' command</t>
@@ -29555,12 +29436,917 @@
       <t xml:space="preserve"> =  </t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>enter the name of your new repo in the '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project slug'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>under</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'Visibility Level' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">title, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Public'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Internal' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>radio buttons</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>navigate to GitLab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>click 'create a blank project'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the radio button for a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'readme'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file if you want one</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Create project'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>click</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Clone' button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and copy the URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (SSH or HTTPS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Git Bash</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>navigate to folder containing files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>you wish to commit</t>
+    </r>
+  </si>
+  <si>
+    <t>git init</t>
+  </si>
+  <si>
+    <t>takes the current folder and initializes it as a local 'working folder' or 'workbench' with the staging and commit trees</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>add files to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>staging</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tree</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>initialize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> local git repo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commit new file(s) to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> commit tree</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "initial commit"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-m </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= specifys that you wish to create a message with the commit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= means 'all files in folder'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>connect local repo to remote repo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on gitlab</t>
+    </r>
+  </si>
+  <si>
+    <t>git remote add gitlab &lt;copied URL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git push -u -f gitlab master </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">this simply connects the local and remote repo, it doesn't push anything
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>add gitlab &lt;copied URL&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = remote repo name/url</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gitlab</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = remote repo name (contains URL?)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = pushes master HEAD
+'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-u</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = set upstream for git pull/downstream for git push
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-f </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= force updates</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>push</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>local repo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> commits </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to remote repo</t>
+    </r>
+  </si>
+  <si>
+    <t>git pull gitlab master</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gitlab</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = remote repo name (contains URL?)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = pushes master HEAD</t>
+    </r>
+  </si>
+  <si>
+    <t>git remote show gitlab</t>
+  </si>
+  <si>
+    <t>displays info for the remote repo named 'gitlab'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> remote repo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show help</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>git config</t>
+    </r>
+  </si>
+  <si>
+    <t>CREATE NEW REPOSITORY - GITLAB</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OPTIONAL - FYSA)
+pull remote repo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> down </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to local repo</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -29637,8 +30423,17 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -29657,8 +30452,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -29715,12 +30522,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -29926,6 +30764,21 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -29958,8 +30811,68 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -30553,7 +31466,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="83" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -30567,7 +31480,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="72.5">
-      <c r="A9" s="78"/>
+      <c r="A9" s="83"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -30579,7 +31492,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29">
-      <c r="A10" s="78"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -30591,7 +31504,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="43.5">
-      <c r="A11" s="78"/>
+      <c r="A11" s="83"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -30603,7 +31516,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5">
-      <c r="A12" s="78"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -30620,7 +31533,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="43.5">
-      <c r="A15" s="79" t="s">
+      <c r="A15" s="84" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -30634,7 +31547,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="72.5">
-      <c r="A16" s="79"/>
+      <c r="A16" s="84"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -30646,7 +31559,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="87">
-      <c r="A17" s="79"/>
+      <c r="A17" s="84"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -30658,7 +31571,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="87">
-      <c r="A18" s="79"/>
+      <c r="A18" s="84"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -30670,7 +31583,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="58">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="84" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -30684,7 +31597,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="58">
-      <c r="A20" s="79"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -30696,7 +31609,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="101.5">
-      <c r="A21" s="79"/>
+      <c r="A21" s="84"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -30708,7 +31621,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="58">
-      <c r="A22" s="79"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -31057,38 +31970,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="80" t="s">
+      <c r="C19" s="85" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="80"/>
+      <c r="D19" s="85"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="80" t="s">
+      <c r="C20" s="85" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="80"/>
+      <c r="D20" s="85"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="80" t="s">
+      <c r="C21" s="85" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="80"/>
+      <c r="D21" s="85"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="80" t="s">
+      <c r="C22" s="85" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="80"/>
+      <c r="D22" s="85"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="80" t="s">
+      <c r="C23" s="85" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="80"/>
+      <c r="D23" s="85"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -31101,38 +32014,38 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="80" t="s">
+      <c r="C25" s="85" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="80"/>
+      <c r="D25" s="85"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="80" t="s">
+      <c r="C26" s="85" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="80"/>
+      <c r="D26" s="85"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="85" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="80"/>
+      <c r="D27" s="85"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="85" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="80"/>
+      <c r="D28" s="85"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="80" t="s">
+      <c r="C29" s="85" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="80"/>
+      <c r="D29" s="85"/>
     </row>
     <row r="30" spans="2:4" ht="39">
       <c r="B30" s="27" t="s">
@@ -31188,139 +32101,139 @@
   <sheetData>
     <row r="3" spans="2:4">
       <c r="B3" s="43" t="s">
-        <v>721</v>
+        <v>706</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="72" t="s">
-        <v>724</v>
-      </c>
-      <c r="D4" s="72"/>
+      <c r="C4" s="77" t="s">
+        <v>709</v>
+      </c>
+      <c r="D4" s="77"/>
     </row>
     <row r="5" spans="2:4" ht="75" customHeight="1">
-      <c r="C5" s="72" t="s">
-        <v>756</v>
-      </c>
-      <c r="D5" s="72"/>
+      <c r="C5" s="77" t="s">
+        <v>740</v>
+      </c>
+      <c r="D5" s="77"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="72" t="s">
-        <v>754</v>
-      </c>
-      <c r="D6" s="72"/>
+      <c r="C6" s="77" t="s">
+        <v>738</v>
+      </c>
+      <c r="D6" s="77"/>
     </row>
     <row r="7" spans="2:4" ht="75" customHeight="1">
-      <c r="C7" s="72" t="s">
-        <v>744</v>
-      </c>
-      <c r="D7" s="72"/>
+      <c r="C7" s="77" t="s">
+        <v>728</v>
+      </c>
+      <c r="D7" s="77"/>
     </row>
     <row r="9" spans="2:4" ht="75" customHeight="1">
       <c r="B9" s="8" t="s">
-        <v>757</v>
+        <v>741</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>758</v>
+        <v>742</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>769</v>
+        <v>753</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="29">
       <c r="B10" s="45" t="s">
-        <v>722</v>
+        <v>707</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>745</v>
+        <v>729</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>752</v>
+        <v>736</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="72.5">
       <c r="B11" s="8" t="s">
-        <v>743</v>
+        <v>727</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>748</v>
+        <v>732</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>726</v>
+        <v>711</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="58">
       <c r="B12" s="10" t="s">
-        <v>725</v>
+        <v>710</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>746</v>
+        <v>730</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>753</v>
+        <v>737</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="87">
       <c r="B13" s="8" t="s">
-        <v>749</v>
+        <v>733</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>747</v>
+        <v>731</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>764</v>
+        <v>748</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="29">
       <c r="B14" s="46" t="s">
-        <v>750</v>
+        <v>734</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>751</v>
+        <v>735</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>755</v>
+        <v>739</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="87">
       <c r="B15" s="8" t="s">
-        <v>760</v>
+        <v>744</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>759</v>
+        <v>743</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>767</v>
+        <v>751</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="105" customHeight="1">
       <c r="B16" s="8" t="s">
-        <v>765</v>
+        <v>749</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>766</v>
+        <v>750</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>768</v>
+        <v>752</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="180" customHeight="1">
       <c r="B17" s="8" t="s">
-        <v>770</v>
+        <v>754</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>773</v>
+        <v>757</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>772</v>
-      </c>
-      <c r="E17" s="81" t="s">
-        <v>771</v>
-      </c>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="70"/>
-      <c r="I17" s="70"/>
-      <c r="J17" s="70"/>
+        <v>756</v>
+      </c>
+      <c r="E17" s="86" t="s">
+        <v>755</v>
+      </c>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -31687,12 +32600,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="82" t="s">
+      <c r="B3" s="87" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -31700,11 +32613,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="79" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -31722,19 +32635,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="87" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="87"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="87" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="82"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -31771,7 +32684,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29">
+    <row r="4" spans="1:3">
       <c r="B4" s="39" t="s">
         <v>419</v>
       </c>
@@ -33285,14 +34198,14 @@
       <c r="D18" s="66" t="s">
         <v>583</v>
       </c>
-      <c r="E18" s="70" t="s">
+      <c r="E18" s="75" t="s">
         <v>584</v>
       </c>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -33304,17 +34217,17 @@
       <c r="D19" s="66" t="s">
         <v>587</v>
       </c>
-      <c r="E19" s="70" t="s">
+      <c r="E19" s="75" t="s">
         <v>588</v>
       </c>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="70"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="75"/>
+      <c r="M19" s="75"/>
     </row>
     <row r="20" spans="2:13" ht="29">
       <c r="B20" s="7" t="s">
@@ -33335,19 +34248,19 @@
         <v>593</v>
       </c>
       <c r="D21" s="66" t="s">
-        <v>774</v>
-      </c>
-      <c r="E21" s="70" t="s">
-        <v>775</v>
-      </c>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="70"/>
-      <c r="J21" s="70"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="70"/>
+        <v>758</v>
+      </c>
+      <c r="E21" s="75" t="s">
+        <v>759</v>
+      </c>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
+      <c r="J21" s="75"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="75"/>
+      <c r="M21" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -33362,16 +34275,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D53"/>
+  <dimension ref="B2:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="27"/>
-    <col min="2" max="2" width="49" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.90625" style="27" customWidth="1"/>
     <col min="3" max="3" width="43.54296875" style="27" customWidth="1"/>
     <col min="4" max="4" width="56.453125" style="27" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="27"/>
@@ -33460,13 +34373,13 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="27" t="s">
-        <v>737</v>
+        <v>792</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>736</v>
+        <v>721</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>738</v>
+        <v>722</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -33480,9 +34393,20 @@
         <v>608</v>
       </c>
     </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="27" t="s">
+        <v>791</v>
+      </c>
+      <c r="C16" s="72" t="s">
+        <v>789</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>790</v>
+      </c>
+    </row>
     <row r="18" spans="2:4">
       <c r="B18" s="60" t="s">
-        <v>742</v>
+        <v>726</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -33501,7 +34425,7 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="60" t="s">
-        <v>739</v>
+        <v>723</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -33546,156 +34470,224 @@
       <c r="D27" s="21"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="60" t="s">
-        <v>706</v>
-      </c>
+      <c r="B28" s="98" t="s">
+        <v>793</v>
+      </c>
+      <c r="C28" s="99"/>
+      <c r="D28" s="100"/>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" s="27" t="s">
-        <v>709</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>707</v>
-      </c>
-      <c r="D29" s="45" t="s">
+      <c r="B29" s="88" t="s">
+        <v>768</v>
+      </c>
+      <c r="C29" s="89"/>
+      <c r="D29" s="90"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="101" t="s">
+        <v>766</v>
+      </c>
+      <c r="C30" s="102"/>
+      <c r="D30" s="103"/>
+    </row>
+    <row r="31" spans="2:4" s="73" customFormat="1" ht="29">
+      <c r="B31" s="92" t="s">
+        <v>767</v>
+      </c>
+      <c r="C31" s="89"/>
+      <c r="D31" s="91"/>
+    </row>
+    <row r="32" spans="2:4" s="73" customFormat="1">
+      <c r="B32" s="104" t="s">
+        <v>769</v>
+      </c>
+      <c r="C32" s="102"/>
+      <c r="D32" s="103"/>
+    </row>
+    <row r="33" spans="2:4" s="73" customFormat="1">
+      <c r="B33" s="92" t="s">
+        <v>770</v>
+      </c>
+      <c r="C33" s="89"/>
+      <c r="D33" s="91"/>
+    </row>
+    <row r="34" spans="2:4" s="73" customFormat="1">
+      <c r="B34" s="104" t="s">
+        <v>771</v>
+      </c>
+      <c r="C34" s="102"/>
+      <c r="D34" s="103"/>
+    </row>
+    <row r="35" spans="2:4" s="73" customFormat="1" ht="29">
+      <c r="B35" s="92" t="s">
+        <v>772</v>
+      </c>
+      <c r="C35" s="89"/>
+      <c r="D35" s="91"/>
+    </row>
+    <row r="36" spans="2:4" s="73" customFormat="1" ht="29">
+      <c r="B36" s="105" t="s">
+        <v>776</v>
+      </c>
+      <c r="C36" s="106" t="s">
+        <v>773</v>
+      </c>
+      <c r="D36" s="107" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" s="73" customFormat="1">
+      <c r="B37" s="93" t="s">
+        <v>775</v>
+      </c>
+      <c r="C37" s="94" t="s">
+        <v>617</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" s="73" customFormat="1">
+      <c r="B38" s="105" t="s">
+        <v>777</v>
+      </c>
+      <c r="C38" s="106" t="s">
+        <v>778</v>
+      </c>
+      <c r="D38" s="108" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" s="73" customFormat="1" ht="43.5">
+      <c r="B39" s="93" t="s">
+        <v>781</v>
+      </c>
+      <c r="C39" s="94" t="s">
+        <v>782</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" s="73" customFormat="1" ht="58">
+      <c r="B40" s="105" t="s">
+        <v>786</v>
+      </c>
+      <c r="C40" s="106" t="s">
+        <v>783</v>
+      </c>
+      <c r="D40" s="108" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" s="73" customFormat="1" ht="29">
+      <c r="B41" s="95" t="s">
+        <v>794</v>
+      </c>
+      <c r="C41" s="96" t="s">
+        <v>787</v>
+      </c>
+      <c r="D41" s="97" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" s="73" customFormat="1">
+      <c r="B42" s="6"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="70"/>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="60" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="27" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="27" t="s">
-        <v>710</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>617</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="29">
-      <c r="B31" s="38" t="s">
+      <c r="C45" s="43" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="60" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4">
+      <c r="B49" s="27" t="s">
+        <v>713</v>
+      </c>
+      <c r="C49" s="43" t="s">
         <v>714</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>712</v>
-      </c>
-      <c r="D31" s="46" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="27" t="s">
+    </row>
+    <row r="50" spans="2:4" ht="29">
+      <c r="B50" s="38" t="s">
+        <v>715</v>
+      </c>
+      <c r="C50" s="39" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="27" t="s">
         <v>717</v>
       </c>
-      <c r="C32" s="43" t="s">
-        <v>715</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="27" t="s">
+      <c r="C51" s="43" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="29">
+      <c r="B52" s="38" t="s">
         <v>719</v>
       </c>
-      <c r="C33" s="43" t="s">
-        <v>718</v>
-      </c>
-      <c r="D33" s="27" t="s">
+      <c r="C52" s="77" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="60" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="27" t="s">
-        <v>723</v>
-      </c>
-      <c r="C37" s="43" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4">
-      <c r="B40" s="60" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4">
-      <c r="B41" s="27" t="s">
-        <v>728</v>
-      </c>
-      <c r="C41" s="43" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="29">
-      <c r="B42" s="38" t="s">
-        <v>730</v>
-      </c>
-      <c r="C42" s="39" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4">
-      <c r="B43" s="27" t="s">
-        <v>732</v>
-      </c>
-      <c r="C43" s="43" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="29">
-      <c r="B44" s="38" t="s">
-        <v>734</v>
-      </c>
-      <c r="C44" s="72" t="s">
-        <v>735</v>
-      </c>
-      <c r="D44" s="73"/>
-    </row>
-    <row r="47" spans="2:4">
-      <c r="B47" s="60" t="s">
+      <c r="D52" s="78"/>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="60" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="27" t="s">
+        <v>747</v>
+      </c>
+      <c r="C56" s="43" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="60" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" s="68" customFormat="1" ht="116">
+      <c r="B60" s="74" t="s">
+        <v>763</v>
+      </c>
+      <c r="C60" s="67" t="s">
+        <v>764</v>
+      </c>
+      <c r="D60" s="69" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="29">
+      <c r="C61" s="2" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="48" spans="2:4">
-      <c r="B48" s="27" t="s">
-        <v>763</v>
-      </c>
-      <c r="C48" s="43" t="s">
+      <c r="D61" s="69" t="s">
         <v>762</v>
       </c>
     </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="60" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" s="68" customFormat="1" ht="116">
-      <c r="B52" s="83" t="s">
-        <v>779</v>
-      </c>
-      <c r="C52" s="67" t="s">
-        <v>780</v>
-      </c>
-      <c r="D52" s="69" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="29">
-      <c r="C53" s="2" t="s">
-        <v>777</v>
-      </c>
-      <c r="D53" s="69" t="s">
-        <v>778</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C44:D44"/>
+  <mergeCells count="2">
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="B28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -33871,17 +34863,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="80" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="75"/>
+      <c r="C2" s="80"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="81" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="81"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -33889,10 +34881,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="82" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="77"/>
+      <c r="B6" s="82"/>
     </row>
     <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="35" t="s">
@@ -34021,88 +35013,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="79" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
+      <c r="B22" s="79"/>
+      <c r="C22" s="79"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="74" t="s">
+      <c r="A23" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="74" t="s">
+      <c r="A24" s="79" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
+      <c r="B24" s="79"/>
+      <c r="C24" s="79"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="79" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="74"/>
-      <c r="C25" s="74"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="79"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="79" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="74"/>
-      <c r="C26" s="74"/>
+      <c r="B26" s="79"/>
+      <c r="C26" s="79"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="79" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
+      <c r="B27" s="79"/>
+      <c r="C27" s="79"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="79" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
+      <c r="B28" s="79"/>
+      <c r="C28" s="79"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="74" t="s">
+      <c r="A29" s="79" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="74"/>
-      <c r="C29" s="74"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="79"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="80" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="75"/>
-      <c r="C30" s="75"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="80"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="80" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="79" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="74"/>
-      <c r="C32" s="74"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="79"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="79" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="74"/>
-      <c r="C33" s="74"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
fleshed out git some more
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1DFA90-7A51-4BD7-9748-D2AA2FDC18B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC476CE6-7D77-4A3A-969A-523643B92E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -29310,1036 +29310,1046 @@
     <t>git diff</t>
   </si>
   <si>
-    <t>show differences between file in working folder and file in local repo</t>
-  </si>
-  <si>
     <t>Basic output guide</t>
   </si>
   <si>
-    <t>diff --git a/file.txt b/file.txt
+    <r>
+      <t>enter the name of your new repo in the '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Project slug'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>under</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'Visibility Level' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">title, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Public'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Internal' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>radio buttons</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>navigate to GitLab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>click 'create a blank project'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>select</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the radio button for a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'readme'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> file if you want one</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">click </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Create project'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>click</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Clone' button</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and copy the URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (SSH or HTTPS)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Git Bash</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>navigate to folder containing files</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>you wish to commit</t>
+    </r>
+  </si>
+  <si>
+    <t>git init</t>
+  </si>
+  <si>
+    <t>takes the current folder and initializes it as a local 'working folder' or 'workbench' with the staging and commit trees</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>add files to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>staging</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tree</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>initialize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> local git repo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commit new file(s) to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> commit tree</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "initial commit"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-m </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= specifys that you wish to create a message with the commit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= means 'all files in folder'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>connect local repo to remote repo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on gitlab</t>
+    </r>
+  </si>
+  <si>
+    <t>git remote add gitlab &lt;copied URL&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git push -u -f gitlab master </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">this simply connects the local and remote repo, it doesn't push anything
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>add gitlab &lt;copied URL&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = remote repo name/url</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gitlab</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = remote repo name (contains URL?)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = pushes master HEAD
+'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-u</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = set upstream for git pull/downstream for git push
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">-f </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= force updates</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>push</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>local repo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> commits </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to remote repo</t>
+    </r>
+  </si>
+  <si>
+    <t>git pull gitlab master</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gitlab</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = remote repo name (contains URL?)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = pushes master HEAD</t>
+    </r>
+  </si>
+  <si>
+    <t>git remote show gitlab</t>
+  </si>
+  <si>
+    <t>displays info for the remote repo named 'gitlab'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> remote repo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show help</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>git config</t>
+    </r>
+  </si>
+  <si>
+    <t>CREATE NEW REPOSITORY - GITLAB</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OPTIONAL - FYSA)
+pull remote repo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> down </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to local repo</t>
+    </r>
+  </si>
+  <si>
+    <t>show differences between working folder and local repo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">diff --git a/test.txt b/test.txt </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= comparing 2 versions of same file, 'a' and 'b'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>index b473041..69040e2  100644</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = different hashes for old and new files, plus '100644' is the 'mode' of the file (what functions are allowed on the file - e.g. '100644' is a non-executable)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">--- a/test.txt = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file version 'a' is symbolized by a '-'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
++++ b/test.txt = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">file version 'b' is symbolized by a '+'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@@ -1,2  +1,3 @@</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =   </t>
+    </r>
+  </si>
+  <si>
+    <t>diff --git a/test.txt b/test.txt
 index f2aa86d..1831a89  100644
 --- a/file.txt
 +++ b/file.txt
-@@ -1 +1,2 @@ 
-hello
-+added text to line 2
-\ No newline at end of file</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">diff --git a/file b/file </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= comparing 2 versions of same file, 'a' and 'b'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>index f2aa86d..1831a89  100644</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = different hashes for old and new files, plus '100644' is the 'mode' of the file (what functions are allowed on the file)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">--- a/file.txt = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>file version 'a' is symbolized by a '-'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-+++ b/file.txt = </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">file version 'b' is symbolized by a '+'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@@ -1 +1,2 @@</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =  </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>enter the name of your new repo in the '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Project slug'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> field</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>under</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 'Visibility Level' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">title, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>select</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Public'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> or '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Internal' </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>radio buttons</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>navigate to GitLab</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>click 'create a blank project'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>select</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the radio button for a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'readme'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> file if you want one</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">click </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Create project'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>click</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'Clone' button</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>and copy the URL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (SSH or HTTPS)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Git Bash</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>navigate to folder containing files</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>you wish to commit</t>
-    </r>
-  </si>
-  <si>
-    <t>git init</t>
-  </si>
-  <si>
-    <t>takes the current folder and initializes it as a local 'working folder' or 'workbench' with the staging and commit trees</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>add files to</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>staging</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> tree</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>initialize</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> local git repo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>commit new file(s) to</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> commit tree</t>
-    </r>
-  </si>
-  <si>
-    <t>git commit -m "initial commit"</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-m </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= specifys that you wish to create a message with the commit</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= means 'all files in folder'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>connect local repo to remote repo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> on gitlab</t>
-    </r>
-  </si>
-  <si>
-    <t>git remote add gitlab &lt;copied URL&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">git push -u -f gitlab master </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">this simply connects the local and remote repo, it doesn't push anything
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>add gitlab &lt;copied URL&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = remote repo name/url</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>gitlab</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = remote repo name (contains URL?)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>master</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = pushes master HEAD
-'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-u</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = set upstream for git pull/downstream for git push
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">-f </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>= force updates</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>push</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>local repo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> commits </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to remote repo</t>
-    </r>
-  </si>
-  <si>
-    <t>git pull gitlab master</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>gitlab</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = remote repo name (contains URL?)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>master</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = pushes master HEAD</t>
-    </r>
-  </si>
-  <si>
-    <t>git remote show gitlab</t>
-  </si>
-  <si>
-    <t>displays info for the remote repo named 'gitlab'</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>show info</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> remote repo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> name</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>show help</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>git config</t>
-    </r>
-  </si>
-  <si>
-    <t>CREATE NEW REPOSITORY - GITLAB</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(OPTIONAL - FYSA)
-pull remote repo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> down </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to local repo</t>
-    </r>
+@@ -1,2 +1,3 @@ 
++This is a test of the emergency alert system
+This is a test
+This is only a test</t>
   </si>
 </sst>
 </file>
@@ -30754,9 +30764,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -30774,42 +30781,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -30841,15 +30812,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -30873,6 +30835,54 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -31466,7 +31476,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="104" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -31480,7 +31490,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="72.5">
-      <c r="A9" s="83"/>
+      <c r="A9" s="104"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -31492,7 +31502,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29">
-      <c r="A10" s="83"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -31504,7 +31514,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="43.5">
-      <c r="A11" s="83"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -31516,7 +31526,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5">
-      <c r="A12" s="83"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -31533,7 +31543,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="43.5">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="105" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -31547,7 +31557,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="72.5">
-      <c r="A16" s="84"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -31559,7 +31569,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="87">
-      <c r="A17" s="84"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -31571,7 +31581,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="87">
-      <c r="A18" s="84"/>
+      <c r="A18" s="105"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -31583,7 +31593,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="58">
-      <c r="A19" s="84" t="s">
+      <c r="A19" s="105" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -31597,7 +31607,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="58">
-      <c r="A20" s="84"/>
+      <c r="A20" s="105"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -31609,7 +31619,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="101.5">
-      <c r="A21" s="84"/>
+      <c r="A21" s="105"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -31621,7 +31631,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="58">
-      <c r="A22" s="84"/>
+      <c r="A22" s="105"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -31970,38 +31980,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="106" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="85"/>
+      <c r="D19" s="106"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="85" t="s">
+      <c r="C20" s="106" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="85"/>
+      <c r="D20" s="106"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="85" t="s">
+      <c r="C21" s="106" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="85"/>
+      <c r="D21" s="106"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="85" t="s">
+      <c r="C22" s="106" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="85"/>
+      <c r="D22" s="106"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="85" t="s">
+      <c r="C23" s="106" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="85"/>
+      <c r="D23" s="106"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -32014,38 +32024,38 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="85" t="s">
+      <c r="C25" s="106" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="85"/>
+      <c r="D25" s="106"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="85" t="s">
+      <c r="C26" s="106" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="85"/>
+      <c r="D26" s="106"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="85" t="s">
+      <c r="C27" s="106" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="85"/>
+      <c r="D27" s="106"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="85" t="s">
+      <c r="C28" s="106" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="85"/>
+      <c r="D28" s="106"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="106" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="85"/>
+      <c r="D29" s="106"/>
     </row>
     <row r="30" spans="2:4" ht="39">
       <c r="B30" s="27" t="s">
@@ -32105,28 +32115,28 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="95" t="s">
         <v>709</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="95"/>
     </row>
     <row r="5" spans="2:4" ht="75" customHeight="1">
-      <c r="C5" s="77" t="s">
+      <c r="C5" s="95" t="s">
         <v>740</v>
       </c>
-      <c r="D5" s="77"/>
+      <c r="D5" s="95"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="95" t="s">
         <v>738</v>
       </c>
-      <c r="D6" s="77"/>
+      <c r="D6" s="95"/>
     </row>
     <row r="7" spans="2:4" ht="75" customHeight="1">
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="95" t="s">
         <v>728</v>
       </c>
-      <c r="D7" s="77"/>
+      <c r="D7" s="95"/>
     </row>
     <row r="9" spans="2:4" ht="75" customHeight="1">
       <c r="B9" s="8" t="s">
@@ -32226,14 +32236,14 @@
       <c r="D17" s="18" t="s">
         <v>756</v>
       </c>
-      <c r="E17" s="86" t="s">
+      <c r="E17" s="107" t="s">
         <v>755</v>
       </c>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="75"/>
-      <c r="J17" s="75"/>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="93"/>
+      <c r="J17" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -32600,12 +32610,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="108" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
+      <c r="E3" s="108"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -32613,11 +32623,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="79" t="s">
+      <c r="B5" s="100" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -32635,19 +32645,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="108" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="87"/>
+      <c r="C11" s="108"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="108" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="87"/>
+      <c r="C12" s="108"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -32684,7 +32694,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="29">
       <c r="B4" s="39" t="s">
         <v>419</v>
       </c>
@@ -34198,14 +34208,14 @@
       <c r="D18" s="66" t="s">
         <v>583</v>
       </c>
-      <c r="E18" s="75" t="s">
+      <c r="E18" s="93" t="s">
         <v>584</v>
       </c>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -34217,17 +34227,17 @@
       <c r="D19" s="66" t="s">
         <v>587</v>
       </c>
-      <c r="E19" s="75" t="s">
+      <c r="E19" s="93" t="s">
         <v>588</v>
       </c>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
+      <c r="F19" s="93"/>
+      <c r="G19" s="93"/>
+      <c r="H19" s="93"/>
+      <c r="I19" s="93"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="93"/>
+      <c r="L19" s="93"/>
+      <c r="M19" s="93"/>
     </row>
     <row r="20" spans="2:13" ht="29">
       <c r="B20" s="7" t="s">
@@ -34250,17 +34260,17 @@
       <c r="D21" s="66" t="s">
         <v>758</v>
       </c>
-      <c r="E21" s="75" t="s">
+      <c r="E21" s="93" t="s">
         <v>759</v>
       </c>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
-      <c r="I21" s="75"/>
-      <c r="J21" s="75"/>
-      <c r="K21" s="75"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="75"/>
+      <c r="F21" s="93"/>
+      <c r="G21" s="93"/>
+      <c r="H21" s="93"/>
+      <c r="I21" s="93"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="93"/>
+      <c r="L21" s="93"/>
+      <c r="M21" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -34277,8 +34287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
   <dimension ref="B2:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -34373,7 +34383,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="27" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C14" s="43" t="s">
         <v>721</v>
@@ -34395,13 +34405,13 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="27" t="s">
-        <v>791</v>
-      </c>
-      <c r="C16" s="72" t="s">
-        <v>789</v>
-      </c>
-      <c r="D16" s="71" t="s">
-        <v>790</v>
+        <v>788</v>
+      </c>
+      <c r="C16" s="71" t="s">
+        <v>786</v>
+      </c>
+      <c r="D16" s="70" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -34470,131 +34480,131 @@
       <c r="D27" s="21"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="98" t="s">
-        <v>793</v>
-      </c>
-      <c r="C28" s="99"/>
-      <c r="D28" s="100"/>
+      <c r="B28" s="97" t="s">
+        <v>790</v>
+      </c>
+      <c r="C28" s="98"/>
+      <c r="D28" s="99"/>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" s="88" t="s">
+      <c r="B29" s="75" t="s">
+        <v>765</v>
+      </c>
+      <c r="C29" s="76"/>
+      <c r="D29" s="77"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="85" t="s">
+        <v>763</v>
+      </c>
+      <c r="C30" s="86"/>
+      <c r="D30" s="87"/>
+    </row>
+    <row r="31" spans="2:4" s="72" customFormat="1" ht="29">
+      <c r="B31" s="79" t="s">
+        <v>764</v>
+      </c>
+      <c r="C31" s="76"/>
+      <c r="D31" s="78"/>
+    </row>
+    <row r="32" spans="2:4" s="72" customFormat="1">
+      <c r="B32" s="88" t="s">
+        <v>766</v>
+      </c>
+      <c r="C32" s="86"/>
+      <c r="D32" s="87"/>
+    </row>
+    <row r="33" spans="2:4" s="72" customFormat="1">
+      <c r="B33" s="79" t="s">
+        <v>767</v>
+      </c>
+      <c r="C33" s="76"/>
+      <c r="D33" s="78"/>
+    </row>
+    <row r="34" spans="2:4" s="72" customFormat="1">
+      <c r="B34" s="88" t="s">
         <v>768</v>
       </c>
-      <c r="C29" s="89"/>
-      <c r="D29" s="90"/>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="101" t="s">
-        <v>766</v>
-      </c>
-      <c r="C30" s="102"/>
-      <c r="D30" s="103"/>
-    </row>
-    <row r="31" spans="2:4" s="73" customFormat="1" ht="29">
-      <c r="B31" s="92" t="s">
-        <v>767</v>
-      </c>
-      <c r="C31" s="89"/>
-      <c r="D31" s="91"/>
-    </row>
-    <row r="32" spans="2:4" s="73" customFormat="1">
-      <c r="B32" s="104" t="s">
+      <c r="C34" s="86"/>
+      <c r="D34" s="87"/>
+    </row>
+    <row r="35" spans="2:4" s="72" customFormat="1" ht="29">
+      <c r="B35" s="79" t="s">
         <v>769</v>
       </c>
-      <c r="C32" s="102"/>
-      <c r="D32" s="103"/>
-    </row>
-    <row r="33" spans="2:4" s="73" customFormat="1">
-      <c r="B33" s="92" t="s">
+      <c r="C35" s="76"/>
+      <c r="D35" s="78"/>
+    </row>
+    <row r="36" spans="2:4" s="72" customFormat="1" ht="29">
+      <c r="B36" s="89" t="s">
+        <v>773</v>
+      </c>
+      <c r="C36" s="90" t="s">
         <v>770</v>
       </c>
-      <c r="C33" s="89"/>
-      <c r="D33" s="91"/>
-    </row>
-    <row r="34" spans="2:4" s="73" customFormat="1">
-      <c r="B34" s="104" t="s">
+      <c r="D36" s="91" t="s">
         <v>771</v>
       </c>
-      <c r="C34" s="102"/>
-      <c r="D34" s="103"/>
-    </row>
-    <row r="35" spans="2:4" s="73" customFormat="1" ht="29">
-      <c r="B35" s="92" t="s">
+    </row>
+    <row r="37" spans="2:4" s="72" customFormat="1">
+      <c r="B37" s="80" t="s">
         <v>772</v>
       </c>
-      <c r="C35" s="89"/>
-      <c r="D35" s="91"/>
-    </row>
-    <row r="36" spans="2:4" s="73" customFormat="1" ht="29">
-      <c r="B36" s="105" t="s">
+      <c r="C37" s="81" t="s">
+        <v>617</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" s="72" customFormat="1">
+      <c r="B38" s="89" t="s">
+        <v>774</v>
+      </c>
+      <c r="C38" s="90" t="s">
+        <v>775</v>
+      </c>
+      <c r="D38" s="92" t="s">
         <v>776</v>
       </c>
-      <c r="C36" s="106" t="s">
-        <v>773</v>
-      </c>
-      <c r="D36" s="107" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" s="73" customFormat="1">
-      <c r="B37" s="93" t="s">
-        <v>775</v>
-      </c>
-      <c r="C37" s="94" t="s">
-        <v>617</v>
-      </c>
-      <c r="D37" s="40" t="s">
+    </row>
+    <row r="39" spans="2:4" s="72" customFormat="1" ht="43.5">
+      <c r="B39" s="80" t="s">
+        <v>778</v>
+      </c>
+      <c r="C39" s="81" t="s">
+        <v>779</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" s="72" customFormat="1" ht="58">
+      <c r="B40" s="89" t="s">
+        <v>783</v>
+      </c>
+      <c r="C40" s="90" t="s">
         <v>780</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" s="73" customFormat="1">
-      <c r="B38" s="105" t="s">
-        <v>777</v>
-      </c>
-      <c r="C38" s="106" t="s">
-        <v>778</v>
-      </c>
-      <c r="D38" s="108" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" s="73" customFormat="1" ht="43.5">
-      <c r="B39" s="93" t="s">
-        <v>781</v>
-      </c>
-      <c r="C39" s="94" t="s">
+      <c r="D40" s="92" t="s">
         <v>782</v>
       </c>
-      <c r="D39" s="40" t="s">
+    </row>
+    <row r="41" spans="2:4" s="72" customFormat="1" ht="29">
+      <c r="B41" s="82" t="s">
+        <v>791</v>
+      </c>
+      <c r="C41" s="83" t="s">
         <v>784</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" s="73" customFormat="1" ht="58">
-      <c r="B40" s="105" t="s">
-        <v>786</v>
-      </c>
-      <c r="C40" s="106" t="s">
-        <v>783</v>
-      </c>
-      <c r="D40" s="108" t="s">
+      <c r="D41" s="84" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="41" spans="2:4" s="73" customFormat="1" ht="29">
-      <c r="B41" s="95" t="s">
-        <v>794</v>
-      </c>
-      <c r="C41" s="96" t="s">
-        <v>787</v>
-      </c>
-      <c r="D41" s="97" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" s="73" customFormat="1">
+    <row r="42" spans="2:4" s="72" customFormat="1">
       <c r="B42" s="6"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="70"/>
+      <c r="D42" s="69"/>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" s="60" t="s">
@@ -34642,10 +34652,10 @@
       <c r="B52" s="38" t="s">
         <v>719</v>
       </c>
-      <c r="C52" s="77" t="s">
+      <c r="C52" s="95" t="s">
         <v>720</v>
       </c>
-      <c r="D52" s="78"/>
+      <c r="D52" s="96"/>
     </row>
     <row r="55" spans="2:4">
       <c r="B55" s="60" t="s">
@@ -34666,22 +34676,22 @@
       </c>
     </row>
     <row r="60" spans="2:4" s="68" customFormat="1" ht="116">
-      <c r="B60" s="74" t="s">
-        <v>763</v>
+      <c r="B60" s="73" t="s">
+        <v>762</v>
       </c>
       <c r="C60" s="67" t="s">
-        <v>764</v>
-      </c>
-      <c r="D60" s="69" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" ht="29">
+        <v>794</v>
+      </c>
+      <c r="D60" s="74" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
       <c r="C61" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="D61" s="69" t="s">
-        <v>762</v>
+      <c r="D61" s="74" t="s">
+        <v>792</v>
       </c>
     </row>
   </sheetData>
@@ -34863,17 +34873,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="101" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="80"/>
+      <c r="C2" s="101"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="102" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -34881,10 +34891,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="82"/>
+      <c r="B6" s="103"/>
     </row>
     <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="35" t="s">
@@ -35013,88 +35023,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="100" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="79"/>
-      <c r="C22" s="79"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="79"/>
-      <c r="C23" s="79"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="79" t="s">
+      <c r="A24" s="100" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="79"/>
-      <c r="C24" s="79"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="79" t="s">
+      <c r="A25" s="100" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="79"/>
-      <c r="C25" s="79"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="79" t="s">
+      <c r="A26" s="100" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="79"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="100"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="79" t="s">
+      <c r="A27" s="100" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="79"/>
-      <c r="C27" s="79"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="100"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="79" t="s">
+      <c r="A28" s="100" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="79"/>
-      <c r="C28" s="79"/>
+      <c r="B28" s="100"/>
+      <c r="C28" s="100"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="79" t="s">
+      <c r="A29" s="100" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="79"/>
-      <c r="C29" s="79"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="100"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="101" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="80"/>
-      <c r="C30" s="80"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="101"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="101" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="80"/>
-      <c r="C31" s="80"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="79" t="s">
+      <c r="A32" s="100" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="79"/>
-      <c r="C32" s="79"/>
+      <c r="B32" s="100"/>
+      <c r="C32" s="100"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="100" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="79"/>
-      <c r="C33" s="79"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="100"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
git tab work 11.16.2023
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC476CE6-7D77-4A3A-969A-523643B92E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8F7216-A0F7-4846-869F-A04A4F97357E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="804">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -30218,138 +30218,438 @@
     </r>
   </si>
   <si>
-    <t>show differences between working folder and local repo</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">diff --git a/test.txt b/test.txt </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= comparing 2 versions of same file, 'a' and 'b'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>index b473041..69040e2  100644</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = different hashes for old and new files, plus '100644' is the 'mode' of the file (what functions are allowed on the file - e.g. '100644' is a non-executable)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">--- a/test.txt = </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>file version 'a' is symbolized by a '-'</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-+++ b/test.txt = </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">file version 'b' is symbolized by a '+'
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@@ -1,2  +1,3 @@</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =   </t>
-    </r>
-  </si>
-  <si>
     <t>diff --git a/test.txt b/test.txt
 index f2aa86d..1831a89  100644
 --- a/file.txt
 +++ b/file.txt
 @@ -1,2 +1,3 @@ 
-+This is a test of the emergency alert system
++This is a test of the alert system
 This is a test
 This is only a test</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">diff --git a/test.txt b/test.txt </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= comparing 2 versions of same file, 'a' and 'b'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>index b473041..69040e2  100644</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = different hashes for old and new files, plus '100644' is the 'mode' of the file (what functions are allowed on the file - e.g. '100644' is a non-executable)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">--- a/test.txt = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>file version 'a' is symbolized by a '-'</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
++++ b/test.txt = </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">file version 'b' is symbolized by a '+'
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@@ -1,2  +1,3 @@</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = file version 'a' (-1) has 2 lines starting from line 1. File version 'b' (+1) has 3 lines, starting from line 1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+This is a test of the alert system</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = file located in workbench tree aka 'new file' (designated by the '+' sign) contains this line
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">This is a test </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= line exists in both workbench tree and staged tree (index) version of file
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This is only a test</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = line exists in both workbench tree and staged tree (index) version of file</t>
+    </r>
+  </si>
+  <si>
+    <t>show differences between working folder tree (workbench) and staged tree (index)</t>
+  </si>
+  <si>
+    <t>git log --oneline test.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>log --oneline &lt;filename&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = show hashes for historical changes</t>
+    </r>
+  </si>
+  <si>
+    <t>show the log of changes for the 'test.txt' file in one line per change</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git diff &lt;hash 1&gt; &lt;hash 2&gt; = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show the difference between historical file changes by hash</t>
+    </r>
+  </si>
+  <si>
+    <t>git diff cfe6410 f74470c</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>displays the changes between</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> historical hash </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>cfe6410</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and historical hash </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>f74470c</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>git diff --staged</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = displays the differences between the staged tree (index) and the commit tree (local repo)</t>
+    </r>
+  </si>
+  <si>
+    <t>git diff --staged</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>show differences</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> between </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>staged tree</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (index) and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>commit tree</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (local repo)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">NOTE: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>you can also use the option '--cached' to display the same thing</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -30568,7 +30868,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -30834,6 +31134,24 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -31476,7 +31794,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="110" t="s">
         <v>414</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -31490,7 +31808,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="72.5">
-      <c r="A9" s="104"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="6" t="s">
         <v>403</v>
       </c>
@@ -31502,7 +31820,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29">
-      <c r="A10" s="104"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="6" t="s">
         <v>404</v>
       </c>
@@ -31514,7 +31832,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="43.5">
-      <c r="A11" s="104"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="6" t="s">
         <v>406</v>
       </c>
@@ -31526,7 +31844,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5">
-      <c r="A12" s="104"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="47" t="s">
         <v>408</v>
       </c>
@@ -31543,7 +31861,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="43.5">
-      <c r="A15" s="105" t="s">
+      <c r="A15" s="111" t="s">
         <v>415</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -31557,7 +31875,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="72.5">
-      <c r="A16" s="105"/>
+      <c r="A16" s="111"/>
       <c r="B16" s="8" t="s">
         <v>413</v>
       </c>
@@ -31569,7 +31887,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="87">
-      <c r="A17" s="105"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="8" t="s">
         <v>518</v>
       </c>
@@ -31581,7 +31899,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="87">
-      <c r="A18" s="105"/>
+      <c r="A18" s="111"/>
       <c r="B18" s="8" t="s">
         <v>519</v>
       </c>
@@ -31593,7 +31911,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="58">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="111" t="s">
         <v>415</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -31607,7 +31925,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="58">
-      <c r="A20" s="105"/>
+      <c r="A20" s="111"/>
       <c r="B20" s="11" t="s">
         <v>527</v>
       </c>
@@ -31619,7 +31937,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="101.5">
-      <c r="A21" s="105"/>
+      <c r="A21" s="111"/>
       <c r="B21" s="11" t="s">
         <v>530</v>
       </c>
@@ -31631,7 +31949,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="58">
-      <c r="A22" s="105"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="55" t="s">
         <v>532</v>
       </c>
@@ -31980,38 +32298,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="106" t="s">
+      <c r="C19" s="112" t="s">
         <v>689</v>
       </c>
-      <c r="D19" s="106"/>
+      <c r="D19" s="112"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="106" t="s">
+      <c r="C20" s="112" t="s">
         <v>690</v>
       </c>
-      <c r="D20" s="106"/>
+      <c r="D20" s="112"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="112" t="s">
         <v>691</v>
       </c>
-      <c r="D21" s="106"/>
+      <c r="D21" s="112"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="106" t="s">
+      <c r="C22" s="112" t="s">
         <v>692</v>
       </c>
-      <c r="D22" s="106"/>
+      <c r="D22" s="112"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="106" t="s">
+      <c r="C23" s="112" t="s">
         <v>693</v>
       </c>
-      <c r="D23" s="106"/>
+      <c r="D23" s="112"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -32024,38 +32342,38 @@
       <c r="B25" s="63" t="s">
         <v>695</v>
       </c>
-      <c r="C25" s="106" t="s">
+      <c r="C25" s="112" t="s">
         <v>696</v>
       </c>
-      <c r="D25" s="106"/>
+      <c r="D25" s="112"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="106" t="s">
+      <c r="C26" s="112" t="s">
         <v>697</v>
       </c>
-      <c r="D26" s="106"/>
+      <c r="D26" s="112"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="106" t="s">
+      <c r="C27" s="112" t="s">
         <v>698</v>
       </c>
-      <c r="D27" s="106"/>
+      <c r="D27" s="112"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="106" t="s">
+      <c r="C28" s="112" t="s">
         <v>699</v>
       </c>
-      <c r="D28" s="106"/>
+      <c r="D28" s="112"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="106" t="s">
+      <c r="C29" s="112" t="s">
         <v>700</v>
       </c>
-      <c r="D29" s="106"/>
+      <c r="D29" s="112"/>
     </row>
     <row r="30" spans="2:4" ht="39">
       <c r="B30" s="27" t="s">
@@ -32115,28 +32433,28 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="101" t="s">
         <v>709</v>
       </c>
-      <c r="D4" s="95"/>
+      <c r="D4" s="101"/>
     </row>
     <row r="5" spans="2:4" ht="75" customHeight="1">
-      <c r="C5" s="95" t="s">
+      <c r="C5" s="101" t="s">
         <v>740</v>
       </c>
-      <c r="D5" s="95"/>
+      <c r="D5" s="101"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="101" t="s">
         <v>738</v>
       </c>
-      <c r="D6" s="95"/>
+      <c r="D6" s="101"/>
     </row>
     <row r="7" spans="2:4" ht="75" customHeight="1">
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="101" t="s">
         <v>728</v>
       </c>
-      <c r="D7" s="95"/>
+      <c r="D7" s="101"/>
     </row>
     <row r="9" spans="2:4" ht="75" customHeight="1">
       <c r="B9" s="8" t="s">
@@ -32236,14 +32554,14 @@
       <c r="D17" s="18" t="s">
         <v>756</v>
       </c>
-      <c r="E17" s="107" t="s">
+      <c r="E17" s="113" t="s">
         <v>755</v>
       </c>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
+      <c r="F17" s="99"/>
+      <c r="G17" s="99"/>
+      <c r="H17" s="99"/>
+      <c r="I17" s="99"/>
+      <c r="J17" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -32610,12 +32928,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="114" t="s">
         <v>359</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -32623,11 +32941,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="106" t="s">
         <v>360</v>
       </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -32645,19 +32963,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="114" t="s">
         <v>365</v>
       </c>
-      <c r="C11" s="108"/>
+      <c r="C11" s="114"/>
       <c r="D11" s="27" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="114" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="108"/>
+      <c r="C12" s="114"/>
       <c r="D12" s="27" t="s">
         <v>368</v>
       </c>
@@ -32694,7 +33012,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29">
+    <row r="4" spans="1:3">
       <c r="B4" s="39" t="s">
         <v>419</v>
       </c>
@@ -34208,14 +34526,14 @@
       <c r="D18" s="66" t="s">
         <v>583</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="99" t="s">
         <v>584</v>
       </c>
-      <c r="F18" s="94"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="94"/>
-      <c r="I18" s="94"/>
-      <c r="J18" s="94"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="100"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -34227,17 +34545,17 @@
       <c r="D19" s="66" t="s">
         <v>587</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="E19" s="99" t="s">
         <v>588</v>
       </c>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
-      <c r="I19" s="93"/>
-      <c r="J19" s="93"/>
-      <c r="K19" s="93"/>
-      <c r="L19" s="93"/>
-      <c r="M19" s="93"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="99"/>
+      <c r="K19" s="99"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="99"/>
     </row>
     <row r="20" spans="2:13" ht="29">
       <c r="B20" s="7" t="s">
@@ -34260,17 +34578,17 @@
       <c r="D21" s="66" t="s">
         <v>758</v>
       </c>
-      <c r="E21" s="93" t="s">
+      <c r="E21" s="99" t="s">
         <v>759</v>
       </c>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="93"/>
-      <c r="L21" s="93"/>
-      <c r="M21" s="93"/>
+      <c r="F21" s="99"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="99"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -34285,10 +34603,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D61"/>
+  <dimension ref="B2:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -34414,290 +34732,327 @@
         <v>787</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
-      <c r="B18" s="60" t="s">
+    <row r="17" spans="2:4" s="97" customFormat="1">
+      <c r="B17" s="97" t="s">
+        <v>796</v>
+      </c>
+      <c r="C17" s="96" t="s">
+        <v>795</v>
+      </c>
+      <c r="D17" s="94" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" s="97" customFormat="1">
+      <c r="C18" s="96"/>
+      <c r="D18" s="94"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="60" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
-      <c r="B19" s="27" t="s">
+    <row r="21" spans="2:4">
+      <c r="B21" s="27" t="s">
         <v>622</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C21" s="43" t="s">
         <v>623</v>
       </c>
-      <c r="D19" s="61" t="s">
+      <c r="D21" s="61" t="s">
         <v>624</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
-      <c r="B20" s="60"/>
-    </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="60"/>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="60" t="s">
         <v>723</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="27" t="s">
-        <v>619</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>617</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="27" t="s">
-        <v>625</v>
-      </c>
-      <c r="C24" s="43" t="s">
-        <v>627</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="27" t="s">
+        <v>619</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>617</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="27" t="s">
+        <v>625</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>627</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="27" t="s">
         <v>626</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C27" s="43" t="s">
         <v>620</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D27" s="21" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
-      <c r="C26" s="43"/>
-      <c r="D26" s="21"/>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="C27" s="43"/>
-      <c r="D27" s="21"/>
-    </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="97" t="s">
+      <c r="C28" s="43"/>
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="C29" s="43"/>
+      <c r="D29" s="21"/>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="103" t="s">
         <v>790</v>
       </c>
-      <c r="C28" s="98"/>
-      <c r="D28" s="99"/>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="75" t="s">
+      <c r="C30" s="104"/>
+      <c r="D30" s="105"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="75" t="s">
         <v>765</v>
       </c>
-      <c r="C29" s="76"/>
-      <c r="D29" s="77"/>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="85" t="s">
+      <c r="C31" s="76"/>
+      <c r="D31" s="77"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="85" t="s">
         <v>763</v>
-      </c>
-      <c r="C30" s="86"/>
-      <c r="D30" s="87"/>
-    </row>
-    <row r="31" spans="2:4" s="72" customFormat="1" ht="29">
-      <c r="B31" s="79" t="s">
-        <v>764</v>
-      </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="78"/>
-    </row>
-    <row r="32" spans="2:4" s="72" customFormat="1">
-      <c r="B32" s="88" t="s">
-        <v>766</v>
       </c>
       <c r="C32" s="86"/>
       <c r="D32" s="87"/>
     </row>
-    <row r="33" spans="2:4" s="72" customFormat="1">
+    <row r="33" spans="2:4" s="72" customFormat="1" ht="29">
       <c r="B33" s="79" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="C33" s="76"/>
       <c r="D33" s="78"/>
     </row>
     <row r="34" spans="2:4" s="72" customFormat="1">
       <c r="B34" s="88" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C34" s="86"/>
       <c r="D34" s="87"/>
     </row>
-    <row r="35" spans="2:4" s="72" customFormat="1" ht="29">
+    <row r="35" spans="2:4" s="72" customFormat="1">
       <c r="B35" s="79" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C35" s="76"/>
       <c r="D35" s="78"/>
     </row>
-    <row r="36" spans="2:4" s="72" customFormat="1" ht="29">
-      <c r="B36" s="89" t="s">
+    <row r="36" spans="2:4" s="72" customFormat="1">
+      <c r="B36" s="88" t="s">
+        <v>768</v>
+      </c>
+      <c r="C36" s="86"/>
+      <c r="D36" s="87"/>
+    </row>
+    <row r="37" spans="2:4" s="72" customFormat="1" ht="29">
+      <c r="B37" s="79" t="s">
+        <v>769</v>
+      </c>
+      <c r="C37" s="76"/>
+      <c r="D37" s="78"/>
+    </row>
+    <row r="38" spans="2:4" s="72" customFormat="1" ht="29">
+      <c r="B38" s="89" t="s">
         <v>773</v>
       </c>
-      <c r="C36" s="90" t="s">
+      <c r="C38" s="90" t="s">
         <v>770</v>
       </c>
-      <c r="D36" s="91" t="s">
+      <c r="D38" s="91" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="37" spans="2:4" s="72" customFormat="1">
-      <c r="B37" s="80" t="s">
+    <row r="39" spans="2:4" s="72" customFormat="1">
+      <c r="B39" s="80" t="s">
         <v>772</v>
       </c>
-      <c r="C37" s="81" t="s">
+      <c r="C39" s="81" t="s">
         <v>617</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D39" s="40" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="38" spans="2:4" s="72" customFormat="1">
-      <c r="B38" s="89" t="s">
+    <row r="40" spans="2:4" s="72" customFormat="1">
+      <c r="B40" s="89" t="s">
         <v>774</v>
       </c>
-      <c r="C38" s="90" t="s">
+      <c r="C40" s="90" t="s">
         <v>775</v>
       </c>
-      <c r="D38" s="92" t="s">
+      <c r="D40" s="92" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="39" spans="2:4" s="72" customFormat="1" ht="43.5">
-      <c r="B39" s="80" t="s">
+    <row r="41" spans="2:4" s="72" customFormat="1" ht="43.5">
+      <c r="B41" s="80" t="s">
         <v>778</v>
       </c>
-      <c r="C39" s="81" t="s">
+      <c r="C41" s="81" t="s">
         <v>779</v>
       </c>
-      <c r="D39" s="40" t="s">
+      <c r="D41" s="40" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="40" spans="2:4" s="72" customFormat="1" ht="58">
-      <c r="B40" s="89" t="s">
+    <row r="42" spans="2:4" s="72" customFormat="1" ht="58">
+      <c r="B42" s="89" t="s">
         <v>783</v>
       </c>
-      <c r="C40" s="90" t="s">
+      <c r="C42" s="90" t="s">
         <v>780</v>
       </c>
-      <c r="D40" s="92" t="s">
+      <c r="D42" s="92" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="41" spans="2:4" s="72" customFormat="1" ht="29">
-      <c r="B41" s="82" t="s">
+    <row r="43" spans="2:4" s="72" customFormat="1" ht="29">
+      <c r="B43" s="82" t="s">
         <v>791</v>
       </c>
-      <c r="C41" s="83" t="s">
+      <c r="C43" s="83" t="s">
         <v>784</v>
       </c>
-      <c r="D41" s="84" t="s">
+      <c r="D43" s="84" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="42" spans="2:4" s="72" customFormat="1">
-      <c r="B42" s="6"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="69"/>
-    </row>
-    <row r="44" spans="2:4">
-      <c r="B44" s="60" t="s">
+    <row r="44" spans="2:4" s="72" customFormat="1">
+      <c r="B44" s="6"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="69"/>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="60" t="s">
         <v>725</v>
       </c>
     </row>
-    <row r="45" spans="2:4">
-      <c r="B45" s="27" t="s">
+    <row r="47" spans="2:4">
+      <c r="B47" s="27" t="s">
         <v>708</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="C47" s="43" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="48" spans="2:4">
-      <c r="B48" s="60" t="s">
+    <row r="50" spans="2:4">
+      <c r="B50" s="60" t="s">
         <v>712</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4">
-      <c r="B49" s="27" t="s">
-        <v>713</v>
-      </c>
-      <c r="C49" s="43" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="29">
-      <c r="B50" s="38" t="s">
-        <v>715</v>
-      </c>
-      <c r="C50" s="39" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" s="27" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="C51" s="43" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="29">
       <c r="B52" s="38" t="s">
+        <v>715</v>
+      </c>
+      <c r="C52" s="39" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="27" t="s">
+        <v>717</v>
+      </c>
+      <c r="C53" s="43" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="29">
+      <c r="B54" s="38" t="s">
         <v>719</v>
       </c>
-      <c r="C52" s="95" t="s">
+      <c r="C54" s="101" t="s">
         <v>720</v>
       </c>
-      <c r="D52" s="96"/>
-    </row>
-    <row r="55" spans="2:4">
-      <c r="B55" s="60" t="s">
+      <c r="D54" s="102"/>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="60" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="56" spans="2:4">
-      <c r="B56" s="27" t="s">
+    <row r="58" spans="2:4">
+      <c r="B58" s="27" t="s">
         <v>747</v>
       </c>
-      <c r="C56" s="43" t="s">
+      <c r="C58" s="43" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="59" spans="2:4">
-      <c r="B59" s="60" t="s">
+    <row r="61" spans="2:4">
+      <c r="B61" s="60" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="60" spans="2:4" s="68" customFormat="1" ht="116">
-      <c r="B60" s="73" t="s">
+    <row r="62" spans="2:4" s="68" customFormat="1" ht="217.5">
+      <c r="B62" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="C60" s="67" t="s">
+      <c r="C62" s="67" t="s">
+        <v>792</v>
+      </c>
+      <c r="D62" s="74" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="29">
+      <c r="C63" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="D63" s="74" t="s">
         <v>794</v>
       </c>
-      <c r="D60" s="74" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4">
-      <c r="C61" s="2" t="s">
-        <v>761</v>
-      </c>
-      <c r="D61" s="74" t="s">
-        <v>792</v>
+    </row>
+    <row r="64" spans="2:4" ht="58">
+      <c r="B64" s="98" t="s">
+        <v>801</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="D64" s="93" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="29">
+      <c r="B65" s="95" t="s">
+        <v>798</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="D65" s="93" t="s">
+        <v>800</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="B30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -34873,17 +35228,17 @@
       <c r="A2" s="28" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="107" t="s">
         <v>329</v>
       </c>
-      <c r="C2" s="101"/>
+      <c r="C2" s="107"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="108" t="s">
         <v>309</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="108"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -34891,10 +35246,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="109" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="103"/>
+      <c r="B6" s="109"/>
     </row>
     <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="35" t="s">
@@ -35023,88 +35378,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="100" t="s">
+      <c r="A22" s="106" t="s">
         <v>317</v>
       </c>
-      <c r="B22" s="100"/>
-      <c r="C22" s="100"/>
+      <c r="B22" s="106"/>
+      <c r="C22" s="106"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="100" t="s">
+      <c r="A23" s="106" t="s">
         <v>320</v>
       </c>
-      <c r="B23" s="100"/>
-      <c r="C23" s="100"/>
+      <c r="B23" s="106"/>
+      <c r="C23" s="106"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="100" t="s">
+      <c r="A24" s="106" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="100"/>
-      <c r="C24" s="100"/>
+      <c r="B24" s="106"/>
+      <c r="C24" s="106"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="106" t="s">
         <v>326</v>
       </c>
-      <c r="B25" s="100"/>
-      <c r="C25" s="100"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="106"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="100" t="s">
+      <c r="A26" s="106" t="s">
         <v>327</v>
       </c>
-      <c r="B26" s="100"/>
-      <c r="C26" s="100"/>
+      <c r="B26" s="106"/>
+      <c r="C26" s="106"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="100" t="s">
+      <c r="A27" s="106" t="s">
         <v>328</v>
       </c>
-      <c r="B27" s="100"/>
-      <c r="C27" s="100"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="106"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="100" t="s">
+      <c r="A28" s="106" t="s">
         <v>330</v>
       </c>
-      <c r="B28" s="100"/>
-      <c r="C28" s="100"/>
+      <c r="B28" s="106"/>
+      <c r="C28" s="106"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="100" t="s">
+      <c r="A29" s="106" t="s">
         <v>331</v>
       </c>
-      <c r="B29" s="100"/>
-      <c r="C29" s="100"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="106"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="101" t="s">
+      <c r="A30" s="107" t="s">
         <v>332</v>
       </c>
-      <c r="B30" s="101"/>
-      <c r="C30" s="101"/>
+      <c r="B30" s="107"/>
+      <c r="C30" s="107"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="101" t="s">
+      <c r="A31" s="107" t="s">
         <v>340</v>
       </c>
-      <c r="B31" s="101"/>
-      <c r="C31" s="101"/>
+      <c r="B31" s="107"/>
+      <c r="C31" s="107"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="100" t="s">
+      <c r="A32" s="106" t="s">
         <v>341</v>
       </c>
-      <c r="B32" s="100"/>
-      <c r="C32" s="100"/>
+      <c r="B32" s="106"/>
+      <c r="C32" s="106"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="100" t="s">
+      <c r="A33" s="106" t="s">
         <v>342</v>
       </c>
-      <c r="B33" s="100"/>
-      <c r="C33" s="100"/>
+      <c r="B33" s="106"/>
+      <c r="C33" s="106"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
made some minor tweaks to the git tab
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E85B1F9-B664-4B0B-9E8B-7C1D3A5C0A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B52207-E42C-44D4-9315-EAE4D6D0BCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="814">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -26713,9 +26713,6 @@
   </si>
   <si>
     <t>git pull origin main</t>
-  </si>
-  <si>
-    <t>OVERWRITE LOCAL REPO WITH REMOTE REPO</t>
   </si>
   <si>
     <t>CREATE NEW LOCAL REPO FROM REMOTE REPO</t>
@@ -30847,6 +30844,12 @@
   </si>
   <si>
     <t>grep -r Washing *</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OVERWRITE LOCAL REPO WITH REMOTE REPO </t>
+  </si>
+  <si>
+    <t>CD to local main github folder</t>
   </si>
 </sst>
 </file>
@@ -31040,7 +31043,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -31263,44 +31266,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -31356,11 +31323,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -31954,7 +31963,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="107" t="s">
         <v>413</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -31968,7 +31977,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="72.5">
-      <c r="A9" s="86"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="6" t="s">
         <v>402</v>
       </c>
@@ -31980,7 +31989,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="29">
-      <c r="A10" s="86"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="6" t="s">
         <v>403</v>
       </c>
@@ -31992,7 +32001,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="43.5">
-      <c r="A11" s="86"/>
+      <c r="A11" s="107"/>
       <c r="B11" s="6" t="s">
         <v>405</v>
       </c>
@@ -32004,7 +32013,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="43.5">
-      <c r="A12" s="86"/>
+      <c r="A12" s="107"/>
       <c r="B12" s="47" t="s">
         <v>407</v>
       </c>
@@ -32021,7 +32030,7 @@
       <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:13" ht="43.5">
-      <c r="A15" s="87" t="s">
+      <c r="A15" s="108" t="s">
         <v>414</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -32035,7 +32044,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="72.5">
-      <c r="A16" s="87"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="8" t="s">
         <v>412</v>
       </c>
@@ -32047,7 +32056,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="87">
-      <c r="A17" s="87"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="8" t="s">
         <v>517</v>
       </c>
@@ -32059,7 +32068,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="87">
-      <c r="A18" s="87"/>
+      <c r="A18" s="108"/>
       <c r="B18" s="8" t="s">
         <v>518</v>
       </c>
@@ -32071,7 +32080,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" ht="58">
-      <c r="A19" s="87" t="s">
+      <c r="A19" s="108" t="s">
         <v>414</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -32085,7 +32094,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="58">
-      <c r="A20" s="87"/>
+      <c r="A20" s="108"/>
       <c r="B20" s="11" t="s">
         <v>526</v>
       </c>
@@ -32097,7 +32106,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="101.5">
-      <c r="A21" s="87"/>
+      <c r="A21" s="108"/>
       <c r="B21" s="11" t="s">
         <v>529</v>
       </c>
@@ -32109,7 +32118,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="58">
-      <c r="A22" s="87"/>
+      <c r="A22" s="108"/>
       <c r="B22" s="55" t="s">
         <v>531</v>
       </c>
@@ -32458,38 +32467,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="88" t="s">
+      <c r="C19" s="109" t="s">
         <v>688</v>
       </c>
-      <c r="D19" s="88"/>
+      <c r="D19" s="109"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="88" t="s">
+      <c r="C20" s="109" t="s">
         <v>689</v>
       </c>
-      <c r="D20" s="88"/>
+      <c r="D20" s="109"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="88" t="s">
+      <c r="C21" s="109" t="s">
         <v>690</v>
       </c>
-      <c r="D21" s="88"/>
+      <c r="D21" s="109"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="109" t="s">
         <v>691</v>
       </c>
-      <c r="D22" s="88"/>
+      <c r="D22" s="109"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="109" t="s">
         <v>692</v>
       </c>
-      <c r="D23" s="88"/>
+      <c r="D23" s="109"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -32502,38 +32511,38 @@
       <c r="B25" s="63" t="s">
         <v>694</v>
       </c>
-      <c r="C25" s="88" t="s">
+      <c r="C25" s="109" t="s">
         <v>695</v>
       </c>
-      <c r="D25" s="88"/>
+      <c r="D25" s="109"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="88" t="s">
+      <c r="C26" s="109" t="s">
         <v>696</v>
       </c>
-      <c r="D26" s="88"/>
+      <c r="D26" s="109"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="109" t="s">
         <v>697</v>
       </c>
-      <c r="D27" s="88"/>
+      <c r="D27" s="109"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="88" t="s">
+      <c r="C28" s="109" t="s">
         <v>698</v>
       </c>
-      <c r="D28" s="88"/>
+      <c r="D28" s="109"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="88" t="s">
+      <c r="C29" s="109" t="s">
         <v>699</v>
       </c>
-      <c r="D29" s="88"/>
+      <c r="D29" s="109"/>
     </row>
     <row r="30" spans="2:4" ht="39">
       <c r="B30" s="27" t="s">
@@ -32593,38 +32602,38 @@
       </c>
     </row>
     <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="99" t="s">
         <v>708</v>
       </c>
-      <c r="D4" s="80"/>
+      <c r="D4" s="99"/>
     </row>
     <row r="5" spans="2:4" ht="75" customHeight="1">
-      <c r="C5" s="80" t="s">
-        <v>739</v>
-      </c>
-      <c r="D5" s="80"/>
+      <c r="C5" s="99" t="s">
+        <v>738</v>
+      </c>
+      <c r="D5" s="99"/>
     </row>
     <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="80" t="s">
-        <v>737</v>
-      </c>
-      <c r="D6" s="80"/>
+      <c r="C6" s="99" t="s">
+        <v>736</v>
+      </c>
+      <c r="D6" s="99"/>
     </row>
     <row r="7" spans="2:4" ht="75" customHeight="1">
-      <c r="C7" s="80" t="s">
-        <v>727</v>
-      </c>
-      <c r="D7" s="80"/>
+      <c r="C7" s="99" t="s">
+        <v>726</v>
+      </c>
+      <c r="D7" s="99"/>
     </row>
     <row r="9" spans="2:4" ht="75" customHeight="1">
       <c r="B9" s="8" t="s">
+        <v>739</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>740</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>741</v>
-      </c>
       <c r="D9" s="26" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="29">
@@ -32632,18 +32641,18 @@
         <v>706</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="72.5">
       <c r="B11" s="8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>710</v>
@@ -32654,74 +32663,74 @@
         <v>709</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="87">
       <c r="B13" s="8" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="29">
       <c r="B14" s="46" t="s">
+        <v>732</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>734</v>
-      </c>
       <c r="D14" s="19" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="87">
       <c r="B15" s="8" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="105" customHeight="1">
       <c r="B16" s="8" t="s">
+        <v>747</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>748</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>749</v>
-      </c>
       <c r="D16" s="19" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="180" customHeight="1">
       <c r="B17" s="8" t="s">
+        <v>752</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>755</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>754</v>
+      </c>
+      <c r="E17" s="110" t="s">
         <v>753</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>756</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>755</v>
-      </c>
-      <c r="E17" s="89" t="s">
-        <v>754</v>
-      </c>
-      <c r="F17" s="78"/>
-      <c r="G17" s="78"/>
-      <c r="H17" s="78"/>
-      <c r="I17" s="78"/>
-      <c r="J17" s="78"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -33088,12 +33097,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="111" t="s">
         <v>358</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -33101,11 +33110,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="103" t="s">
         <v>359</v>
       </c>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -33123,19 +33132,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="90" t="s">
+      <c r="B11" s="111" t="s">
         <v>364</v>
       </c>
-      <c r="C11" s="90"/>
+      <c r="C11" s="111"/>
       <c r="D11" s="27" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="90" t="s">
+      <c r="B12" s="111" t="s">
         <v>365</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="111"/>
       <c r="D12" s="27" t="s">
         <v>367</v>
       </c>
@@ -33172,7 +33181,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" ht="29">
       <c r="B4" s="39" t="s">
         <v>418</v>
       </c>
@@ -33400,7 +33409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F0B4C89-AE87-4187-8C18-5F20544A3D88}">
   <dimension ref="A3:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -33528,7 +33537,7 @@
         <v>274</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>215</v>
@@ -34686,14 +34695,14 @@
       <c r="D18" s="66" t="s">
         <v>582</v>
       </c>
-      <c r="E18" s="78" t="s">
+      <c r="E18" s="97" t="s">
         <v>583</v>
       </c>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="79"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -34705,17 +34714,17 @@
       <c r="D19" s="66" t="s">
         <v>586</v>
       </c>
-      <c r="E19" s="78" t="s">
+      <c r="E19" s="97" t="s">
         <v>587</v>
       </c>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="78"/>
-      <c r="M19" s="78"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="97"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="97"/>
     </row>
     <row r="20" spans="2:13" ht="29">
       <c r="B20" s="7" t="s">
@@ -34736,19 +34745,19 @@
         <v>592</v>
       </c>
       <c r="D21" s="66" t="s">
+        <v>756</v>
+      </c>
+      <c r="E21" s="97" t="s">
         <v>757</v>
       </c>
-      <c r="E21" s="78" t="s">
-        <v>758</v>
-      </c>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="78"/>
-      <c r="M21" s="78"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="97"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -34763,10 +34772,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
-  <dimension ref="B2:D71"/>
+  <dimension ref="B2:D72"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -34861,7 +34870,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="27" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C14" s="43" t="s">
         <v>720</v>
@@ -34883,24 +34892,24 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="27" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C16" s="70" t="s">
+        <v>784</v>
+      </c>
+      <c r="D16" s="69" t="s">
         <v>785</v>
-      </c>
-      <c r="D16" s="69" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="17" spans="2:4" s="74" customFormat="1">
       <c r="B17" s="74" t="s">
+        <v>793</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>792</v>
+      </c>
+      <c r="D17" s="72" t="s">
         <v>794</v>
-      </c>
-      <c r="C17" s="73" t="s">
-        <v>793</v>
-      </c>
-      <c r="D17" s="72" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="18" spans="2:4" s="74" customFormat="1">
@@ -34909,355 +34918,360 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="60" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="27" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" s="78" customFormat="1">
+      <c r="B21" s="112" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="27" t="s">
         <v>621</v>
       </c>
-      <c r="C21" s="43" t="s">
+      <c r="C22" s="43" t="s">
         <v>622</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="D22" s="61" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="60"/>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="60" t="s">
+    <row r="23" spans="2:4">
+      <c r="B23" s="60"/>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="60" t="s">
         <v>722</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="27" t="s">
-        <v>618</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>616</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="C26" s="43" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27" t="s">
+        <v>624</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>626</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="27" t="s">
         <v>625</v>
       </c>
-      <c r="C27" s="43" t="s">
+      <c r="C28" s="43" t="s">
         <v>619</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D28" s="21" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="C28" s="43"/>
-      <c r="D28" s="21"/>
     </row>
     <row r="29" spans="2:4">
       <c r="C29" s="43"/>
       <c r="D29" s="21"/>
     </row>
     <row r="30" spans="2:4">
-      <c r="B30" s="110" t="s">
+      <c r="C30" s="43"/>
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="101" t="s">
+        <v>788</v>
+      </c>
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="88" t="s">
+        <v>763</v>
+      </c>
+      <c r="C32" s="89"/>
+      <c r="D32" s="90"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="82" t="s">
+        <v>761</v>
+      </c>
+      <c r="C33" s="91"/>
+      <c r="D33" s="82"/>
+    </row>
+    <row r="34" spans="2:4" s="71" customFormat="1" ht="29">
+      <c r="B34" s="85" t="s">
+        <v>762</v>
+      </c>
+      <c r="C34" s="89"/>
+      <c r="D34" s="88"/>
+    </row>
+    <row r="35" spans="2:4" s="71" customFormat="1">
+      <c r="B35" s="92" t="s">
+        <v>764</v>
+      </c>
+      <c r="C35" s="91"/>
+      <c r="D35" s="82"/>
+    </row>
+    <row r="36" spans="2:4" s="71" customFormat="1">
+      <c r="B36" s="85" t="s">
+        <v>765</v>
+      </c>
+      <c r="C36" s="89"/>
+      <c r="D36" s="88"/>
+    </row>
+    <row r="37" spans="2:4" s="71" customFormat="1">
+      <c r="B37" s="92" t="s">
+        <v>766</v>
+      </c>
+      <c r="C37" s="91"/>
+      <c r="D37" s="82"/>
+    </row>
+    <row r="38" spans="2:4" s="71" customFormat="1" ht="29">
+      <c r="B38" s="85" t="s">
+        <v>767</v>
+      </c>
+      <c r="C38" s="89"/>
+      <c r="D38" s="88"/>
+    </row>
+    <row r="39" spans="2:4" s="71" customFormat="1" ht="29">
+      <c r="B39" s="93" t="s">
+        <v>771</v>
+      </c>
+      <c r="C39" s="83" t="s">
+        <v>768</v>
+      </c>
+      <c r="D39" s="84" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" s="71" customFormat="1">
+      <c r="B40" s="94" t="s">
+        <v>770</v>
+      </c>
+      <c r="C40" s="86" t="s">
+        <v>616</v>
+      </c>
+      <c r="D40" s="81" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" s="71" customFormat="1">
+      <c r="B41" s="93" t="s">
+        <v>772</v>
+      </c>
+      <c r="C41" s="83" t="s">
+        <v>773</v>
+      </c>
+      <c r="D41" s="95" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" s="71" customFormat="1" ht="43.5">
+      <c r="B42" s="94" t="s">
+        <v>776</v>
+      </c>
+      <c r="C42" s="86" t="s">
+        <v>777</v>
+      </c>
+      <c r="D42" s="81" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" s="71" customFormat="1" ht="58">
+      <c r="B43" s="93" t="s">
+        <v>781</v>
+      </c>
+      <c r="C43" s="83" t="s">
+        <v>778</v>
+      </c>
+      <c r="D43" s="95" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" s="71" customFormat="1" ht="29">
+      <c r="B44" s="94" t="s">
         <v>789</v>
       </c>
-      <c r="C30" s="110"/>
-      <c r="D30" s="110"/>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31" s="100" t="s">
-        <v>764</v>
-      </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="102"/>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="94" t="s">
-        <v>762</v>
-      </c>
-      <c r="C32" s="103"/>
-      <c r="D32" s="94"/>
-    </row>
-    <row r="33" spans="2:4" s="71" customFormat="1" ht="29">
-      <c r="B33" s="97" t="s">
-        <v>763</v>
-      </c>
-      <c r="C33" s="101"/>
-      <c r="D33" s="100"/>
-    </row>
-    <row r="34" spans="2:4" s="71" customFormat="1">
-      <c r="B34" s="104" t="s">
-        <v>765</v>
-      </c>
-      <c r="C34" s="103"/>
-      <c r="D34" s="94"/>
-    </row>
-    <row r="35" spans="2:4" s="71" customFormat="1">
-      <c r="B35" s="97" t="s">
-        <v>766</v>
-      </c>
-      <c r="C35" s="101"/>
-      <c r="D35" s="100"/>
-    </row>
-    <row r="36" spans="2:4" s="71" customFormat="1">
-      <c r="B36" s="104" t="s">
-        <v>767</v>
-      </c>
-      <c r="C36" s="103"/>
-      <c r="D36" s="94"/>
-    </row>
-    <row r="37" spans="2:4" s="71" customFormat="1" ht="29">
-      <c r="B37" s="97" t="s">
-        <v>768</v>
-      </c>
-      <c r="C37" s="101"/>
-      <c r="D37" s="100"/>
-    </row>
-    <row r="38" spans="2:4" s="71" customFormat="1" ht="29">
-      <c r="B38" s="105" t="s">
-        <v>772</v>
-      </c>
-      <c r="C38" s="95" t="s">
-        <v>769</v>
-      </c>
-      <c r="D38" s="96" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" s="71" customFormat="1">
-      <c r="B39" s="106" t="s">
-        <v>771</v>
-      </c>
-      <c r="C39" s="98" t="s">
-        <v>616</v>
-      </c>
-      <c r="D39" s="93" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" s="71" customFormat="1">
-      <c r="B40" s="105" t="s">
-        <v>773</v>
-      </c>
-      <c r="C40" s="95" t="s">
-        <v>774</v>
-      </c>
-      <c r="D40" s="107" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" s="71" customFormat="1" ht="43.5">
-      <c r="B41" s="106" t="s">
-        <v>777</v>
-      </c>
-      <c r="C41" s="98" t="s">
-        <v>778</v>
-      </c>
-      <c r="D41" s="93" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" s="71" customFormat="1" ht="58">
-      <c r="B42" s="105" t="s">
+      <c r="C44" s="86" t="s">
         <v>782</v>
       </c>
-      <c r="C42" s="95" t="s">
-        <v>779</v>
-      </c>
-      <c r="D42" s="107" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" s="71" customFormat="1" ht="29">
-      <c r="B43" s="106" t="s">
+      <c r="D44" s="96" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" s="71" customFormat="1">
+      <c r="B45" s="6"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="68"/>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="60" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="27" t="s">
+        <v>707</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="60" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="27" t="s">
+        <v>712</v>
+      </c>
+      <c r="C52" s="43" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="29">
+      <c r="B53" s="38" t="s">
+        <v>714</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4">
+      <c r="B54" s="27" t="s">
+        <v>716</v>
+      </c>
+      <c r="C54" s="43" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="29">
+      <c r="B55" s="38" t="s">
+        <v>718</v>
+      </c>
+      <c r="C55" s="99" t="s">
+        <v>719</v>
+      </c>
+      <c r="D55" s="100"/>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="B58" s="60" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="27" t="s">
+        <v>745</v>
+      </c>
+      <c r="C59" s="43" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="101" t="s">
+        <v>758</v>
+      </c>
+      <c r="C62" s="101"/>
+      <c r="D62" s="101"/>
+    </row>
+    <row r="63" spans="2:4" s="67" customFormat="1" ht="217.5">
+      <c r="B63" s="79" t="s">
+        <v>760</v>
+      </c>
+      <c r="C63" s="80" t="s">
         <v>790</v>
       </c>
-      <c r="C43" s="98" t="s">
-        <v>783</v>
-      </c>
-      <c r="D43" s="108" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" s="71" customFormat="1">
-      <c r="B44" s="6"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="68"/>
-    </row>
-    <row r="46" spans="2:4">
-      <c r="B46" s="60" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4">
-      <c r="B47" s="27" t="s">
-        <v>707</v>
-      </c>
-      <c r="C47" s="43" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4">
-      <c r="B50" s="60" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4">
-      <c r="B51" s="27" t="s">
-        <v>712</v>
-      </c>
-      <c r="C51" s="43" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" ht="29">
-      <c r="B52" s="38" t="s">
-        <v>714</v>
-      </c>
-      <c r="C52" s="39" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4">
-      <c r="B53" s="27" t="s">
-        <v>716</v>
-      </c>
-      <c r="C53" s="43" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" ht="29">
-      <c r="B54" s="38" t="s">
-        <v>718</v>
-      </c>
-      <c r="C54" s="80" t="s">
-        <v>719</v>
-      </c>
-      <c r="D54" s="81"/>
-    </row>
-    <row r="57" spans="2:4">
-      <c r="B57" s="60" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4">
-      <c r="B58" s="27" t="s">
-        <v>746</v>
-      </c>
-      <c r="C58" s="43" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4">
-      <c r="B61" s="110" t="s">
+      <c r="D63" s="81" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="29">
+      <c r="B64" s="82"/>
+      <c r="C64" s="83" t="s">
         <v>759</v>
       </c>
-      <c r="C61" s="110"/>
-      <c r="D61" s="110"/>
-    </row>
-    <row r="62" spans="2:4" s="67" customFormat="1" ht="217.5">
-      <c r="B62" s="91" t="s">
-        <v>761</v>
-      </c>
-      <c r="C62" s="92" t="s">
-        <v>791</v>
-      </c>
-      <c r="D62" s="93" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" ht="29">
-      <c r="B63" s="94"/>
-      <c r="C63" s="95" t="s">
-        <v>760</v>
-      </c>
-      <c r="D63" s="96" t="s">
+      <c r="D64" s="84" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="72.5">
+      <c r="B65" s="85" t="s">
+        <v>798</v>
+      </c>
+      <c r="C65" s="86" t="s">
+        <v>799</v>
+      </c>
+      <c r="D65" s="81" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="64" spans="2:4" ht="72.5">
-      <c r="B64" s="97" t="s">
-        <v>799</v>
-      </c>
-      <c r="C64" s="98" t="s">
-        <v>800</v>
-      </c>
-      <c r="D64" s="93" t="s">
+    <row r="66" spans="2:4" ht="29">
+      <c r="B66" s="87" t="s">
+        <v>795</v>
+      </c>
+      <c r="C66" s="83" t="s">
+        <v>796</v>
+      </c>
+      <c r="D66" s="84" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="102" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" ht="29">
-      <c r="B65" s="99" t="s">
-        <v>796</v>
-      </c>
-      <c r="C65" s="95" t="s">
-        <v>797</v>
-      </c>
-      <c r="D65" s="96" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="68" spans="2:4">
-      <c r="B68" s="109" t="s">
-        <v>803</v>
-      </c>
-      <c r="C68" s="109"/>
-      <c r="D68" s="109"/>
-    </row>
-    <row r="69" spans="2:4">
-      <c r="B69" s="76" t="s">
-        <v>804</v>
-      </c>
-      <c r="C69" s="76" t="s">
-        <v>804</v>
-      </c>
-      <c r="D69" s="75" t="s">
-        <v>805</v>
-      </c>
+      <c r="C69" s="102"/>
+      <c r="D69" s="102"/>
     </row>
     <row r="70" spans="2:4">
       <c r="B70" s="76" t="s">
+        <v>803</v>
+      </c>
+      <c r="C70" s="76" t="s">
+        <v>803</v>
+      </c>
+      <c r="D70" s="75" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" s="76" t="s">
+        <v>807</v>
+      </c>
+      <c r="C71" s="76" t="s">
+        <v>805</v>
+      </c>
+      <c r="D71" s="75" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="29">
+      <c r="B72" s="77" t="s">
         <v>808</v>
       </c>
-      <c r="C70" s="76" t="s">
-        <v>806</v>
-      </c>
-      <c r="D70" s="75" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" ht="29">
-      <c r="B71" s="77" t="s">
+      <c r="C72" s="2" t="s">
         <v>809</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="D72" s="75" t="s">
         <v>810</v>
-      </c>
-      <c r="D71" s="75" t="s">
-        <v>811</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B69:D69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -35433,17 +35447,17 @@
       <c r="A2" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="104" t="s">
         <v>328</v>
       </c>
-      <c r="C2" s="83"/>
+      <c r="C2" s="104"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="105" t="s">
         <v>308</v>
       </c>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -35451,10 +35465,10 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="85" t="s">
+      <c r="A6" s="106" t="s">
         <v>322</v>
       </c>
-      <c r="B6" s="85"/>
+      <c r="B6" s="106"/>
     </row>
     <row r="7" spans="1:4" ht="43.5">
       <c r="A7" s="35" t="s">
@@ -35583,88 +35597,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="103" t="s">
         <v>316</v>
       </c>
-      <c r="B22" s="82"/>
-      <c r="C22" s="82"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="103"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="82" t="s">
+      <c r="A23" s="103" t="s">
         <v>319</v>
       </c>
-      <c r="B23" s="82"/>
-      <c r="C23" s="82"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="103"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="82" t="s">
+      <c r="A24" s="103" t="s">
         <v>323</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="82"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="103"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="82" t="s">
+      <c r="A25" s="103" t="s">
         <v>325</v>
       </c>
-      <c r="B25" s="82"/>
-      <c r="C25" s="82"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="103"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="103" t="s">
         <v>326</v>
       </c>
-      <c r="B26" s="82"/>
-      <c r="C26" s="82"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="103"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="103" t="s">
         <v>327</v>
       </c>
-      <c r="B27" s="82"/>
-      <c r="C27" s="82"/>
+      <c r="B27" s="103"/>
+      <c r="C27" s="103"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="B28" s="82"/>
-      <c r="C28" s="82"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="103"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="82" t="s">
+      <c r="A29" s="103" t="s">
         <v>330</v>
       </c>
-      <c r="B29" s="82"/>
-      <c r="C29" s="82"/>
+      <c r="B29" s="103"/>
+      <c r="C29" s="103"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="83" t="s">
+      <c r="A30" s="104" t="s">
         <v>331</v>
       </c>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
+      <c r="B30" s="104"/>
+      <c r="C30" s="104"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="83" t="s">
+      <c r="A31" s="104" t="s">
         <v>339</v>
       </c>
-      <c r="B31" s="83"/>
-      <c r="C31" s="83"/>
+      <c r="B31" s="104"/>
+      <c r="C31" s="104"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="103" t="s">
         <v>340</v>
       </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="82" t="s">
+      <c r="A33" s="103" t="s">
         <v>341</v>
       </c>
-      <c r="B33" s="82"/>
-      <c r="C33" s="82"/>
+      <c r="B33" s="103"/>
+      <c r="C33" s="103"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>

<commit_message>
updated 'iptables' tab with more info
</commit_message>
<xml_diff>
--- a/Linux_cmd_master_sheet.xlsx
+++ b/Linux_cmd_master_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoyle\github\Linux-cmds-cheat-sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoyle\git\Linux-cmds-cheat-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B52207-E42C-44D4-9315-EAE4D6D0BCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5946E5B-399D-4889-B348-6F37DD328DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="11" xr2:uid="{3287689C-6E77-4F11-B67F-07FDB207D0E0}"/>
   </bookViews>
   <sheets>
     <sheet name="ls" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="814">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="815">
   <si>
     <t>Linux cmd 'LS'</t>
   </si>
@@ -26485,143 +26485,6 @@
   </si>
   <si>
     <t>fetch all remote repo differences</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">host firewall installed by default on Linux systems. 
-It uses 3 lists or 'chains':
-Input chain: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>list that</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>controls behavior for incoming connections</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Forward chain: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">list that controls incoming connections not meant for the local system but rather just being passed through or 'forwarded' on to another destination
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Output chain: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">list that controls how data being sent </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">out </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">of the local host to another destination is handled
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">IMPORTANT: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>almost all connections need to talk back and forth, so both 'input' and 'output' chains are used!</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-https://www.howtogeek.com/177621/the-beginners-guide-to-iptables-the-linux-firewall/</t>
-    </r>
   </si>
   <si>
     <r>
@@ -30850,6 +30713,152 @@
   </si>
   <si>
     <t>CD to local main github folder</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">host firewall installed by default on Linux systems
+(packet filter rules in Linux kernel)
+It uses 3 lists or 'chains':
+Input chain: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>list that</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>controls behavior for incoming connections</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Forward chain: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">list that controls incoming connections not meant for the local system but rather just being passed through or 'forwarded' on to another destination
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Output chain: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">list that controls how data being sent </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">of the local host to another destination is handled
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">IMPORTANT: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>almost all connections need to talk back and forth, so both 'input' and 'output' chains are used!</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+https://www.howtogeek.com/177621/the-beginners-guide-to-iptables-the-linux-firewall/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">setup, maintain, and inspect the tables of packet filter rules in the Linux kernel.
+A table consists of a number of built-in 'chains' and may also contain user-defined 'chains'.
+A chain contains a list of 'rules' that specify what to do with a packet it matches.
+A 'target' is what action is taken with a packet that matches a 'rule'.
+A 'target' may be a 'jump' (go-to action) to a user-defined 'chain' in the same 'table'
+</t>
   </si>
 </sst>
 </file>
@@ -31043,7 +31052,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -31233,43 +31242,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -31295,9 +31268,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -31367,9 +31337,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -31692,11 +31659,11 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -31731,7 +31698,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="29">
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="7" t="s">
         <v>63</v>
       </c>
@@ -31742,7 +31709,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="159.5">
+    <row r="9" spans="1:3" ht="165">
       <c r="A9" s="7" t="s">
         <v>66</v>
       </c>
@@ -31753,7 +31720,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="59.5" customHeight="1">
+    <row r="10" spans="1:3" ht="59.45" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>82</v>
       </c>
@@ -31764,7 +31731,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="58">
+    <row r="11" spans="1:3" ht="60">
       <c r="A11" s="8" t="s">
         <v>67</v>
       </c>
@@ -31775,7 +31742,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="58">
+    <row r="12" spans="1:3" ht="60">
       <c r="A12" s="8" t="s">
         <v>68</v>
       </c>
@@ -31797,7 +31764,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" ht="30">
       <c r="A14" s="8" t="s">
         <v>170</v>
       </c>
@@ -31808,7 +31775,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29">
+    <row r="15" spans="1:3" ht="30">
       <c r="A15" s="8" t="s">
         <v>169</v>
       </c>
@@ -31841,7 +31808,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29">
+    <row r="18" spans="1:3" ht="30">
       <c r="A18" s="8" t="s">
         <v>78</v>
       </c>
@@ -31899,11 +31866,11 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.7265625" customWidth="1"/>
-    <col min="3" max="4" width="55.7265625" customWidth="1"/>
-    <col min="5" max="5" width="59.7265625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="4" width="55.7109375" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
@@ -31913,7 +31880,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:13" ht="101.5">
+    <row r="3" spans="1:13" ht="120">
       <c r="A3" s="28"/>
       <c r="B3" s="3"/>
       <c r="C3" s="39" t="s">
@@ -31963,7 +31930,7 @@
       <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="107" t="s">
+      <c r="A8" s="94" t="s">
         <v>413</v>
       </c>
       <c r="B8" s="48" t="s">
@@ -31976,8 +31943,8 @@
         <v>398</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="72.5">
-      <c r="A9" s="107"/>
+    <row r="9" spans="1:13" ht="75">
+      <c r="A9" s="94"/>
       <c r="B9" s="6" t="s">
         <v>402</v>
       </c>
@@ -31988,8 +31955,8 @@
         <v>406</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="29">
-      <c r="A10" s="107"/>
+    <row r="10" spans="1:13" ht="30">
+      <c r="A10" s="94"/>
       <c r="B10" s="6" t="s">
         <v>403</v>
       </c>
@@ -32000,8 +31967,8 @@
         <v>513</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="43.5">
-      <c r="A11" s="107"/>
+    <row r="11" spans="1:13" ht="45">
+      <c r="A11" s="94"/>
       <c r="B11" s="6" t="s">
         <v>405</v>
       </c>
@@ -32012,8 +31979,8 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="43.5">
-      <c r="A12" s="107"/>
+    <row r="12" spans="1:13" ht="45">
+      <c r="A12" s="94"/>
       <c r="B12" s="47" t="s">
         <v>407</v>
       </c>
@@ -32029,8 +31996,8 @@
       <c r="C14" s="9"/>
       <c r="D14" s="19"/>
     </row>
-    <row r="15" spans="1:13" ht="43.5">
-      <c r="A15" s="108" t="s">
+    <row r="15" spans="1:13" ht="60">
+      <c r="A15" s="95" t="s">
         <v>414</v>
       </c>
       <c r="B15" s="51" t="s">
@@ -32043,8 +32010,8 @@
         <v>411</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="72.5">
-      <c r="A16" s="108"/>
+    <row r="16" spans="1:13" ht="75">
+      <c r="A16" s="95"/>
       <c r="B16" s="8" t="s">
         <v>412</v>
       </c>
@@ -32055,8 +32022,8 @@
         <v>522</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="87">
-      <c r="A17" s="108"/>
+    <row r="17" spans="1:13" ht="105">
+      <c r="A17" s="95"/>
       <c r="B17" s="8" t="s">
         <v>517</v>
       </c>
@@ -32067,8 +32034,8 @@
         <v>523</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="87">
-      <c r="A18" s="108"/>
+    <row r="18" spans="1:13" ht="105">
+      <c r="A18" s="95"/>
       <c r="B18" s="8" t="s">
         <v>518</v>
       </c>
@@ -32079,8 +32046,8 @@
         <v>524</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="58">
-      <c r="A19" s="108" t="s">
+    <row r="19" spans="1:13" ht="60">
+      <c r="A19" s="95" t="s">
         <v>414</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -32093,8 +32060,8 @@
         <v>525</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="58">
-      <c r="A20" s="108"/>
+    <row r="20" spans="1:13" ht="60">
+      <c r="A20" s="95"/>
       <c r="B20" s="11" t="s">
         <v>526</v>
       </c>
@@ -32105,8 +32072,8 @@
         <v>528</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="101.5">
-      <c r="A21" s="108"/>
+    <row r="21" spans="1:13" ht="105">
+      <c r="A21" s="95"/>
       <c r="B21" s="11" t="s">
         <v>529</v>
       </c>
@@ -32117,8 +32084,8 @@
         <v>540</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="58">
-      <c r="A22" s="108"/>
+    <row r="22" spans="1:13" ht="60">
+      <c r="A22" s="95"/>
       <c r="B22" s="55" t="s">
         <v>531</v>
       </c>
@@ -32151,7 +32118,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
     </row>
-    <row r="25" spans="1:13" ht="130.5">
+    <row r="25" spans="1:13" ht="150">
       <c r="B25" s="11" t="s">
         <v>537</v>
       </c>
@@ -32173,7 +32140,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" ht="145">
+    <row r="26" spans="1:13" ht="150">
       <c r="A26" s="28"/>
       <c r="B26" s="11" t="s">
         <v>628</v>
@@ -32196,7 +32163,7 @@
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
     </row>
-    <row r="27" spans="1:13" ht="145">
+    <row r="27" spans="1:13" ht="165">
       <c r="B27" s="11" t="s">
         <v>631</v>
       </c>
@@ -32216,7 +32183,7 @@
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
     </row>
-    <row r="28" spans="1:13" ht="200.15" customHeight="1">
+    <row r="28" spans="1:13" ht="200.1" customHeight="1">
       <c r="B28" s="11" t="s">
         <v>634</v>
       </c>
@@ -32252,7 +32219,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="211" customHeight="1">
+    <row r="30" spans="1:13" ht="210.95" customHeight="1">
       <c r="B30" s="11" t="s">
         <v>642</v>
       </c>
@@ -32266,7 +32233,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="232">
+    <row r="31" spans="1:13" ht="270">
       <c r="B31" s="11" t="s">
         <v>646</v>
       </c>
@@ -32280,7 +32247,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="72.5">
+    <row r="32" spans="1:13" ht="75">
       <c r="B32" s="11" t="s">
         <v>650</v>
       </c>
@@ -32309,10 +32276,10 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="28.7265625" customWidth="1"/>
-    <col min="3" max="4" width="53.7265625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="4" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4">
@@ -32467,38 +32434,38 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="27"/>
-      <c r="C19" s="109" t="s">
+      <c r="C19" s="96" t="s">
         <v>688</v>
       </c>
-      <c r="D19" s="109"/>
+      <c r="D19" s="96"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="27"/>
-      <c r="C20" s="109" t="s">
+      <c r="C20" s="96" t="s">
         <v>689</v>
       </c>
-      <c r="D20" s="109"/>
+      <c r="D20" s="96"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="27"/>
-      <c r="C21" s="109" t="s">
+      <c r="C21" s="96" t="s">
         <v>690</v>
       </c>
-      <c r="D21" s="109"/>
+      <c r="D21" s="96"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="27"/>
-      <c r="C22" s="109" t="s">
+      <c r="C22" s="96" t="s">
         <v>691</v>
       </c>
-      <c r="D22" s="109"/>
+      <c r="D22" s="96"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="27"/>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="96" t="s">
         <v>692</v>
       </c>
-      <c r="D23" s="109"/>
+      <c r="D23" s="96"/>
     </row>
     <row r="24" spans="2:4">
       <c r="B24" s="63" t="s">
@@ -32511,40 +32478,40 @@
       <c r="B25" s="63" t="s">
         <v>694</v>
       </c>
-      <c r="C25" s="109" t="s">
+      <c r="C25" s="96" t="s">
         <v>695</v>
       </c>
-      <c r="D25" s="109"/>
+      <c r="D25" s="96"/>
     </row>
     <row r="26" spans="2:4">
       <c r="B26" s="27"/>
-      <c r="C26" s="109" t="s">
+      <c r="C26" s="96" t="s">
         <v>696</v>
       </c>
-      <c r="D26" s="109"/>
+      <c r="D26" s="96"/>
     </row>
     <row r="27" spans="2:4">
       <c r="B27" s="27"/>
-      <c r="C27" s="109" t="s">
+      <c r="C27" s="96" t="s">
         <v>697</v>
       </c>
-      <c r="D27" s="109"/>
+      <c r="D27" s="96"/>
     </row>
     <row r="28" spans="2:4">
       <c r="B28" s="27"/>
-      <c r="C28" s="109" t="s">
+      <c r="C28" s="96" t="s">
         <v>698</v>
       </c>
-      <c r="D28" s="109"/>
+      <c r="D28" s="96"/>
     </row>
     <row r="29" spans="2:4">
       <c r="B29" s="27"/>
-      <c r="C29" s="109" t="s">
+      <c r="C29" s="96" t="s">
         <v>699</v>
       </c>
-      <c r="D29" s="109"/>
-    </row>
-    <row r="30" spans="2:4" ht="39">
+      <c r="D29" s="96"/>
+    </row>
+    <row r="30" spans="2:4" ht="38.25">
       <c r="B30" s="27" t="s">
         <v>700</v>
       </c>
@@ -32581,164 +32548,176 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C8E1A6-37F1-4C42-99E1-83B41D1CB98D}">
-  <dimension ref="B3:J17"/>
+  <dimension ref="B3:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="27"/>
-    <col min="2" max="2" width="43.7265625" style="27" customWidth="1"/>
-    <col min="3" max="3" width="51.81640625" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.7265625" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="27"/>
+    <col min="1" max="1" width="9.140625" style="27"/>
+    <col min="2" max="2" width="43.7109375" style="27" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.7109375" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:13">
       <c r="B3" s="43" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="120" customHeight="1">
-      <c r="C4" s="99" t="s">
-        <v>708</v>
-      </c>
-      <c r="D4" s="99"/>
-    </row>
-    <row r="5" spans="2:4" ht="75" customHeight="1">
-      <c r="C5" s="99" t="s">
+    <row r="4" spans="2:13" ht="120" customHeight="1">
+      <c r="C4" s="86" t="s">
+        <v>813</v>
+      </c>
+      <c r="D4" s="86"/>
+      <c r="E4" s="91" t="s">
+        <v>814</v>
+      </c>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+    </row>
+    <row r="5" spans="2:13" ht="75" customHeight="1">
+      <c r="C5" s="86" t="s">
+        <v>737</v>
+      </c>
+      <c r="D5" s="86"/>
+    </row>
+    <row r="6" spans="2:13" ht="90" customHeight="1">
+      <c r="C6" s="86" t="s">
+        <v>735</v>
+      </c>
+      <c r="D6" s="86"/>
+    </row>
+    <row r="7" spans="2:13" ht="75" customHeight="1">
+      <c r="C7" s="86" t="s">
+        <v>725</v>
+      </c>
+      <c r="D7" s="86"/>
+    </row>
+    <row r="9" spans="2:13" ht="75" customHeight="1">
+      <c r="B9" s="8" t="s">
         <v>738</v>
       </c>
-      <c r="D5" s="99"/>
-    </row>
-    <row r="6" spans="2:4" ht="90" customHeight="1">
-      <c r="C6" s="99" t="s">
-        <v>736</v>
-      </c>
-      <c r="D6" s="99"/>
-    </row>
-    <row r="7" spans="2:4" ht="75" customHeight="1">
-      <c r="C7" s="99" t="s">
-        <v>726</v>
-      </c>
-      <c r="D7" s="99"/>
-    </row>
-    <row r="9" spans="2:4" ht="75" customHeight="1">
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>739</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>740</v>
-      </c>
       <c r="D9" s="26" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="29">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="30">
       <c r="B10" s="45" t="s">
         <v>706</v>
       </c>
       <c r="C10" s="43" t="s">
+        <v>726</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="75">
+      <c r="B11" s="8" t="s">
+        <v>724</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>729</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="60">
+      <c r="B12" s="10" t="s">
+        <v>708</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D12" s="19" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="72.5">
-      <c r="B11" s="8" t="s">
-        <v>725</v>
-      </c>
-      <c r="C11" s="9" t="s">
+    <row r="13" spans="2:13" ht="90">
+      <c r="B13" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="58">
-      <c r="B12" s="10" t="s">
-        <v>709</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="87">
-      <c r="B13" s="8" t="s">
+      <c r="D13" s="19" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="30">
+      <c r="B14" s="46" t="s">
         <v>731</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>729</v>
-      </c>
-      <c r="D13" s="19" t="s">
+      <c r="C14" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="90">
+      <c r="B15" s="8" t="s">
+        <v>741</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" ht="105" customHeight="1">
+      <c r="B16" s="8" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="29">
-      <c r="B14" s="46" t="s">
-        <v>732</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>733</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="87">
-      <c r="B15" s="8" t="s">
-        <v>742</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="C16" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>749</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="105" customHeight="1">
-      <c r="B16" s="8" t="s">
-        <v>747</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>748</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="180" customHeight="1">
       <c r="B17" s="8" t="s">
+        <v>751</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>754</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>753</v>
+      </c>
+      <c r="E17" s="97" t="s">
         <v>752</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>755</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>754</v>
-      </c>
-      <c r="E17" s="110" t="s">
-        <v>753</v>
-      </c>
-      <c r="F17" s="97"/>
-      <c r="G17" s="97"/>
-      <c r="H17" s="97"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="97"/>
+      <c r="F17" s="84"/>
+      <c r="G17" s="84"/>
+      <c r="H17" s="84"/>
+      <c r="I17" s="84"/>
+      <c r="J17" s="84"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E17:J17"/>
+    <mergeCell ref="E4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -32753,16 +32732,16 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="27"/>
-    <col min="2" max="2" width="43.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.54296875" style="27" customWidth="1"/>
-    <col min="5" max="5" width="34.453125" style="27" customWidth="1"/>
-    <col min="6" max="6" width="42.453125" style="27" customWidth="1"/>
-    <col min="7" max="8" width="40.54296875" style="27" customWidth="1"/>
-    <col min="9" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="8.85546875" style="27"/>
+    <col min="2" max="2" width="43.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="34.42578125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" style="27" customWidth="1"/>
+    <col min="7" max="8" width="40.5703125" style="27" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8">
@@ -32775,7 +32754,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="29.5" customHeight="1">
+    <row r="5" spans="2:8" ht="29.45" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>465</v>
       </c>
@@ -32799,7 +32778,7 @@
       </c>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" spans="2:8" ht="29.15" customHeight="1">
+    <row r="7" spans="2:8" ht="29.1" customHeight="1">
       <c r="C7" s="27" t="s">
         <v>464</v>
       </c>
@@ -32808,7 +32787,7 @@
       </c>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="2:8" ht="43.5">
+    <row r="8" spans="2:8" ht="45">
       <c r="C8" s="27" t="s">
         <v>466</v>
       </c>
@@ -32825,7 +32804,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="2:8" ht="29">
+    <row r="11" spans="2:8" ht="30">
       <c r="B11" s="10" t="s">
         <v>476</v>
       </c>
@@ -32837,7 +32816,7 @@
       </c>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="2:8" ht="115.4" customHeight="1">
+    <row r="12" spans="2:8" ht="115.35" customHeight="1">
       <c r="B12" s="10" t="s">
         <v>471</v>
       </c>
@@ -32849,7 +32828,7 @@
       </c>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="2:8" ht="43.5">
+    <row r="13" spans="2:8" ht="45">
       <c r="B13" s="46" t="s">
         <v>458</v>
       </c>
@@ -32861,7 +32840,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="2:8" ht="29">
+    <row r="14" spans="2:8" ht="30">
       <c r="B14" s="46" t="s">
         <v>477</v>
       </c>
@@ -32873,7 +32852,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="2:8" ht="101.15" customHeight="1">
+    <row r="15" spans="2:8" ht="101.1" customHeight="1">
       <c r="B15" s="8" t="s">
         <v>480</v>
       </c>
@@ -32885,7 +32864,7 @@
       </c>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="2:8" ht="72.5">
+    <row r="16" spans="2:8" ht="75">
       <c r="B16" s="8" t="s">
         <v>494</v>
       </c>
@@ -32908,7 +32887,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="58">
+    <row r="17" spans="2:8" ht="90">
       <c r="B17" s="8" t="s">
         <v>493</v>
       </c>
@@ -32923,7 +32902,7 @@
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
     </row>
-    <row r="18" spans="2:8" ht="43.5">
+    <row r="18" spans="2:8" ht="45">
       <c r="B18" s="8" t="s">
         <v>490</v>
       </c>
@@ -32938,7 +32917,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
-    <row r="19" spans="2:8" ht="72.5">
+    <row r="19" spans="2:8" ht="75">
       <c r="B19" s="8" t="s">
         <v>495</v>
       </c>
@@ -32953,7 +32932,7 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
-    <row r="20" spans="2:8" ht="116">
+    <row r="20" spans="2:8" ht="120">
       <c r="B20" s="8" t="s">
         <v>500</v>
       </c>
@@ -32970,7 +32949,7 @@
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
-    <row r="21" spans="2:8" ht="43.4" customHeight="1">
+    <row r="21" spans="2:8" ht="43.35" customHeight="1">
       <c r="B21" s="8" t="s">
         <v>503</v>
       </c>
@@ -32985,7 +32964,7 @@
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
-    <row r="22" spans="2:8" ht="87">
+    <row r="22" spans="2:8" ht="90">
       <c r="B22" s="8" t="s">
         <v>509</v>
       </c>
@@ -33000,7 +32979,7 @@
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" ht="30">
       <c r="B23" s="8" t="s">
         <v>542</v>
       </c>
@@ -33029,7 +33008,7 @@
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
-    <row r="26" spans="2:8" ht="29">
+    <row r="26" spans="2:8" ht="30">
       <c r="B26" s="10" t="s">
         <v>504</v>
       </c>
@@ -33065,7 +33044,7 @@
       </c>
       <c r="E29" s="21"/>
     </row>
-    <row r="30" spans="2:8" ht="29">
+    <row r="30" spans="2:8" ht="30">
       <c r="B30" s="46" t="s">
         <v>508</v>
       </c>
@@ -33076,7 +33055,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="14.5" customHeight="1"/>
+    <row r="32" spans="2:8" ht="14.45" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="4294967295" r:id="rId1"/>
@@ -33091,18 +33070,18 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="98" t="s">
         <v>358</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="27" t="s">
@@ -33110,11 +33089,11 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="90" t="s">
         <v>359</v>
       </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="103"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="27" t="s">
@@ -33132,19 +33111,19 @@
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="111" t="s">
+      <c r="B11" s="98" t="s">
         <v>364</v>
       </c>
-      <c r="C11" s="111"/>
+      <c r="C11" s="98"/>
       <c r="D11" s="27" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="111" t="s">
+      <c r="B12" s="98" t="s">
         <v>365</v>
       </c>
-      <c r="C12" s="111"/>
+      <c r="C12" s="98"/>
       <c r="D12" s="27" t="s">
         <v>367</v>
       </c>
@@ -33168,12 +33147,12 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="16.42578125" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -33181,13 +33160,13 @@
         <v>417</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29">
+    <row r="4" spans="1:3" ht="30">
       <c r="B4" s="39" t="s">
         <v>418</v>
       </c>
       <c r="C4" s="38"/>
     </row>
-    <row r="6" spans="1:3" ht="87">
+    <row r="6" spans="1:3" ht="90">
       <c r="A6" s="44" t="s">
         <v>419</v>
       </c>
@@ -33212,12 +33191,12 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -33230,7 +33209,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="46" t="s">
         <v>429</v>
       </c>
@@ -33265,12 +33244,12 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -33283,7 +33262,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="46" t="s">
         <v>437</v>
       </c>
@@ -33294,7 +33273,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29">
+    <row r="7" spans="1:3" ht="30">
       <c r="A7" s="46" t="s">
         <v>440</v>
       </c>
@@ -33318,12 +33297,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="38" customWidth="1"/>
-    <col min="2" max="2" width="26.54296875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="38" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="38"/>
+    <col min="1" max="1" width="23.5703125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="38" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="38"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -33331,12 +33310,12 @@
         <v>443</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29">
+    <row r="4" spans="1:3" ht="30">
       <c r="B4" s="39" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="46" t="s">
         <v>445</v>
       </c>
@@ -33347,7 +33326,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29">
+    <row r="7" spans="1:3" ht="30">
       <c r="A7" s="46" t="s">
         <v>447</v>
       </c>
@@ -33371,12 +33350,12 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="43.54296875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="54.54296875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="23.5703125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" style="27" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:3">
@@ -33384,12 +33363,12 @@
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="43.5">
+    <row r="4" spans="1:3" ht="45">
       <c r="B4" s="39" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29">
+    <row r="6" spans="1:3" ht="30">
       <c r="A6" s="46" t="s">
         <v>425</v>
       </c>
@@ -33413,12 +33392,12 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.453125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="63.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4">
@@ -33427,7 +33406,7 @@
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="43.5">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
@@ -33448,7 +33427,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="43.5">
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -33460,7 +33439,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="43.5">
+    <row r="8" spans="1:4" ht="45">
       <c r="A8" s="7" t="s">
         <v>87</v>
       </c>
@@ -33472,7 +33451,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" ht="72.5">
+    <row r="9" spans="1:4" ht="90">
       <c r="A9" s="8" t="s">
         <v>269</v>
       </c>
@@ -33484,7 +33463,7 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" ht="43.5">
+    <row r="10" spans="1:4" ht="45">
       <c r="A10" s="8" t="s">
         <v>17</v>
       </c>
@@ -33496,7 +33475,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="58">
+    <row r="11" spans="1:4" ht="75">
       <c r="A11" s="8" t="s">
         <v>264</v>
       </c>
@@ -33508,7 +33487,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" s="12" customFormat="1" ht="43.5">
+    <row r="12" spans="1:4" s="12" customFormat="1" ht="45">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
@@ -33520,7 +33499,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" s="12" customFormat="1" ht="43.5">
+    <row r="13" spans="1:4" s="12" customFormat="1" ht="45">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -33532,19 +33511,19 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" ht="43.5">
+    <row r="14" spans="1:4" ht="45">
       <c r="A14" s="8" t="s">
         <v>274</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>215</v>
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" ht="43.5">
+    <row r="15" spans="1:4" s="3" customFormat="1" ht="45">
       <c r="A15" s="10" t="s">
         <v>44</v>
       </c>
@@ -33556,7 +33535,7 @@
       </c>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:4" ht="43.5">
+    <row r="16" spans="1:4" ht="45">
       <c r="A16" s="8" t="s">
         <v>218</v>
       </c>
@@ -33568,7 +33547,7 @@
       </c>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="1:4" ht="43.5">
+    <row r="17" spans="1:4" ht="60">
       <c r="A17" s="7" t="s">
         <v>20</v>
       </c>
@@ -33580,7 +33559,7 @@
       </c>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" ht="43.5">
+    <row r="18" spans="1:4" ht="60">
       <c r="A18" s="7" t="s">
         <v>21</v>
       </c>
@@ -33592,7 +33571,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="72.5">
+    <row r="19" spans="1:4" ht="75">
       <c r="A19" s="7" t="s">
         <v>46</v>
       </c>
@@ -33604,7 +33583,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="87">
+    <row r="20" spans="1:4" ht="90">
       <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
@@ -33616,7 +33595,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" spans="1:4" ht="58">
+    <row r="21" spans="1:4" ht="60">
       <c r="A21" s="30" t="s">
         <v>224</v>
       </c>
@@ -33628,7 +33607,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="29">
+    <row r="22" spans="1:4" ht="30">
       <c r="A22" s="12" t="s">
         <v>22</v>
       </c>
@@ -33640,7 +33619,7 @@
       </c>
       <c r="D22" s="12"/>
     </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" ht="29">
+    <row r="23" spans="1:4" s="3" customFormat="1" ht="30">
       <c r="A23" s="3" t="s">
         <v>23</v>
       </c>
@@ -33662,7 +33641,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="72.5">
+    <row r="25" spans="1:4" ht="75">
       <c r="A25" s="8" t="s">
         <v>227</v>
       </c>
@@ -33674,7 +33653,7 @@
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" ht="87">
+    <row r="26" spans="1:4" ht="120">
       <c r="A26" s="6" t="s">
         <v>229</v>
       </c>
@@ -33686,7 +33665,7 @@
       </c>
       <c r="D26" s="12"/>
     </row>
-    <row r="27" spans="1:4" ht="58">
+    <row r="27" spans="1:4" ht="60">
       <c r="A27" s="6" t="s">
         <v>231</v>
       </c>
@@ -33734,11 +33713,11 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.54296875" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
@@ -33760,7 +33739,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="43.5">
+    <row r="5" spans="1:6" ht="45">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -33771,7 +33750,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.5">
+    <row r="6" spans="1:6" ht="45">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -33782,7 +33761,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="58">
+    <row r="7" spans="1:6" ht="60">
       <c r="A7" s="6" t="s">
         <v>104</v>
       </c>
@@ -33793,7 +33772,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.5">
+    <row r="8" spans="1:6" ht="45">
       <c r="A8" s="6" t="s">
         <v>89</v>
       </c>
@@ -33807,7 +33786,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="174">
+    <row r="9" spans="1:6" ht="195">
       <c r="A9" s="8" t="s">
         <v>119</v>
       </c>
@@ -33818,7 +33797,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.5">
+    <row r="10" spans="1:6" ht="45">
       <c r="A10" s="8" t="s">
         <v>90</v>
       </c>
@@ -33829,7 +33808,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="72.5">
+    <row r="11" spans="1:6" ht="75">
       <c r="A11" s="8" t="s">
         <v>92</v>
       </c>
@@ -33840,7 +33819,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="58">
+    <row r="12" spans="1:6" ht="60">
       <c r="A12" s="8" t="s">
         <v>93</v>
       </c>
@@ -33851,7 +33830,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="72.5">
+    <row r="13" spans="1:6" ht="75">
       <c r="A13" s="8" t="s">
         <v>97</v>
       </c>
@@ -33862,7 +33841,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="72.5">
+    <row r="14" spans="1:6" ht="90">
       <c r="A14" s="8" t="s">
         <v>98</v>
       </c>
@@ -33873,7 +33852,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="58">
+    <row r="15" spans="1:6" ht="60">
       <c r="A15" s="8" t="s">
         <v>99</v>
       </c>
@@ -33884,7 +33863,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="87">
+    <row r="16" spans="1:6" ht="90">
       <c r="A16" s="8" t="s">
         <v>103</v>
       </c>
@@ -33895,7 +33874,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="72.5">
+    <row r="17" spans="1:3" ht="75">
       <c r="A17" s="8" t="s">
         <v>101</v>
       </c>
@@ -33906,7 +33885,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="87">
+    <row r="18" spans="1:3" ht="105">
       <c r="A18" s="8" t="s">
         <v>196</v>
       </c>
@@ -33917,7 +33896,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="87">
+    <row r="19" spans="1:3" ht="90">
       <c r="A19" s="8" t="s">
         <v>102</v>
       </c>
@@ -33928,7 +33907,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="43.5">
+    <row r="20" spans="1:3" ht="60">
       <c r="A20" s="8" t="s">
         <v>203</v>
       </c>
@@ -33939,7 +33918,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="87">
+    <row r="21" spans="1:3" ht="90">
       <c r="A21" s="8" t="s">
         <v>106</v>
       </c>
@@ -33950,7 +33929,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5">
+    <row r="22" spans="1:3" ht="75">
       <c r="A22" s="8" t="s">
         <v>108</v>
       </c>
@@ -33961,7 +33940,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="87">
+    <row r="23" spans="1:3" ht="90">
       <c r="A23" s="8" t="s">
         <v>109</v>
       </c>
@@ -33972,7 +33951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="87">
+    <row r="24" spans="1:3" ht="105">
       <c r="A24" s="8" t="s">
         <v>110</v>
       </c>
@@ -33994,7 +33973,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="72.5">
+    <row r="26" spans="1:3" ht="90">
       <c r="A26" s="8" t="s">
         <v>111</v>
       </c>
@@ -34005,7 +33984,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="87">
+    <row r="27" spans="1:3" ht="90">
       <c r="A27" s="8" t="s">
         <v>113</v>
       </c>
@@ -34016,7 +33995,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="72.5">
+    <row r="28" spans="1:3" ht="75">
       <c r="A28" s="8" t="s">
         <v>114</v>
       </c>
@@ -34027,7 +34006,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="116">
+    <row r="29" spans="1:3" ht="120">
       <c r="A29" s="8" t="s">
         <v>115</v>
       </c>
@@ -34038,7 +34017,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="174">
+    <row r="30" spans="1:3" ht="195">
       <c r="A30" s="6" t="s">
         <v>116</v>
       </c>
@@ -34049,7 +34028,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="159.5">
+    <row r="31" spans="1:3" ht="210">
       <c r="A31" s="6" t="s">
         <v>117</v>
       </c>
@@ -34060,7 +34039,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="203">
+    <row r="32" spans="1:3" ht="240">
       <c r="A32" s="9" t="s">
         <v>60</v>
       </c>
@@ -34096,11 +34075,11 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -34125,7 +34104,7 @@
       <c r="B4" s="3"/>
       <c r="C4" s="27"/>
     </row>
-    <row r="5" spans="1:3" ht="29">
+    <row r="5" spans="1:3" ht="30">
       <c r="A5" s="3" t="s">
         <v>50</v>
       </c>
@@ -34136,7 +34115,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="43.5">
+    <row r="6" spans="1:3" ht="60">
       <c r="A6" s="3" t="s">
         <v>135</v>
       </c>
@@ -34147,7 +34126,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29">
+    <row r="7" spans="1:3" ht="30">
       <c r="A7" s="10" t="s">
         <v>136</v>
       </c>
@@ -34158,7 +34137,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="29">
+    <row r="8" spans="1:3" ht="30">
       <c r="A8" s="10" t="s">
         <v>139</v>
       </c>
@@ -34169,7 +34148,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="43.5">
+    <row r="9" spans="1:3" ht="45">
       <c r="A9" s="10" t="s">
         <v>140</v>
       </c>
@@ -34180,7 +34159,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="43.5">
+    <row r="10" spans="1:3" ht="45">
       <c r="A10" s="10" t="s">
         <v>142</v>
       </c>
@@ -34202,7 +34181,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.5">
+    <row r="12" spans="1:3" ht="45">
       <c r="A12" s="10" t="s">
         <v>152</v>
       </c>
@@ -34213,7 +34192,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="43.5">
+    <row r="13" spans="1:3" ht="45">
       <c r="A13" s="8" t="s">
         <v>156</v>
       </c>
@@ -34224,7 +34203,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="43.5">
+    <row r="14" spans="1:3" ht="45">
       <c r="A14" s="8" t="s">
         <v>161</v>
       </c>
@@ -34235,7 +34214,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="72.5">
+    <row r="15" spans="1:3" ht="75">
       <c r="A15" s="8" t="s">
         <v>166</v>
       </c>
@@ -34246,7 +34225,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="43.5">
+    <row r="16" spans="1:3" ht="45">
       <c r="A16" s="8" t="s">
         <v>175</v>
       </c>
@@ -34257,7 +34236,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="43.5">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" s="8" t="s">
         <v>177</v>
       </c>
@@ -34268,7 +34247,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="43.5">
+    <row r="18" spans="1:3" ht="45">
       <c r="A18" s="8" t="s">
         <v>178</v>
       </c>
@@ -34279,7 +34258,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="43.5">
+    <row r="19" spans="1:3" ht="45">
       <c r="A19" s="8" t="s">
         <v>181</v>
       </c>
@@ -34290,7 +34269,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="58">
+    <row r="20" spans="1:3" ht="60">
       <c r="A20" s="8" t="s">
         <v>82</v>
       </c>
@@ -34301,7 +34280,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="72.5">
+    <row r="21" spans="1:3" ht="90">
       <c r="A21" s="10" t="s">
         <v>150</v>
       </c>
@@ -34312,7 +34291,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.5">
+    <row r="22" spans="1:3" ht="75">
       <c r="A22" s="8" t="s">
         <v>183</v>
       </c>
@@ -34323,7 +34302,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="58">
+    <row r="23" spans="1:3" ht="60">
       <c r="A23" s="10" t="s">
         <v>67</v>
       </c>
@@ -34334,7 +34313,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="87">
+    <row r="24" spans="1:3" ht="90">
       <c r="A24" s="8" t="s">
         <v>186</v>
       </c>
@@ -34345,7 +34324,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="101.5">
+    <row r="25" spans="1:3" ht="120">
       <c r="A25" s="10" t="s">
         <v>232</v>
       </c>
@@ -34356,7 +34335,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="72.5">
+    <row r="26" spans="1:3" ht="90">
       <c r="A26" s="8" t="s">
         <v>234</v>
       </c>
@@ -34367,7 +34346,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="72.5">
+    <row r="27" spans="1:3" ht="75">
       <c r="A27" s="10" t="s">
         <v>236</v>
       </c>
@@ -34378,7 +34357,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="43.5">
+    <row r="28" spans="1:3" ht="45">
       <c r="A28" s="7" t="s">
         <v>240</v>
       </c>
@@ -34389,7 +34368,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="58">
+    <row r="29" spans="1:3" ht="75">
       <c r="A29" s="7" t="s">
         <v>242</v>
       </c>
@@ -34400,7 +34379,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="45.65" customHeight="1">
+    <row r="30" spans="1:3" ht="45.6" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>245</v>
       </c>
@@ -34411,7 +34390,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="43.5">
+    <row r="31" spans="1:3" ht="45">
       <c r="A31" s="7" t="s">
         <v>247</v>
       </c>
@@ -34422,7 +34401,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="43.5">
+    <row r="32" spans="1:3" ht="45">
       <c r="A32" s="7" t="s">
         <v>251</v>
       </c>
@@ -34433,7 +34412,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="43.5">
+    <row r="33" spans="1:3" ht="45">
       <c r="A33" s="8" t="s">
         <v>148</v>
       </c>
@@ -34444,7 +34423,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="58">
+    <row r="34" spans="1:3" ht="60">
       <c r="A34" s="8" t="s">
         <v>148</v>
       </c>
@@ -34537,13 +34516,13 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="28"/>
-    <col min="2" max="2" width="30.54296875" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1796875" style="28" customWidth="1"/>
-    <col min="4" max="4" width="52.54296875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="28"/>
+    <col min="1" max="1" width="8.85546875" style="28"/>
+    <col min="2" max="2" width="30.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="28"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -34551,7 +34530,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="58">
+    <row r="3" spans="2:4" ht="60">
       <c r="C3" s="37" t="s">
         <v>544</v>
       </c>
@@ -34575,7 +34554,7 @@
       <c r="B7" s="59"/>
       <c r="C7" s="34"/>
     </row>
-    <row r="8" spans="2:4" ht="29">
+    <row r="8" spans="2:4" ht="30">
       <c r="B8" s="11" t="s">
         <v>559</v>
       </c>
@@ -34586,7 +34565,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="29">
+    <row r="9" spans="2:4" ht="30">
       <c r="B9" s="7" t="s">
         <v>552</v>
       </c>
@@ -34597,7 +34576,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="29">
+    <row r="10" spans="2:4" ht="30">
       <c r="B10" s="7" t="s">
         <v>555</v>
       </c>
@@ -34608,7 +34587,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="29">
+    <row r="11" spans="2:4" ht="30">
       <c r="B11" s="11" t="s">
         <v>558</v>
       </c>
@@ -34619,7 +34598,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="29">
+    <row r="12" spans="2:4" ht="30">
       <c r="B12" s="11" t="s">
         <v>562</v>
       </c>
@@ -34630,7 +34609,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="43.5">
+    <row r="13" spans="2:4" ht="45">
       <c r="B13" s="11" t="s">
         <v>564</v>
       </c>
@@ -34641,7 +34620,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="43.5">
+    <row r="14" spans="2:4" ht="45">
       <c r="B14" s="11" t="s">
         <v>568</v>
       </c>
@@ -34652,7 +34631,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="43.5">
+    <row r="15" spans="2:4" ht="45">
       <c r="B15" s="11" t="s">
         <v>570</v>
       </c>
@@ -34663,7 +34642,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="29">
+    <row r="16" spans="2:4" ht="30">
       <c r="B16" s="7" t="s">
         <v>573</v>
       </c>
@@ -34674,7 +34653,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="159.5">
+    <row r="17" spans="2:13" ht="165">
       <c r="B17" s="7" t="s">
         <v>577</v>
       </c>
@@ -34685,7 +34664,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="145" customHeight="1">
+    <row r="18" spans="2:13" ht="144.94999999999999" customHeight="1">
       <c r="B18" s="11" t="s">
         <v>580</v>
       </c>
@@ -34695,14 +34674,14 @@
       <c r="D18" s="66" t="s">
         <v>582</v>
       </c>
-      <c r="E18" s="97" t="s">
+      <c r="E18" s="84" t="s">
         <v>583</v>
       </c>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="98"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
     </row>
     <row r="19" spans="2:13" ht="234" customHeight="1">
       <c r="B19" s="7" t="s">
@@ -34714,19 +34693,19 @@
       <c r="D19" s="66" t="s">
         <v>586</v>
       </c>
-      <c r="E19" s="97" t="s">
+      <c r="E19" s="84" t="s">
         <v>587</v>
       </c>
-      <c r="F19" s="97"/>
-      <c r="G19" s="97"/>
-      <c r="H19" s="97"/>
-      <c r="I19" s="97"/>
-      <c r="J19" s="97"/>
-      <c r="K19" s="97"/>
-      <c r="L19" s="97"/>
-      <c r="M19" s="97"/>
-    </row>
-    <row r="20" spans="2:13" ht="29">
+      <c r="F19" s="84"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="84"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="84"/>
+    </row>
+    <row r="20" spans="2:13" ht="30">
       <c r="B20" s="7" t="s">
         <v>588</v>
       </c>
@@ -34737,7 +34716,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="238" customHeight="1">
+    <row r="21" spans="2:13" ht="237.95" customHeight="1">
       <c r="B21" s="7" t="s">
         <v>591</v>
       </c>
@@ -34745,19 +34724,19 @@
         <v>592</v>
       </c>
       <c r="D21" s="66" t="s">
+        <v>755</v>
+      </c>
+      <c r="E21" s="84" t="s">
         <v>756</v>
       </c>
-      <c r="E21" s="97" t="s">
-        <v>757</v>
-      </c>
-      <c r="F21" s="97"/>
-      <c r="G21" s="97"/>
-      <c r="H21" s="97"/>
-      <c r="I21" s="97"/>
-      <c r="J21" s="97"/>
-      <c r="K21" s="97"/>
-      <c r="L21" s="97"/>
-      <c r="M21" s="97"/>
+      <c r="F21" s="84"/>
+      <c r="G21" s="84"/>
+      <c r="H21" s="84"/>
+      <c r="I21" s="84"/>
+      <c r="J21" s="84"/>
+      <c r="K21" s="84"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -34774,17 +34753,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C07AE43-F09A-4DAB-AE6D-B6737219C51B}">
   <dimension ref="B2:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="27"/>
-    <col min="2" max="2" width="54.08984375" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.54296875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="56.453125" style="27" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="27"/>
+    <col min="1" max="1" width="8.7109375" style="27"/>
+    <col min="2" max="2" width="54.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="27" customWidth="1"/>
+    <col min="5" max="16384" width="8.7109375" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -34870,13 +34849,13 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" s="27" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C14" s="43" t="s">
+        <v>719</v>
+      </c>
+      <c r="D14" s="21" t="s">
         <v>720</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -34892,38 +34871,38 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" s="27" t="s">
-        <v>786</v>
-      </c>
-      <c r="C16" s="70" t="s">
+        <v>785</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>783</v>
+      </c>
+      <c r="D16" s="21" t="s">
         <v>784</v>
       </c>
-      <c r="D16" s="69" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" s="74" customFormat="1">
-      <c r="B17" s="74" t="s">
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="27" t="s">
+        <v>792</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>791</v>
+      </c>
+      <c r="D17" s="21" t="s">
         <v>793</v>
       </c>
-      <c r="C17" s="73" t="s">
-        <v>792</v>
-      </c>
-      <c r="D17" s="72" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" s="74" customFormat="1">
-      <c r="C18" s="73"/>
-      <c r="D18" s="72"/>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="C18" s="43"/>
+      <c r="D18" s="21"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="60" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" s="78" customFormat="1">
-      <c r="B21" s="112" t="s">
-        <v>813</v>
+        <v>723</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="27" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -34942,7 +34921,7 @@
     </row>
     <row r="25" spans="2:4">
       <c r="B25" s="60" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -34987,135 +34966,135 @@
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="2:4">
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="88" t="s">
+        <v>787</v>
+      </c>
+      <c r="C31" s="88"/>
+      <c r="D31" s="88"/>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="67" t="s">
+        <v>762</v>
+      </c>
+      <c r="C32" s="76"/>
+      <c r="D32" s="77"/>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="70" t="s">
+        <v>760</v>
+      </c>
+      <c r="C33" s="78"/>
+      <c r="D33" s="70"/>
+    </row>
+    <row r="34" spans="2:4" ht="30">
+      <c r="B34" s="73" t="s">
+        <v>761</v>
+      </c>
+      <c r="C34" s="76"/>
+      <c r="D34" s="67"/>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="79" t="s">
+        <v>763</v>
+      </c>
+      <c r="C35" s="78"/>
+      <c r="D35" s="70"/>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="73" t="s">
+        <v>764</v>
+      </c>
+      <c r="C36" s="76"/>
+      <c r="D36" s="67"/>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="79" t="s">
+        <v>765</v>
+      </c>
+      <c r="C37" s="78"/>
+      <c r="D37" s="70"/>
+    </row>
+    <row r="38" spans="2:4" ht="30">
+      <c r="B38" s="73" t="s">
+        <v>766</v>
+      </c>
+      <c r="C38" s="76"/>
+      <c r="D38" s="67"/>
+    </row>
+    <row r="39" spans="2:4" ht="30">
+      <c r="B39" s="80" t="s">
+        <v>770</v>
+      </c>
+      <c r="C39" s="71" t="s">
+        <v>767</v>
+      </c>
+      <c r="D39" s="72" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="81" t="s">
+        <v>769</v>
+      </c>
+      <c r="C40" s="74" t="s">
+        <v>616</v>
+      </c>
+      <c r="D40" s="69" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="30">
+      <c r="B41" s="80" t="s">
+        <v>771</v>
+      </c>
+      <c r="C41" s="71" t="s">
+        <v>772</v>
+      </c>
+      <c r="D41" s="82" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="45">
+      <c r="B42" s="81" t="s">
+        <v>775</v>
+      </c>
+      <c r="C42" s="74" t="s">
+        <v>776</v>
+      </c>
+      <c r="D42" s="69" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="60">
+      <c r="B43" s="80" t="s">
+        <v>780</v>
+      </c>
+      <c r="C43" s="71" t="s">
+        <v>777</v>
+      </c>
+      <c r="D43" s="82" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="30">
+      <c r="B44" s="81" t="s">
         <v>788</v>
       </c>
-      <c r="C31" s="101"/>
-      <c r="D31" s="101"/>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32" s="88" t="s">
-        <v>763</v>
-      </c>
-      <c r="C32" s="89"/>
-      <c r="D32" s="90"/>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="82" t="s">
-        <v>761</v>
-      </c>
-      <c r="C33" s="91"/>
-      <c r="D33" s="82"/>
-    </row>
-    <row r="34" spans="2:4" s="71" customFormat="1" ht="29">
-      <c r="B34" s="85" t="s">
-        <v>762</v>
-      </c>
-      <c r="C34" s="89"/>
-      <c r="D34" s="88"/>
-    </row>
-    <row r="35" spans="2:4" s="71" customFormat="1">
-      <c r="B35" s="92" t="s">
-        <v>764</v>
-      </c>
-      <c r="C35" s="91"/>
-      <c r="D35" s="82"/>
-    </row>
-    <row r="36" spans="2:4" s="71" customFormat="1">
-      <c r="B36" s="85" t="s">
-        <v>765</v>
-      </c>
-      <c r="C36" s="89"/>
-      <c r="D36" s="88"/>
-    </row>
-    <row r="37" spans="2:4" s="71" customFormat="1">
-      <c r="B37" s="92" t="s">
-        <v>766</v>
-      </c>
-      <c r="C37" s="91"/>
-      <c r="D37" s="82"/>
-    </row>
-    <row r="38" spans="2:4" s="71" customFormat="1" ht="29">
-      <c r="B38" s="85" t="s">
-        <v>767</v>
-      </c>
-      <c r="C38" s="89"/>
-      <c r="D38" s="88"/>
-    </row>
-    <row r="39" spans="2:4" s="71" customFormat="1" ht="29">
-      <c r="B39" s="93" t="s">
-        <v>771</v>
-      </c>
-      <c r="C39" s="83" t="s">
-        <v>768</v>
-      </c>
-      <c r="D39" s="84" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" s="71" customFormat="1">
-      <c r="B40" s="94" t="s">
-        <v>770</v>
-      </c>
-      <c r="C40" s="86" t="s">
-        <v>616</v>
-      </c>
-      <c r="D40" s="81" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" s="71" customFormat="1">
-      <c r="B41" s="93" t="s">
-        <v>772</v>
-      </c>
-      <c r="C41" s="83" t="s">
-        <v>773</v>
-      </c>
-      <c r="D41" s="95" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" s="71" customFormat="1" ht="43.5">
-      <c r="B42" s="94" t="s">
-        <v>776</v>
-      </c>
-      <c r="C42" s="86" t="s">
-        <v>777</v>
-      </c>
-      <c r="D42" s="81" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" s="71" customFormat="1" ht="58">
-      <c r="B43" s="93" t="s">
+      <c r="C44" s="74" t="s">
         <v>781</v>
       </c>
-      <c r="C43" s="83" t="s">
-        <v>778</v>
-      </c>
-      <c r="D43" s="95" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" s="71" customFormat="1" ht="29">
-      <c r="B44" s="94" t="s">
-        <v>789</v>
-      </c>
-      <c r="C44" s="86" t="s">
+      <c r="D44" s="83" t="s">
         <v>782</v>
       </c>
-      <c r="D44" s="96" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" s="71" customFormat="1">
+    </row>
+    <row r="45" spans="2:4">
       <c r="B45" s="6"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="68"/>
+      <c r="D45" s="19"/>
     </row>
     <row r="47" spans="2:4">
       <c r="B47" s="60" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -35123,147 +35102,147 @@
         <v>707</v>
       </c>
       <c r="C48" s="43" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51" s="60" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52" s="27" t="s">
+        <v>711</v>
+      </c>
+      <c r="C52" s="43" t="s">
         <v>712</v>
       </c>
-      <c r="C52" s="43" t="s">
+    </row>
+    <row r="53" spans="2:4" ht="30">
+      <c r="B53" s="38" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" ht="29">
-      <c r="B53" s="38" t="s">
+      <c r="C53" s="39" t="s">
         <v>714</v>
-      </c>
-      <c r="C53" s="39" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54" s="27" t="s">
+        <v>715</v>
+      </c>
+      <c r="C54" s="43" t="s">
         <v>716</v>
       </c>
-      <c r="C54" s="43" t="s">
+    </row>
+    <row r="55" spans="2:4" ht="30">
+      <c r="B55" s="38" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" ht="29">
-      <c r="B55" s="38" t="s">
+      <c r="C55" s="86" t="s">
         <v>718</v>
       </c>
-      <c r="C55" s="99" t="s">
-        <v>719</v>
-      </c>
-      <c r="D55" s="100"/>
+      <c r="D55" s="87"/>
     </row>
     <row r="58" spans="2:4">
       <c r="B58" s="60" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59" s="27" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C59" s="43" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="62" spans="2:4">
-      <c r="B62" s="101" t="s">
+      <c r="B62" s="88" t="s">
+        <v>757</v>
+      </c>
+      <c r="C62" s="88"/>
+      <c r="D62" s="88"/>
+    </row>
+    <row r="63" spans="2:4" ht="255">
+      <c r="B63" s="67" t="s">
+        <v>759</v>
+      </c>
+      <c r="C63" s="68" t="s">
+        <v>789</v>
+      </c>
+      <c r="D63" s="69" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="30">
+      <c r="B64" s="70"/>
+      <c r="C64" s="71" t="s">
         <v>758</v>
       </c>
-      <c r="C62" s="101"/>
-      <c r="D62" s="101"/>
-    </row>
-    <row r="63" spans="2:4" s="67" customFormat="1" ht="217.5">
-      <c r="B63" s="79" t="s">
-        <v>760</v>
-      </c>
-      <c r="C63" s="80" t="s">
-        <v>790</v>
-      </c>
-      <c r="D63" s="81" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" ht="29">
-      <c r="B64" s="82"/>
-      <c r="C64" s="83" t="s">
-        <v>759</v>
-      </c>
-      <c r="D64" s="84" t="s">
+      <c r="D64" s="72" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="75">
+      <c r="B65" s="73" t="s">
+        <v>797</v>
+      </c>
+      <c r="C65" s="74" t="s">
+        <v>798</v>
+      </c>
+      <c r="D65" s="69" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="65" spans="2:4" ht="72.5">
-      <c r="B65" s="85" t="s">
-        <v>798</v>
-      </c>
-      <c r="C65" s="86" t="s">
-        <v>799</v>
-      </c>
-      <c r="D65" s="81" t="s">
+    <row r="66" spans="2:4" ht="30">
+      <c r="B66" s="75" t="s">
+        <v>794</v>
+      </c>
+      <c r="C66" s="71" t="s">
+        <v>795</v>
+      </c>
+      <c r="D66" s="72" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="89" t="s">
         <v>801</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" ht="29">
-      <c r="B66" s="87" t="s">
-        <v>795</v>
-      </c>
-      <c r="C66" s="83" t="s">
-        <v>796</v>
-      </c>
-      <c r="D66" s="84" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="69" spans="2:4">
-      <c r="B69" s="102" t="s">
+      <c r="C69" s="89"/>
+      <c r="D69" s="89"/>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="43" t="s">
         <v>802</v>
       </c>
-      <c r="C69" s="102"/>
-      <c r="D69" s="102"/>
-    </row>
-    <row r="70" spans="2:4">
-      <c r="B70" s="76" t="s">
+      <c r="C70" s="43" t="s">
+        <v>802</v>
+      </c>
+      <c r="D70" s="21" t="s">
         <v>803</v>
       </c>
-      <c r="C70" s="76" t="s">
-        <v>803</v>
-      </c>
-      <c r="D70" s="75" t="s">
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" s="43" t="s">
+        <v>806</v>
+      </c>
+      <c r="C71" s="43" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="71" spans="2:4">
-      <c r="B71" s="76" t="s">
+      <c r="D71" s="21" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" ht="30">
+      <c r="B72" s="38" t="s">
         <v>807</v>
       </c>
-      <c r="C71" s="76" t="s">
-        <v>805</v>
-      </c>
-      <c r="D71" s="75" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="72" spans="2:4" ht="29">
-      <c r="B72" s="77" t="s">
+      <c r="C72" s="2" t="s">
         <v>808</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="D72" s="21" t="s">
         <v>809</v>
-      </c>
-      <c r="D72" s="75" t="s">
-        <v>810</v>
       </c>
     </row>
   </sheetData>
@@ -35286,13 +35265,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="27"/>
-    <col min="2" max="2" width="30.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1796875" style="27" customWidth="1"/>
-    <col min="4" max="4" width="52.54296875" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="27"/>
+    <col min="1" max="1" width="8.85546875" style="27"/>
+    <col min="2" max="2" width="30.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" style="27" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
@@ -35320,7 +35299,7 @@
       <c r="B6" s="45"/>
       <c r="C6" s="43"/>
     </row>
-    <row r="7" spans="2:4" ht="29">
+    <row r="7" spans="2:4" ht="30">
       <c r="B7" s="46" t="s">
         <v>549</v>
       </c>
@@ -35332,7 +35311,7 @@
     <row r="9" spans="2:4">
       <c r="B9" s="45"/>
     </row>
-    <row r="10" spans="2:4" ht="101.5" customHeight="1">
+    <row r="10" spans="2:4" ht="101.45" customHeight="1">
       <c r="B10" s="45"/>
       <c r="C10" s="43"/>
       <c r="D10" s="38"/>
@@ -35354,10 +35333,10 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="30.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:3">
@@ -35396,7 +35375,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="101.5" customHeight="1">
+    <row r="9" spans="1:3" ht="101.45" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>294</v>
       </c>
@@ -35429,13 +35408,13 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.453125" style="28" customWidth="1"/>
-    <col min="2" max="2" width="41.453125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="46.81640625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="48.81640625" style="28" customWidth="1"/>
-    <col min="5" max="16384" width="8.81640625" style="28"/>
+    <col min="1" max="1" width="30.42578125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="28" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -35447,17 +35426,17 @@
       <c r="A2" s="28" t="s">
         <v>317</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="91" t="s">
         <v>328</v>
       </c>
-      <c r="C2" s="104"/>
+      <c r="C2" s="91"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="92" t="s">
         <v>308</v>
       </c>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
     </row>
     <row r="5" spans="1:4" s="34" customFormat="1">
       <c r="B5" s="20"/>
@@ -35465,12 +35444,12 @@
       <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="106" t="s">
+      <c r="A6" s="93" t="s">
         <v>322</v>
       </c>
-      <c r="B6" s="106"/>
-    </row>
-    <row r="7" spans="1:4" ht="43.5">
+      <c r="B6" s="93"/>
+    </row>
+    <row r="7" spans="1:4" ht="45">
       <c r="A7" s="35" t="s">
         <v>344</v>
       </c>
@@ -35503,7 +35482,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="72.5">
+    <row r="10" spans="1:4" ht="90">
       <c r="A10" s="9" t="s">
         <v>350</v>
       </c>
@@ -35563,7 +35542,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="29">
+    <row r="18" spans="1:3" ht="30">
       <c r="A18" s="4" t="s">
         <v>354</v>
       </c>
@@ -35585,7 +35564,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="58">
+    <row r="20" spans="1:3" ht="75">
       <c r="A20" s="4" t="s">
         <v>368</v>
       </c>
@@ -35597,88 +35576,88 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="90" t="s">
         <v>316</v>
       </c>
-      <c r="B22" s="103"/>
-      <c r="C22" s="103"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="90"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="103" t="s">
+      <c r="A23" s="90" t="s">
         <v>319</v>
       </c>
-      <c r="B23" s="103"/>
-      <c r="C23" s="103"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="90"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="103" t="s">
+      <c r="A24" s="90" t="s">
         <v>323</v>
       </c>
-      <c r="B24" s="103"/>
-      <c r="C24" s="103"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="103" t="s">
+      <c r="A25" s="90" t="s">
         <v>325</v>
       </c>
-      <c r="B25" s="103"/>
-      <c r="C25" s="103"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="90"/>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="103" t="s">
+      <c r="A26" s="90" t="s">
         <v>326</v>
       </c>
-      <c r="B26" s="103"/>
-      <c r="C26" s="103"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="90"/>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="103" t="s">
+      <c r="A27" s="90" t="s">
         <v>327</v>
       </c>
-      <c r="B27" s="103"/>
-      <c r="C27" s="103"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="90"/>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="103" t="s">
+      <c r="A28" s="90" t="s">
         <v>329</v>
       </c>
-      <c r="B28" s="103"/>
-      <c r="C28" s="103"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="103" t="s">
+      <c r="A29" s="90" t="s">
         <v>330</v>
       </c>
-      <c r="B29" s="103"/>
-      <c r="C29" s="103"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="90"/>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="91" t="s">
         <v>331</v>
       </c>
-      <c r="B30" s="104"/>
-      <c r="C30" s="104"/>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="104" t="s">
+      <c r="A31" s="91" t="s">
         <v>339</v>
       </c>
-      <c r="B31" s="104"/>
-      <c r="C31" s="104"/>
+      <c r="B31" s="91"/>
+      <c r="C31" s="91"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="103" t="s">
+      <c r="A32" s="90" t="s">
         <v>340</v>
       </c>
-      <c r="B32" s="103"/>
-      <c r="C32" s="103"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="90"/>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="103" t="s">
+      <c r="A33" s="90" t="s">
         <v>341</v>
       </c>
-      <c r="B33" s="103"/>
-      <c r="C33" s="103"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="90"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="27" t="s">

</xml_diff>